<commit_message>
Refactor sceanrios and options
</commit_message>
<xml_diff>
--- a/docs/static/examples/tf/accelerator/config/checklist.xlsx
+++ b/docs/static/examples/tf/accelerator/config/checklist.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jaredholgate\Code\azure-landing-zones\docs\static\examples\tf\accelerator\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB3C5B00-6237-40F2-848C-E85B083B70A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E0F5EFA-EF6C-4F04-9CE8-C1680883C79C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" tabRatio="415" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38290" yWindow="-160" windowWidth="38620" windowHeight="21100" tabRatio="415" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Accelerator - Bootstrap" sheetId="13" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1418" uniqueCount="807">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1422" uniqueCount="810">
   <si>
     <t>Description</t>
   </si>
@@ -2595,6 +2595,15 @@
   </si>
   <si>
     <t>Change a policy assignment enforcement mode</t>
+  </si>
+  <si>
+    <t>Number</t>
+  </si>
+  <si>
+    <t>Deploy Azure Monitoring Baseline Alerts</t>
+  </si>
+  <si>
+    <t>Do you want to deploy AMBA policies?</t>
   </si>
 </sst>
 </file>
@@ -8537,24 +8546,24 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE440EAA-007A-486E-B4E3-7FE7599AA545}">
-  <dimension ref="A1:F27"/>
+  <dimension ref="A1:G28"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D30" sqref="D30"/>
+      <selection pane="bottomLeft" activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="55.54296875" customWidth="1"/>
-    <col min="2" max="2" width="42.453125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="39.81640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="48.7265625" customWidth="1"/>
-    <col min="5" max="5" width="50.453125" customWidth="1"/>
-    <col min="6" max="6" width="46.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="55.54296875" customWidth="1"/>
+    <col min="3" max="3" width="42.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="39.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="48.7265625" customWidth="1"/>
+    <col min="6" max="6" width="50.453125" customWidth="1"/>
+    <col min="7" max="7" width="46.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="77.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" ht="77.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="48" t="s">
         <v>797</v>
       </c>
@@ -8563,340 +8572,422 @@
       <c r="D1" s="48"/>
       <c r="E1" s="48"/>
       <c r="F1" s="48"/>
-    </row>
-    <row r="3" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="G1" s="48"/>
+    </row>
+    <row r="3" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="41" t="s">
+        <v>807</v>
+      </c>
+      <c r="B3" s="41" t="s">
         <v>672</v>
       </c>
-      <c r="B3" s="41" t="s">
+      <c r="C3" s="41" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="41" t="s">
+      <c r="D3" s="41" t="s">
         <v>673</v>
       </c>
-      <c r="D3" s="41" t="s">
+      <c r="E3" s="41" t="s">
         <v>676</v>
       </c>
-      <c r="E3" s="41" t="s">
+      <c r="F3" s="41" t="s">
         <v>682</v>
       </c>
-      <c r="F3" s="41" t="s">
+      <c r="G3" s="41" t="s">
         <v>691</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" s="36"/>
-      <c r="B4" s="37"/>
-      <c r="C4" s="36"/>
-      <c r="D4" s="37"/>
-      <c r="E4" s="36"/>
+      <c r="B4" s="36"/>
+      <c r="C4" s="37"/>
+      <c r="D4" s="36"/>
+      <c r="E4" s="37"/>
       <c r="F4" s="36"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G4" s="36"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" s="39" t="s">
         <v>789</v>
       </c>
-      <c r="B5" s="37"/>
-      <c r="C5" s="36"/>
-      <c r="D5" s="37"/>
-      <c r="E5" s="36"/>
+      <c r="B5" s="39"/>
+      <c r="C5" s="37"/>
+      <c r="D5" s="36"/>
+      <c r="E5" s="37"/>
       <c r="F5" s="36"/>
-    </row>
-    <row r="6" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A6" s="34" t="s">
+      <c r="G5" s="36"/>
+    </row>
+    <row r="6" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A6" s="43">
+        <v>1</v>
+      </c>
+      <c r="B6" s="34" t="s">
         <v>762</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="C6" s="1" t="s">
         <v>764</v>
       </c>
-      <c r="C6" s="34"/>
-      <c r="D6" s="1" t="s">
+      <c r="D6" s="34"/>
+      <c r="E6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E6" s="35"/>
-      <c r="F6" s="34"/>
-    </row>
-    <row r="7" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A7" s="34" t="s">
+      <c r="F6" s="35"/>
+      <c r="G6" s="34"/>
+    </row>
+    <row r="7" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A7" s="43">
+        <v>2</v>
+      </c>
+      <c r="B7" s="34" t="s">
         <v>763</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="C7" s="1" t="s">
         <v>765</v>
       </c>
-      <c r="C7" s="34"/>
-      <c r="D7" s="1" t="s">
+      <c r="D7" s="34"/>
+      <c r="E7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E7" s="35"/>
-      <c r="F7" s="34"/>
-    </row>
-    <row r="8" spans="1:6" ht="58" x14ac:dyDescent="0.35">
-      <c r="A8" s="34" t="s">
+      <c r="F7" s="35"/>
+      <c r="G7" s="34"/>
+    </row>
+    <row r="8" spans="1:7" ht="58" x14ac:dyDescent="0.35">
+      <c r="A8" s="43">
+        <v>3</v>
+      </c>
+      <c r="B8" s="34" t="s">
         <v>766</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="C8" s="1" t="s">
         <v>767</v>
       </c>
-      <c r="C8" s="34"/>
-      <c r="D8" s="1" t="s">
+      <c r="D8" s="34"/>
+      <c r="E8" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E8" s="35"/>
-      <c r="F8" s="34"/>
-    </row>
-    <row r="9" spans="1:6" ht="58" x14ac:dyDescent="0.35">
-      <c r="A9" s="34" t="s">
+      <c r="F8" s="35"/>
+      <c r="G8" s="34"/>
+    </row>
+    <row r="9" spans="1:7" ht="58" x14ac:dyDescent="0.35">
+      <c r="A9" s="43">
+        <v>4</v>
+      </c>
+      <c r="B9" s="34" t="s">
         <v>768</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="C9" s="1" t="s">
         <v>769</v>
       </c>
-      <c r="C9" s="34"/>
-      <c r="D9" s="1" t="s">
+      <c r="D9" s="34"/>
+      <c r="E9" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E9" s="35"/>
-      <c r="F9" s="34"/>
-    </row>
-    <row r="10" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A10" s="34" t="s">
+      <c r="F9" s="35"/>
+      <c r="G9" s="34"/>
+    </row>
+    <row r="10" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A10" s="43">
+        <v>5</v>
+      </c>
+      <c r="B10" s="34" t="s">
+        <v>774</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>775</v>
+      </c>
+      <c r="D10" s="34"/>
+      <c r="E10" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F10" s="35"/>
+      <c r="G10" s="34"/>
+    </row>
+    <row r="11" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A11" s="43">
+        <v>6</v>
+      </c>
+      <c r="B11" s="34" t="s">
         <v>770</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="C11" s="1" t="s">
         <v>771</v>
       </c>
-      <c r="C10" s="34"/>
-      <c r="D10" s="1" t="s">
+      <c r="D11" s="34"/>
+      <c r="E11" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E10" s="35"/>
-      <c r="F10" s="34"/>
-    </row>
-    <row r="11" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A11" s="34" t="s">
+      <c r="F11" s="35"/>
+      <c r="G11" s="34"/>
+    </row>
+    <row r="12" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A12" s="43">
+        <v>7</v>
+      </c>
+      <c r="B12" s="34" t="s">
         <v>772</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="C12" s="1" t="s">
         <v>773</v>
       </c>
-      <c r="C11" s="34"/>
-      <c r="D11" s="1" t="s">
+      <c r="D12" s="34"/>
+      <c r="E12" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E11" s="35"/>
-      <c r="F11" s="34"/>
-    </row>
-    <row r="12" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A12" s="34" t="s">
-        <v>774</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>775</v>
-      </c>
-      <c r="C12" s="34"/>
-      <c r="D12" s="1" t="s">
+      <c r="F12" s="35"/>
+      <c r="G12" s="34"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A13" s="45"/>
+      <c r="B13" s="36"/>
+      <c r="C13" s="37"/>
+      <c r="D13" s="36"/>
+      <c r="E13" s="37"/>
+      <c r="F13" s="36"/>
+      <c r="G13" s="36"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A14" s="46" t="s">
+        <v>790</v>
+      </c>
+      <c r="B14" s="39"/>
+      <c r="C14" s="37"/>
+      <c r="D14" s="36"/>
+      <c r="E14" s="37"/>
+      <c r="F14" s="36"/>
+      <c r="G14" s="36"/>
+    </row>
+    <row r="15" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A15" s="43">
+        <v>1</v>
+      </c>
+      <c r="B15" s="34" t="s">
+        <v>781</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>776</v>
+      </c>
+      <c r="D15" s="34"/>
+      <c r="E15" s="1" t="s">
+        <v>788</v>
+      </c>
+      <c r="F15" s="35"/>
+      <c r="G15" s="34"/>
+    </row>
+    <row r="16" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A16" s="43">
+        <v>2</v>
+      </c>
+      <c r="B16" s="34" t="s">
+        <v>780</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>787</v>
+      </c>
+      <c r="D16" s="34"/>
+      <c r="E16" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E12" s="35"/>
-      <c r="F12" s="34"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A13" s="36"/>
-      <c r="B13" s="37"/>
-      <c r="C13" s="36"/>
-      <c r="D13" s="37"/>
-      <c r="E13" s="36"/>
-      <c r="F13" s="36"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A14" s="39" t="s">
-        <v>790</v>
-      </c>
-      <c r="B14" s="37"/>
-      <c r="C14" s="36"/>
-      <c r="D14" s="37"/>
-      <c r="E14" s="36"/>
-      <c r="F14" s="36"/>
-    </row>
-    <row r="15" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A15" s="34" t="s">
-        <v>781</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>776</v>
-      </c>
-      <c r="C15" s="34"/>
-      <c r="D15" s="1" t="s">
-        <v>788</v>
-      </c>
-      <c r="E15" s="35"/>
-      <c r="F15" s="34"/>
-    </row>
-    <row r="16" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A16" s="34" t="s">
-        <v>780</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>787</v>
-      </c>
-      <c r="C16" s="34"/>
-      <c r="D16" s="1" t="s">
+      <c r="F16" s="35"/>
+      <c r="G16" s="34"/>
+    </row>
+    <row r="17" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A17" s="43">
+        <v>3</v>
+      </c>
+      <c r="B17" s="34" t="s">
+        <v>777</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>783</v>
+      </c>
+      <c r="D17" s="34"/>
+      <c r="E17" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E16" s="35"/>
-      <c r="F16" s="34"/>
-    </row>
-    <row r="17" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A17" s="34" t="s">
-        <v>777</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>783</v>
-      </c>
-      <c r="C17" s="34"/>
-      <c r="D17" s="1" t="s">
+      <c r="F17" s="35"/>
+      <c r="G17" s="34"/>
+    </row>
+    <row r="18" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A18" s="43">
+        <v>4</v>
+      </c>
+      <c r="B18" s="34" t="s">
+        <v>779</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>786</v>
+      </c>
+      <c r="D18" s="34"/>
+      <c r="E18" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E17" s="35"/>
-      <c r="F17" s="34"/>
-    </row>
-    <row r="18" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A18" s="34" t="s">
-        <v>779</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>786</v>
-      </c>
-      <c r="C18" s="34"/>
-      <c r="D18" s="1" t="s">
+      <c r="F18" s="35"/>
+      <c r="G18" s="34"/>
+    </row>
+    <row r="19" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A19" s="43">
         <v>5</v>
       </c>
-      <c r="E18" s="35"/>
-      <c r="F18" s="34"/>
-    </row>
-    <row r="19" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A19" s="34" t="s">
+      <c r="B19" s="34" t="s">
         <v>778</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="C19" s="1" t="s">
         <v>782</v>
       </c>
-      <c r="C19" s="34"/>
-      <c r="D19" s="1" t="s">
+      <c r="D19" s="34"/>
+      <c r="E19" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E19" s="40"/>
-      <c r="F19" s="34"/>
-    </row>
-    <row r="20" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A20" s="34" t="s">
+      <c r="F19" s="40"/>
+      <c r="G19" s="34"/>
+    </row>
+    <row r="20" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A20" s="43">
+        <v>6</v>
+      </c>
+      <c r="B20" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="C20" s="1" t="s">
         <v>784</v>
       </c>
-      <c r="C20" s="34"/>
-      <c r="D20" s="1" t="s">
+      <c r="D20" s="34"/>
+      <c r="E20" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E20" s="35"/>
-      <c r="F20" s="34"/>
-    </row>
-    <row r="21" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A21" s="34" t="s">
+      <c r="F20" s="35"/>
+      <c r="G20" s="34"/>
+    </row>
+    <row r="21" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A21" s="43">
+        <v>6</v>
+      </c>
+      <c r="B21" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="C21" s="1" t="s">
         <v>785</v>
       </c>
-      <c r="C21" s="34"/>
-      <c r="D21" s="1" t="s">
+      <c r="D21" s="34"/>
+      <c r="E21" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E21" s="35"/>
-      <c r="F21" s="34"/>
-    </row>
-    <row r="22" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A22" s="34" t="s">
+      <c r="F21" s="35"/>
+      <c r="G21" s="34"/>
+    </row>
+    <row r="22" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A22" s="43">
+        <v>7</v>
+      </c>
+      <c r="B22" s="34" t="s">
         <v>791</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="C22" s="1" t="s">
         <v>792</v>
       </c>
-      <c r="C22" s="34"/>
-      <c r="D22" s="1" t="s">
+      <c r="D22" s="34"/>
+      <c r="E22" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E22" s="40"/>
-      <c r="F22" s="34"/>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A23" s="34" t="s">
+      <c r="F22" s="40"/>
+      <c r="G22" s="34"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A23" s="43">
+        <v>8</v>
+      </c>
+      <c r="B23" s="34" t="s">
         <v>793</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="C23" s="1" t="s">
         <v>794</v>
       </c>
-      <c r="C23" s="34"/>
-      <c r="D23" s="1" t="s">
+      <c r="D23" s="34"/>
+      <c r="E23" s="1" t="s">
         <v>795</v>
       </c>
-      <c r="E23" s="40"/>
-      <c r="F23" s="34"/>
-    </row>
-    <row r="24" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A24" s="34" t="s">
+      <c r="F23" s="40"/>
+      <c r="G23" s="34"/>
+    </row>
+    <row r="24" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A24" s="43">
+        <v>9</v>
+      </c>
+      <c r="B24" s="34" t="s">
         <v>806</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="C24" s="1" t="s">
         <v>805</v>
       </c>
-      <c r="C24" s="34"/>
-      <c r="D24" s="1" t="s">
+      <c r="D24" s="34"/>
+      <c r="E24" s="1" t="s">
         <v>804</v>
       </c>
-      <c r="E24" s="35"/>
-      <c r="F24" s="34"/>
-    </row>
-    <row r="25" spans="1:6" ht="58" x14ac:dyDescent="0.35">
-      <c r="A25" s="34" t="s">
+      <c r="F24" s="35"/>
+      <c r="G24" s="34"/>
+    </row>
+    <row r="25" spans="1:7" ht="58" x14ac:dyDescent="0.35">
+      <c r="A25" s="43">
+        <v>10</v>
+      </c>
+      <c r="B25" s="34" t="s">
         <v>800</v>
       </c>
-      <c r="B25" s="1" t="s">
+      <c r="C25" s="1" t="s">
         <v>803</v>
       </c>
-      <c r="C25" s="34"/>
-      <c r="D25" s="1" t="s">
+      <c r="D25" s="34"/>
+      <c r="E25" s="1" t="s">
         <v>804</v>
       </c>
-      <c r="E25" s="40"/>
-      <c r="F25" s="34"/>
-    </row>
-    <row r="26" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A26" s="34" t="s">
+      <c r="F25" s="40"/>
+      <c r="G25" s="34"/>
+    </row>
+    <row r="26" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A26" s="43">
+        <v>11</v>
+      </c>
+      <c r="B26" s="34" t="s">
         <v>801</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="C26" s="1" t="s">
         <v>802</v>
       </c>
-      <c r="C26" s="34"/>
-      <c r="D26" s="1" t="s">
+      <c r="D26" s="34"/>
+      <c r="E26" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E26" s="40"/>
-      <c r="F26" s="34"/>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A27" s="36"/>
-      <c r="B27" s="37"/>
-      <c r="C27" s="36"/>
-      <c r="D27" s="37"/>
-      <c r="E27" s="36"/>
-      <c r="F27" s="36"/>
+      <c r="F26" s="40"/>
+      <c r="G26" s="34"/>
+    </row>
+    <row r="27" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A27" s="43">
+        <v>12</v>
+      </c>
+      <c r="B27" s="34" t="s">
+        <v>808</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>809</v>
+      </c>
+      <c r="D27" s="34"/>
+      <c r="E27" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F27" s="40"/>
+      <c r="G27" s="34"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B28" s="36"/>
+      <c r="C28" s="37"/>
+      <c r="D28" s="36"/>
+      <c r="E28" s="37"/>
+      <c r="F28" s="36"/>
+      <c r="G28" s="36"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A1:G1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -10186,6 +10277,58 @@
     <row r="116" hidden="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <mergeCells count="64">
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="A6:A8"/>
+    <mergeCell ref="B6:B8"/>
+    <mergeCell ref="C6:C8"/>
+    <mergeCell ref="E6:E8"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="A24:A25"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="E24:E25"/>
+    <mergeCell ref="A26:A27"/>
+    <mergeCell ref="B26:B27"/>
+    <mergeCell ref="C26:C27"/>
+    <mergeCell ref="E26:E27"/>
+    <mergeCell ref="A28:A29"/>
+    <mergeCell ref="B28:B29"/>
+    <mergeCell ref="C28:C29"/>
+    <mergeCell ref="E28:E29"/>
+    <mergeCell ref="A30:A31"/>
+    <mergeCell ref="B30:B31"/>
+    <mergeCell ref="C30:C31"/>
+    <mergeCell ref="E30:E31"/>
+    <mergeCell ref="A32:A33"/>
+    <mergeCell ref="B32:B33"/>
+    <mergeCell ref="C32:C33"/>
+    <mergeCell ref="E32:E33"/>
+    <mergeCell ref="A34:A35"/>
+    <mergeCell ref="B34:B35"/>
+    <mergeCell ref="C34:C35"/>
+    <mergeCell ref="E34:E35"/>
+    <mergeCell ref="A37:A64"/>
+    <mergeCell ref="B37:B64"/>
+    <mergeCell ref="C37:C64"/>
+    <mergeCell ref="E37:E64"/>
+    <mergeCell ref="A65:A79"/>
+    <mergeCell ref="B65:B79"/>
+    <mergeCell ref="C65:C79"/>
+    <mergeCell ref="E65:E79"/>
+    <mergeCell ref="A80:A94"/>
+    <mergeCell ref="B80:B94"/>
+    <mergeCell ref="C80:C94"/>
+    <mergeCell ref="E80:E94"/>
+    <mergeCell ref="A98:A99"/>
+    <mergeCell ref="B98:B99"/>
+    <mergeCell ref="C98:C99"/>
+    <mergeCell ref="E98:E99"/>
     <mergeCell ref="A109:A110"/>
     <mergeCell ref="B109:B110"/>
     <mergeCell ref="C109:C110"/>
@@ -10198,106 +10341,12 @@
     <mergeCell ref="B103:B104"/>
     <mergeCell ref="C103:C104"/>
     <mergeCell ref="E103:E104"/>
-    <mergeCell ref="A80:A94"/>
-    <mergeCell ref="B80:B94"/>
-    <mergeCell ref="C80:C94"/>
-    <mergeCell ref="E80:E94"/>
-    <mergeCell ref="A98:A99"/>
-    <mergeCell ref="B98:B99"/>
-    <mergeCell ref="C98:C99"/>
-    <mergeCell ref="E98:E99"/>
-    <mergeCell ref="A37:A64"/>
-    <mergeCell ref="B37:B64"/>
-    <mergeCell ref="C37:C64"/>
-    <mergeCell ref="E37:E64"/>
-    <mergeCell ref="A65:A79"/>
-    <mergeCell ref="B65:B79"/>
-    <mergeCell ref="C65:C79"/>
-    <mergeCell ref="E65:E79"/>
-    <mergeCell ref="A32:A33"/>
-    <mergeCell ref="B32:B33"/>
-    <mergeCell ref="C32:C33"/>
-    <mergeCell ref="E32:E33"/>
-    <mergeCell ref="A34:A35"/>
-    <mergeCell ref="B34:B35"/>
-    <mergeCell ref="C34:C35"/>
-    <mergeCell ref="E34:E35"/>
-    <mergeCell ref="A28:A29"/>
-    <mergeCell ref="B28:B29"/>
-    <mergeCell ref="C28:C29"/>
-    <mergeCell ref="E28:E29"/>
-    <mergeCell ref="A30:A31"/>
-    <mergeCell ref="B30:B31"/>
-    <mergeCell ref="C30:C31"/>
-    <mergeCell ref="E30:E31"/>
-    <mergeCell ref="A24:A25"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="C24:C25"/>
-    <mergeCell ref="E24:E25"/>
-    <mergeCell ref="A26:A27"/>
-    <mergeCell ref="B26:B27"/>
-    <mergeCell ref="C26:C27"/>
-    <mergeCell ref="E26:E27"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="A6:A8"/>
-    <mergeCell ref="B6:B8"/>
-    <mergeCell ref="C6:C8"/>
-    <mergeCell ref="E6:E8"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="E10:E11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="cea7764e-6bf9-427d-be15-e74097e0a61c">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <SharedWithUsers xmlns="fb9ea31f-0ab8-44ff-80d1-5777f6d9d945">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-    <MediaLengthInSeconds xmlns="cea7764e-6bf9-427d-be15-e74097e0a61c" xsi:nil="true"/>
-    <Sign_x002d_off_x0020_status xmlns="cea7764e-6bf9-427d-be15-e74097e0a61c" xsi:nil="true"/>
-    <Title_x0020_URL xmlns="cea7764e-6bf9-427d-be15-e74097e0a61c">
-      <Url xsi:nil="true"/>
-      <Description xsi:nil="true"/>
-    </Title_x0020_URL>
-    <Mail_x0020_Sent xmlns="cea7764e-6bf9-427d-be15-e74097e0a61c">false</Mail_x0020_Sent>
-    <_Flow_SignoffStatus xmlns="cea7764e-6bf9-427d-be15-e74097e0a61c" xsi:nil="true"/>
-    <State xmlns="cea7764e-6bf9-427d-be15-e74097e0a61c">Open</State>
-    <Comments xmlns="cea7764e-6bf9-427d-be15-e74097e0a61c" xsi:nil="true"/>
-    <Lead_x0020_Signoff xmlns="cea7764e-6bf9-427d-be15-e74097e0a61c">false</Lead_x0020_Signoff>
-    <Title_x0020_ID xmlns="cea7764e-6bf9-427d-be15-e74097e0a61c" xsi:nil="true"/>
-    <TranslatedLang xmlns="cea7764e-6bf9-427d-be15-e74097e0a61c" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010039A62E282DDA434E979CD3E03185182E" ma:contentTypeVersion="33" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="a6c69cf93bfe1fca5d0e373365e7fdfc">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="cea7764e-6bf9-427d-be15-e74097e0a61c" xmlns:ns3="fb9ea31f-0ab8-44ff-80d1-5777f6d9d945" xmlns:ns4="230e9df3-be65-4c73-a93b-d1236ebd677e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="62cb4c6faf5eab163d0c8ea23c8ff408" ns1:_="" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -10639,34 +10688,49 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E53D8182-34C2-4EE5-8FD0-D750C3EB0900}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="fb9ea31f-0ab8-44ff-80d1-5777f6d9d945"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
-    <ds:schemaRef ds:uri="cea7764e-6bf9-427d-be15-e74097e0a61c"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3F377113-5718-41B1-A1CE-B96F830D3573}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="cea7764e-6bf9-427d-be15-e74097e0a61c">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <SharedWithUsers xmlns="fb9ea31f-0ab8-44ff-80d1-5777f6d9d945">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+    <MediaLengthInSeconds xmlns="cea7764e-6bf9-427d-be15-e74097e0a61c" xsi:nil="true"/>
+    <Sign_x002d_off_x0020_status xmlns="cea7764e-6bf9-427d-be15-e74097e0a61c" xsi:nil="true"/>
+    <Title_x0020_URL xmlns="cea7764e-6bf9-427d-be15-e74097e0a61c">
+      <Url xsi:nil="true"/>
+      <Description xsi:nil="true"/>
+    </Title_x0020_URL>
+    <Mail_x0020_Sent xmlns="cea7764e-6bf9-427d-be15-e74097e0a61c">false</Mail_x0020_Sent>
+    <_Flow_SignoffStatus xmlns="cea7764e-6bf9-427d-be15-e74097e0a61c" xsi:nil="true"/>
+    <State xmlns="cea7764e-6bf9-427d-be15-e74097e0a61c">Open</State>
+    <Comments xmlns="cea7764e-6bf9-427d-be15-e74097e0a61c" xsi:nil="true"/>
+    <Lead_x0020_Signoff xmlns="cea7764e-6bf9-427d-be15-e74097e0a61c">false</Lead_x0020_Signoff>
+    <Title_x0020_ID xmlns="cea7764e-6bf9-427d-be15-e74097e0a61c" xsi:nil="true"/>
+    <TranslatedLang xmlns="cea7764e-6bf9-427d-be15-e74097e0a61c" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{23B9621B-458A-4676-8042-F53348150B3A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -10687,6 +10751,33 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3F377113-5718-41B1-A1CE-B96F830D3573}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E53D8182-34C2-4EE5-8FD0-D750C3EB0900}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="fb9ea31f-0ab8-44ff-80d1-5777f6d9d945"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
+    <ds:schemaRef ds:uri="cea7764e-6bf9-427d-be15-e74097e0a61c"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{87867195-f2b8-4ac2-b0b6-6bb73cb33afc}" enabled="1" method="Privileged" siteId="{72f988bf-86f1-41af-91ab-2d7cd011db47}" contentBits="0" removed="0"/>

</xml_diff>

<commit_message>
feat: security management group
</commit_message>
<xml_diff>
--- a/docs/static/examples/tf/accelerator/config/checklist.xlsx
+++ b/docs/static/examples/tf/accelerator/config/checklist.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\Azure-Landing-Zones\docs\static\examples\tf\accelerator\config\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jaredholgate\Code\azure-landing-zones\docs\static\examples\tf\accelerator\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AAF9BDE-F5B8-4497-AF3D-23E3B3919670}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29446722-CE5D-4CA6-97DF-6F4B77F3077C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" tabRatio="415" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" tabRatio="415" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Accelerator - Bootstrap" sheetId="13" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1408" uniqueCount="805">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1412" uniqueCount="807">
   <si>
     <t>Description</t>
   </si>
@@ -2589,6 +2589,12 @@
   </si>
   <si>
     <t>"mgmt"</t>
+  </si>
+  <si>
+    <t>Security subscription id</t>
+  </si>
+  <si>
+    <t>The subscription id for the security subscription</t>
   </si>
 </sst>
 </file>
@@ -2881,7 +2887,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -3043,6 +3049,9 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3399,24 +3408,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D33EA6D-E1B5-4751-908D-ADA676A42D17}">
-  <dimension ref="A1:G45"/>
+  <dimension ref="A1:G46"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="7.85546875" style="42" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="42.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="39.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.81640625" style="42" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="42.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="39.81640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="38" customWidth="1"/>
-    <col min="5" max="5" width="50.42578125" customWidth="1"/>
-    <col min="6" max="7" width="46.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="50.453125" customWidth="1"/>
+    <col min="6" max="7" width="46.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="77.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="77.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="48" t="s">
         <v>787</v>
       </c>
@@ -3427,7 +3436,7 @@
       <c r="F1" s="48"/>
       <c r="G1" s="48"/>
     </row>
-    <row r="3" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="44" t="s">
         <v>790</v>
       </c>
@@ -3450,7 +3459,7 @@
         <v>683</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A4" s="43">
         <v>1</v>
       </c>
@@ -3469,7 +3478,7 @@
       <c r="F4" s="38"/>
       <c r="G4" s="34"/>
     </row>
-    <row r="5" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A5" s="43">
         <v>2</v>
       </c>
@@ -3488,7 +3497,7 @@
       <c r="F5" s="35"/>
       <c r="G5" s="34"/>
     </row>
-    <row r="6" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="87" x14ac:dyDescent="0.35">
       <c r="A6" s="43">
         <v>3</v>
       </c>
@@ -3507,7 +3516,7 @@
       <c r="F6" s="35"/>
       <c r="G6" s="34"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" s="45"/>
       <c r="B7" s="36"/>
       <c r="C7" s="37"/>
@@ -3516,7 +3525,7 @@
       <c r="F7" s="36"/>
       <c r="G7" s="36"/>
     </row>
-    <row r="8" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" s="43">
         <v>4</v>
       </c>
@@ -3537,7 +3546,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A9" s="43">
         <v>5</v>
       </c>
@@ -3558,7 +3567,7 @@
         <v>684</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A10" s="43">
         <v>6</v>
       </c>
@@ -3579,7 +3588,7 @@
       </c>
       <c r="G10" s="34"/>
     </row>
-    <row r="11" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A11" s="43">
         <v>7</v>
       </c>
@@ -3598,7 +3607,7 @@
       <c r="F11" s="35"/>
       <c r="G11" s="34"/>
     </row>
-    <row r="12" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A12" s="43">
         <v>7</v>
       </c>
@@ -3617,7 +3626,7 @@
       <c r="F12" s="35"/>
       <c r="G12" s="34"/>
     </row>
-    <row r="13" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A13" s="43">
         <v>7</v>
       </c>
@@ -3636,152 +3645,150 @@
       <c r="F13" s="35"/>
       <c r="G13" s="34"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="45"/>
-      <c r="B14" s="36"/>
-      <c r="C14" s="37"/>
-      <c r="D14" s="36"/>
-      <c r="E14" s="37"/>
-      <c r="F14" s="36"/>
-      <c r="G14" s="36"/>
-    </row>
-    <row r="15" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="43">
+    <row r="14" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A14" s="43">
+        <v>7</v>
+      </c>
+      <c r="B14" s="34" t="s">
+        <v>805</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>806</v>
+      </c>
+      <c r="D14" s="34" t="s">
+        <v>504</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>688</v>
+      </c>
+      <c r="F14" s="56"/>
+      <c r="G14" s="34"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A15" s="45"/>
+      <c r="B15" s="36"/>
+      <c r="C15" s="37"/>
+      <c r="D15" s="36"/>
+      <c r="E15" s="37"/>
+      <c r="F15" s="36"/>
+      <c r="G15" s="36"/>
+    </row>
+    <row r="16" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A16" s="43">
         <v>8</v>
       </c>
-      <c r="B15" s="34" t="s">
+      <c r="B16" s="34" t="s">
         <v>695</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="C16" s="1" t="s">
         <v>696</v>
       </c>
-      <c r="D15" s="34" t="s">
+      <c r="D16" s="34" t="s">
         <v>46</v>
       </c>
-      <c r="E15" s="1" t="s">
+      <c r="E16" s="1" t="s">
         <v>697</v>
       </c>
-      <c r="F15" s="40" t="s">
+      <c r="F16" s="40" t="s">
         <v>44</v>
       </c>
-      <c r="G15" s="34"/>
-    </row>
-    <row r="16" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="43">
-        <v>9</v>
-      </c>
-      <c r="B16" s="34" t="s">
-        <v>698</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>699</v>
-      </c>
-      <c r="D16" s="34" t="s">
-        <v>47</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>700</v>
-      </c>
-      <c r="F16" s="35" t="s">
-        <v>16</v>
-      </c>
       <c r="G16" s="34"/>
     </row>
-    <row r="17" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A17" s="43">
         <v>9</v>
       </c>
       <c r="B17" s="34" t="s">
-        <v>803</v>
+        <v>698</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>701</v>
+        <v>699</v>
       </c>
       <c r="D17" s="34" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>700</v>
       </c>
       <c r="F17" s="35" t="s">
-        <v>804</v>
+        <v>16</v>
       </c>
       <c r="G17" s="34"/>
     </row>
-    <row r="18" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A18" s="43">
         <v>9</v>
       </c>
       <c r="B18" s="34" t="s">
+        <v>803</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>701</v>
+      </c>
+      <c r="D18" s="34" t="s">
+        <v>49</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>700</v>
+      </c>
+      <c r="F18" s="35" t="s">
+        <v>804</v>
+      </c>
+      <c r="G18" s="34"/>
+    </row>
+    <row r="19" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A19" s="43">
+        <v>9</v>
+      </c>
+      <c r="B19" s="34" t="s">
         <v>703</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="C19" s="1" t="s">
         <v>704</v>
       </c>
-      <c r="D18" s="34" t="s">
+      <c r="D19" s="34" t="s">
         <v>50</v>
       </c>
-      <c r="E18" s="1" t="s">
+      <c r="E19" s="1" t="s">
         <v>702</v>
       </c>
-      <c r="F18" s="35">
+      <c r="F19" s="35">
         <v>1</v>
       </c>
-      <c r="G18" s="34"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="45"/>
-      <c r="B19" s="36"/>
-      <c r="C19" s="37"/>
-      <c r="D19" s="36"/>
-      <c r="E19" s="37"/>
-      <c r="F19" s="36"/>
-      <c r="G19" s="36"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="46"/>
-      <c r="B20" s="39" t="s">
-        <v>717</v>
-      </c>
+      <c r="G19" s="34"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A20" s="45"/>
+      <c r="B20" s="36"/>
       <c r="C20" s="37"/>
       <c r="D20" s="36"/>
       <c r="E20" s="37"/>
       <c r="F20" s="36"/>
       <c r="G20" s="36"/>
     </row>
-    <row r="21" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A21" s="43">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A21" s="46"/>
+      <c r="B21" s="39" t="s">
+        <v>717</v>
+      </c>
+      <c r="C21" s="37"/>
+      <c r="D21" s="36"/>
+      <c r="E21" s="37"/>
+      <c r="F21" s="36"/>
+      <c r="G21" s="36"/>
+    </row>
+    <row r="22" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A22" s="43">
         <v>11</v>
       </c>
-      <c r="B21" s="34" t="s">
+      <c r="B22" s="34" t="s">
         <v>719</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="C22" s="1" t="s">
         <v>720</v>
       </c>
-      <c r="D21" s="34" t="s">
+      <c r="D22" s="34" t="s">
         <v>45</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>711</v>
-      </c>
-      <c r="F21" s="40" t="s">
-        <v>123</v>
-      </c>
-      <c r="G21" s="34"/>
-    </row>
-    <row r="22" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A22" s="43">
-        <v>10</v>
-      </c>
-      <c r="B22" s="34" t="s">
-        <v>721</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>723</v>
-      </c>
-      <c r="D22" s="34" t="s">
-        <v>53</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>711</v>
@@ -3791,380 +3798,380 @@
       </c>
       <c r="G22" s="34"/>
     </row>
-    <row r="23" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A23" s="43"/>
+    <row r="23" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A23" s="43">
+        <v>10</v>
+      </c>
       <c r="B23" s="34" t="s">
-        <v>724</v>
+        <v>721</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>725</v>
+        <v>723</v>
       </c>
       <c r="D23" s="34" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E23" s="1" t="s">
         <v>711</v>
       </c>
       <c r="F23" s="40" t="s">
+        <v>123</v>
+      </c>
+      <c r="G23" s="34"/>
+    </row>
+    <row r="24" spans="1:7" ht="58" x14ac:dyDescent="0.35">
+      <c r="A24" s="43"/>
+      <c r="B24" s="34" t="s">
+        <v>724</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>725</v>
+      </c>
+      <c r="D24" s="34" t="s">
+        <v>54</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>711</v>
+      </c>
+      <c r="F24" s="40" t="s">
         <v>133</v>
       </c>
-      <c r="G23" s="34"/>
-    </row>
-    <row r="24" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A24" s="43">
-        <v>11</v>
-      </c>
-      <c r="B24" s="34" t="s">
-        <v>726</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>727</v>
-      </c>
-      <c r="D24" s="34" t="s">
-        <v>55</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>728</v>
-      </c>
-      <c r="F24" s="35"/>
-      <c r="G24" s="34" t="s">
-        <v>729</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="G24" s="34"/>
+    </row>
+    <row r="25" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A25" s="43">
         <v>11</v>
       </c>
       <c r="B25" s="34" t="s">
+        <v>726</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>727</v>
+      </c>
+      <c r="D25" s="34" t="s">
+        <v>55</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>728</v>
+      </c>
+      <c r="F25" s="35"/>
+      <c r="G25" s="34" t="s">
+        <v>729</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A26" s="43">
+        <v>11</v>
+      </c>
+      <c r="B26" s="34" t="s">
         <v>722</v>
       </c>
-      <c r="C25" s="1" t="s">
+      <c r="C26" s="1" t="s">
         <v>730</v>
       </c>
-      <c r="D25" s="34" t="s">
+      <c r="D26" s="34" t="s">
         <v>56</v>
       </c>
-      <c r="E25" s="1" t="s">
+      <c r="E26" s="1" t="s">
         <v>711</v>
       </c>
-      <c r="F25" s="40" t="s">
+      <c r="F26" s="40" t="s">
         <v>123</v>
       </c>
-      <c r="G25" s="34"/>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="45"/>
-      <c r="B26" s="36"/>
-      <c r="C26" s="37"/>
-      <c r="D26" s="36"/>
-      <c r="E26" s="37"/>
-      <c r="F26" s="36"/>
-      <c r="G26" s="36"/>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="46"/>
-      <c r="B27" s="39" t="s">
-        <v>716</v>
-      </c>
+      <c r="G26" s="34"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A27" s="45"/>
+      <c r="B27" s="36"/>
       <c r="C27" s="37"/>
       <c r="D27" s="36"/>
       <c r="E27" s="37"/>
       <c r="F27" s="36"/>
       <c r="G27" s="36"/>
     </row>
-    <row r="28" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A28" s="43">
-        <v>11</v>
-      </c>
-      <c r="B28" s="34" t="s">
-        <v>731</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>738</v>
-      </c>
-      <c r="D28" s="34" t="s">
-        <v>57</v>
-      </c>
-      <c r="E28" s="1"/>
-      <c r="F28" s="35"/>
-      <c r="G28" s="34"/>
-    </row>
-    <row r="29" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A28" s="46"/>
+      <c r="B28" s="39" t="s">
+        <v>716</v>
+      </c>
+      <c r="C28" s="37"/>
+      <c r="D28" s="36"/>
+      <c r="E28" s="37"/>
+      <c r="F28" s="36"/>
+      <c r="G28" s="36"/>
+    </row>
+    <row r="29" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A29" s="43">
         <v>11</v>
       </c>
       <c r="B29" s="34" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>737</v>
+        <v>738</v>
       </c>
       <c r="D29" s="34" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E29" s="1"/>
       <c r="F29" s="35"/>
       <c r="G29" s="34"/>
     </row>
-    <row r="30" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A30" s="43">
         <v>11</v>
       </c>
       <c r="B30" s="34" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>736</v>
+        <v>737</v>
       </c>
       <c r="D30" s="34" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E30" s="1"/>
       <c r="F30" s="35"/>
       <c r="G30" s="34"/>
     </row>
-    <row r="31" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A31" s="43">
         <v>11</v>
       </c>
       <c r="B31" s="34" t="s">
-        <v>735</v>
+        <v>733</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>739</v>
+        <v>736</v>
       </c>
       <c r="D31" s="34" t="s">
-        <v>60</v>
-      </c>
-      <c r="E31" s="1" t="s">
-        <v>711</v>
-      </c>
-      <c r="F31" s="40" t="s">
-        <v>133</v>
-      </c>
+        <v>59</v>
+      </c>
+      <c r="E31" s="1"/>
+      <c r="F31" s="35"/>
       <c r="G31" s="34"/>
     </row>
-    <row r="32" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A32" s="43">
         <v>11</v>
       </c>
       <c r="B32" s="34" t="s">
-        <v>740</v>
+        <v>735</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>741</v>
+        <v>739</v>
       </c>
       <c r="D32" s="34" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E32" s="1" t="s">
         <v>711</v>
       </c>
       <c r="F32" s="40" t="s">
-        <v>123</v>
+        <v>133</v>
       </c>
       <c r="G32" s="34"/>
     </row>
-    <row r="33" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" ht="58" x14ac:dyDescent="0.35">
       <c r="A33" s="43">
         <v>11</v>
       </c>
       <c r="B33" s="34" t="s">
+        <v>740</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>741</v>
+      </c>
+      <c r="D33" s="34" t="s">
+        <v>61</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>711</v>
+      </c>
+      <c r="F33" s="40" t="s">
+        <v>123</v>
+      </c>
+      <c r="G33" s="34"/>
+    </row>
+    <row r="34" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A34" s="43">
+        <v>11</v>
+      </c>
+      <c r="B34" s="34" t="s">
         <v>734</v>
       </c>
-      <c r="C33" s="1" t="s">
+      <c r="C34" s="1" t="s">
         <v>742</v>
       </c>
-      <c r="D33" s="34" t="s">
+      <c r="D34" s="34" t="s">
         <v>62</v>
       </c>
-      <c r="E33" s="1"/>
-      <c r="F33" s="35"/>
-      <c r="G33" s="34"/>
-    </row>
-    <row r="34" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A34" s="43">
+      <c r="E34" s="1"/>
+      <c r="F34" s="35"/>
+      <c r="G34" s="34"/>
+    </row>
+    <row r="35" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A35" s="43">
         <v>10</v>
       </c>
-      <c r="B34" s="34" t="s">
+      <c r="B35" s="34" t="s">
         <v>743</v>
       </c>
-      <c r="C34" s="1" t="s">
+      <c r="C35" s="1" t="s">
         <v>744</v>
       </c>
-      <c r="D34" s="34" t="s">
+      <c r="D35" s="34" t="s">
         <v>52</v>
       </c>
-      <c r="E34" s="1"/>
-      <c r="F34" s="40" t="s">
+      <c r="E35" s="1"/>
+      <c r="F35" s="40" t="s">
         <v>123</v>
       </c>
-      <c r="G34" s="34"/>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" s="45"/>
-      <c r="B35" s="36"/>
-      <c r="C35" s="37"/>
-      <c r="D35" s="36"/>
-      <c r="E35" s="37"/>
-      <c r="F35" s="36"/>
-      <c r="G35" s="36"/>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" s="46"/>
-      <c r="B36" s="39" t="s">
-        <v>718</v>
-      </c>
+      <c r="G35" s="34"/>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A36" s="45"/>
+      <c r="B36" s="36"/>
       <c r="C36" s="37"/>
       <c r="D36" s="36"/>
       <c r="E36" s="37"/>
       <c r="F36" s="36"/>
       <c r="G36" s="36"/>
     </row>
-    <row r="37" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A37" s="43">
-        <v>11</v>
-      </c>
-      <c r="B37" s="34" t="s">
-        <v>752</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>750</v>
-      </c>
-      <c r="D37" s="34" t="s">
-        <v>63</v>
-      </c>
-      <c r="E37" s="1"/>
-      <c r="F37" s="35"/>
-      <c r="G37" s="34"/>
-    </row>
-    <row r="38" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A37" s="46"/>
+      <c r="B37" s="39" t="s">
+        <v>718</v>
+      </c>
+      <c r="C37" s="37"/>
+      <c r="D37" s="36"/>
+      <c r="E37" s="37"/>
+      <c r="F37" s="36"/>
+      <c r="G37" s="36"/>
+    </row>
+    <row r="38" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A38" s="43">
         <v>11</v>
       </c>
       <c r="B38" s="34" t="s">
-        <v>751</v>
+        <v>752</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>749</v>
+        <v>750</v>
       </c>
       <c r="D38" s="34" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E38" s="1"/>
       <c r="F38" s="35"/>
       <c r="G38" s="34"/>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A39" s="43">
         <v>11</v>
       </c>
       <c r="B39" s="34" t="s">
-        <v>747</v>
+        <v>751</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>748</v>
+        <v>749</v>
       </c>
       <c r="D39" s="34" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E39" s="1"/>
       <c r="F39" s="35"/>
       <c r="G39" s="34"/>
     </row>
-    <row r="40" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A40" s="43">
+        <v>11</v>
+      </c>
+      <c r="B40" s="34" t="s">
+        <v>747</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>748</v>
+      </c>
+      <c r="D40" s="34" t="s">
+        <v>65</v>
+      </c>
+      <c r="E40" s="1"/>
+      <c r="F40" s="35"/>
+      <c r="G40" s="34"/>
+    </row>
+    <row r="41" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A41" s="43">
         <v>10</v>
       </c>
-      <c r="B40" s="34" t="s">
+      <c r="B41" s="34" t="s">
         <v>745</v>
       </c>
-      <c r="C40" s="1" t="s">
+      <c r="C41" s="1" t="s">
         <v>746</v>
       </c>
-      <c r="D40" s="34" t="s">
+      <c r="D41" s="34" t="s">
         <v>506</v>
       </c>
-      <c r="E40" s="1"/>
-      <c r="F40" s="40" t="s">
+      <c r="E41" s="1"/>
+      <c r="F41" s="40" t="s">
         <v>123</v>
       </c>
-      <c r="G40" s="34"/>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41" s="45"/>
-      <c r="B41" s="36"/>
-      <c r="C41" s="37"/>
-      <c r="D41" s="36"/>
-      <c r="E41" s="37"/>
-      <c r="F41" s="36"/>
-      <c r="G41" s="36"/>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A42" s="46"/>
-      <c r="B42" s="39" t="s">
-        <v>705</v>
-      </c>
+      <c r="G41" s="34"/>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A42" s="45"/>
+      <c r="B42" s="36"/>
       <c r="C42" s="37"/>
       <c r="D42" s="36"/>
       <c r="E42" s="37"/>
       <c r="F42" s="36"/>
       <c r="G42" s="36"/>
     </row>
-    <row r="43" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A43" s="43">
-        <v>11</v>
-      </c>
-      <c r="B43" s="34" t="s">
-        <v>706</v>
-      </c>
-      <c r="C43" s="1" t="s">
-        <v>707</v>
-      </c>
-      <c r="D43" s="34" t="s">
-        <v>66</v>
-      </c>
-      <c r="E43" s="1" t="s">
-        <v>708</v>
-      </c>
-      <c r="F43" s="40" t="s">
-        <v>44</v>
-      </c>
-      <c r="G43" s="34"/>
-    </row>
-    <row r="44" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A43" s="46"/>
+      <c r="B43" s="39" t="s">
+        <v>705</v>
+      </c>
+      <c r="C43" s="37"/>
+      <c r="D43" s="36"/>
+      <c r="E43" s="37"/>
+      <c r="F43" s="36"/>
+      <c r="G43" s="36"/>
+    </row>
+    <row r="44" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A44" s="43">
         <v>11</v>
       </c>
       <c r="B44" s="34" t="s">
-        <v>709</v>
+        <v>706</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>710</v>
+        <v>707</v>
       </c>
       <c r="D44" s="34" t="s">
-        <v>712</v>
+        <v>66</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>711</v>
+        <v>708</v>
       </c>
       <c r="F44" s="40" t="s">
-        <v>123</v>
+        <v>44</v>
       </c>
       <c r="G44" s="34"/>
     </row>
-    <row r="45" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A45" s="43">
         <v>11</v>
       </c>
       <c r="B45" s="34" t="s">
-        <v>713</v>
+        <v>709</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>715</v>
+        <v>710</v>
       </c>
       <c r="D45" s="34" t="s">
-        <v>714</v>
+        <v>712</v>
       </c>
       <c r="E45" s="1" t="s">
         <v>711</v>
@@ -4173,6 +4180,27 @@
         <v>123</v>
       </c>
       <c r="G45" s="34"/>
+    </row>
+    <row r="46" spans="1:7" ht="58" x14ac:dyDescent="0.35">
+      <c r="A46" s="43">
+        <v>11</v>
+      </c>
+      <c r="B46" s="34" t="s">
+        <v>713</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>715</v>
+      </c>
+      <c r="D46" s="34" t="s">
+        <v>714</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>711</v>
+      </c>
+      <c r="F46" s="40" t="s">
+        <v>123</v>
+      </c>
+      <c r="G46" s="34"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -4187,25 +4215,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA5559C7-55D7-4845-9950-8EEEDB97C0FA}">
   <dimension ref="A1:H229"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A35" sqref="A35:XFD35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="41.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="47.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="74.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="93.85546875" style="4" customWidth="1"/>
-    <col min="5" max="5" width="38.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="41.1796875" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="47.81640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="74.26953125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="93.81640625" style="4" customWidth="1"/>
+    <col min="5" max="5" width="38.26953125" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="34" style="2" customWidth="1"/>
-    <col min="7" max="7" width="18.28515625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="18.26953125" style="2" customWidth="1"/>
     <col min="8" max="8" width="21" style="2" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="2"/>
+    <col min="9" max="16384" width="9.1796875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="52.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="26" x14ac:dyDescent="0.35">
       <c r="A1" s="12" t="s">
         <v>7</v>
       </c>
@@ -4231,7 +4259,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="43.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="9"/>
       <c r="B2" s="9"/>
       <c r="C2" s="10" t="s">
@@ -4243,7 +4271,7 @@
       <c r="G2" s="9"/>
       <c r="H2" s="9"/>
     </row>
-    <row r="3" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
         <v>13</v>
       </c>
@@ -4263,7 +4291,7 @@
       <c r="G3" s="5"/>
       <c r="H3" s="5"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="s">
         <v>13</v>
       </c>
@@ -4281,7 +4309,7 @@
       <c r="G4" s="5"/>
       <c r="H4" s="5"/>
     </row>
-    <row r="5" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
         <v>13</v>
       </c>
@@ -4301,7 +4329,7 @@
       <c r="G5" s="5"/>
       <c r="H5" s="5"/>
     </row>
-    <row r="6" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="s">
         <v>13</v>
       </c>
@@ -4319,7 +4347,7 @@
       <c r="G6" s="5"/>
       <c r="H6" s="5"/>
     </row>
-    <row r="7" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A7" s="5" t="s">
         <v>13</v>
       </c>
@@ -4337,7 +4365,7 @@
       <c r="G7" s="5"/>
       <c r="H7" s="5"/>
     </row>
-    <row r="8" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A8" s="5" t="s">
         <v>13</v>
       </c>
@@ -4355,7 +4383,7 @@
       <c r="G8" s="5"/>
       <c r="H8" s="5"/>
     </row>
-    <row r="9" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A9" s="5" t="s">
         <v>13</v>
       </c>
@@ -4375,7 +4403,7 @@
       <c r="G9" s="5"/>
       <c r="H9" s="5"/>
     </row>
-    <row r="10" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A10" s="5" t="s">
         <v>13</v>
       </c>
@@ -4395,7 +4423,7 @@
       <c r="G10" s="5"/>
       <c r="H10" s="5"/>
     </row>
-    <row r="11" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" s="5" t="s">
         <v>13</v>
       </c>
@@ -4413,7 +4441,7 @@
       <c r="G11" s="5"/>
       <c r="H11" s="5"/>
     </row>
-    <row r="12" spans="1:8" ht="51" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" ht="51" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="9"/>
       <c r="B12" s="7"/>
       <c r="C12" s="10" t="s">
@@ -4425,7 +4453,7 @@
       <c r="G12" s="8"/>
       <c r="H12" s="8"/>
     </row>
-    <row r="13" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A13" s="5" t="s">
         <v>67</v>
       </c>
@@ -4443,7 +4471,7 @@
       <c r="G13" s="5"/>
       <c r="H13" s="5"/>
     </row>
-    <row r="14" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A14" s="6" t="s">
         <v>67</v>
       </c>
@@ -4461,7 +4489,7 @@
       <c r="G14" s="6"/>
       <c r="H14" s="6"/>
     </row>
-    <row r="15" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A15" s="5" t="s">
         <v>67</v>
       </c>
@@ -4479,7 +4507,7 @@
       <c r="G15" s="5"/>
       <c r="H15" s="5"/>
     </row>
-    <row r="16" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A16" s="6" t="s">
         <v>67</v>
       </c>
@@ -4497,7 +4525,7 @@
       <c r="G16" s="6"/>
       <c r="H16" s="6"/>
     </row>
-    <row r="17" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A17" s="5" t="s">
         <v>67</v>
       </c>
@@ -4515,7 +4543,7 @@
       <c r="G17" s="5"/>
       <c r="H17" s="5"/>
     </row>
-    <row r="18" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A18" s="5" t="s">
         <v>67</v>
       </c>
@@ -4533,7 +4561,7 @@
       <c r="G18" s="6"/>
       <c r="H18" s="6"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A19" s="14" t="s">
         <v>67</v>
       </c>
@@ -4551,7 +4579,7 @@
       <c r="G19" s="14"/>
       <c r="H19" s="14"/>
     </row>
-    <row r="20" spans="1:8" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" ht="50.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="9"/>
       <c r="B20" s="7"/>
       <c r="C20" s="10" t="s">
@@ -4563,7 +4591,7 @@
       <c r="G20" s="8"/>
       <c r="H20" s="8"/>
     </row>
-    <row r="21" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A21" s="5" t="s">
         <v>84</v>
       </c>
@@ -4581,7 +4609,7 @@
       <c r="G21" s="5"/>
       <c r="H21" s="5"/>
     </row>
-    <row r="22" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A22" s="6" t="s">
         <v>87</v>
       </c>
@@ -4599,7 +4627,7 @@
       <c r="G22" s="6"/>
       <c r="H22" s="6"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A23" s="5" t="s">
         <v>87</v>
       </c>
@@ -4617,7 +4645,7 @@
       <c r="G23" s="5"/>
       <c r="H23" s="5"/>
     </row>
-    <row r="24" spans="1:8" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" ht="66.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="9"/>
       <c r="B24" s="9"/>
       <c r="C24" s="10" t="s">
@@ -4629,7 +4657,7 @@
       <c r="G24" s="7"/>
       <c r="H24" s="9"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A25" s="6" t="s">
         <v>90</v>
       </c>
@@ -4649,7 +4677,7 @@
       <c r="G25" s="6"/>
       <c r="H25" s="6"/>
     </row>
-    <row r="26" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A26" s="5" t="s">
         <v>90</v>
       </c>
@@ -4669,7 +4697,7 @@
       <c r="G26" s="5"/>
       <c r="H26" s="5"/>
     </row>
-    <row r="27" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A27" s="6" t="s">
         <v>90</v>
       </c>
@@ -4689,7 +4717,7 @@
       <c r="G27" s="6"/>
       <c r="H27" s="6"/>
     </row>
-    <row r="28" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A28" s="14" t="s">
         <v>90</v>
       </c>
@@ -4707,7 +4735,7 @@
       <c r="G28" s="14"/>
       <c r="H28" s="14"/>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A29" s="6" t="s">
         <v>90</v>
       </c>
@@ -4725,7 +4753,7 @@
       <c r="G29" s="6"/>
       <c r="H29" s="6"/>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A30" s="14" t="s">
         <v>90</v>
       </c>
@@ -4745,7 +4773,7 @@
       <c r="G30" s="14"/>
       <c r="H30" s="14"/>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A31" s="6" t="s">
         <v>90</v>
       </c>
@@ -4763,7 +4791,7 @@
       <c r="G31" s="6"/>
       <c r="H31" s="6"/>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A32" s="14" t="s">
         <v>90</v>
       </c>
@@ -4781,7 +4809,7 @@
       <c r="G32" s="14"/>
       <c r="H32" s="14"/>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A33" s="6" t="s">
         <v>90</v>
       </c>
@@ -4799,7 +4827,7 @@
       <c r="G33" s="6"/>
       <c r="H33" s="6"/>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A34" s="14" t="s">
         <v>90</v>
       </c>
@@ -4817,7 +4845,7 @@
       <c r="G34" s="14"/>
       <c r="H34" s="14"/>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A35" s="14" t="s">
         <v>90</v>
       </c>
@@ -4835,7 +4863,7 @@
       <c r="G35" s="14"/>
       <c r="H35" s="14"/>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A36" s="6" t="s">
         <v>90</v>
       </c>
@@ -4853,7 +4881,7 @@
       <c r="G36" s="6"/>
       <c r="H36" s="6"/>
     </row>
-    <row r="37" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A37" s="14" t="s">
         <v>90</v>
       </c>
@@ -4871,7 +4899,7 @@
       <c r="G37" s="14"/>
       <c r="H37" s="14"/>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A38" s="6" t="s">
         <v>90</v>
       </c>
@@ -4891,7 +4919,7 @@
       <c r="G38" s="6"/>
       <c r="H38" s="6"/>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A39" s="5" t="s">
         <v>90</v>
       </c>
@@ -4911,7 +4939,7 @@
       <c r="G39" s="5"/>
       <c r="H39" s="5"/>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A40" s="6" t="s">
         <v>90</v>
       </c>
@@ -4931,7 +4959,7 @@
       <c r="G40" s="6"/>
       <c r="H40" s="6"/>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A41" s="5" t="s">
         <v>90</v>
       </c>
@@ -4951,7 +4979,7 @@
       <c r="G41" s="5"/>
       <c r="H41" s="5"/>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A42" s="6" t="s">
         <v>90</v>
       </c>
@@ -4971,7 +4999,7 @@
       <c r="G42" s="6"/>
       <c r="H42" s="6"/>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A43" s="5" t="s">
         <v>90</v>
       </c>
@@ -4991,7 +5019,7 @@
       <c r="G43" s="5"/>
       <c r="H43" s="5"/>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A44" s="6" t="s">
         <v>90</v>
       </c>
@@ -5011,7 +5039,7 @@
       <c r="G44" s="6"/>
       <c r="H44" s="6"/>
     </row>
-    <row r="45" spans="1:8" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" ht="48.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A45" s="9"/>
       <c r="B45" s="9"/>
       <c r="C45" s="10" t="s">
@@ -5023,7 +5051,7 @@
       <c r="G45" s="9"/>
       <c r="H45" s="9"/>
     </row>
-    <row r="46" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A46" s="6" t="s">
         <v>153</v>
       </c>
@@ -5041,7 +5069,7 @@
       <c r="G46" s="6"/>
       <c r="H46" s="6"/>
     </row>
-    <row r="47" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A47" s="5" t="s">
         <v>153</v>
       </c>
@@ -5059,7 +5087,7 @@
       <c r="G47" s="5"/>
       <c r="H47" s="5"/>
     </row>
-    <row r="48" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A48" s="6" t="s">
         <v>153</v>
       </c>
@@ -5077,7 +5105,7 @@
       <c r="G48" s="6"/>
       <c r="H48" s="6"/>
     </row>
-    <row r="49" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A49" s="14" t="s">
         <v>153</v>
       </c>
@@ -5095,7 +5123,7 @@
       <c r="G49" s="14"/>
       <c r="H49" s="14"/>
     </row>
-    <row r="50" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A50" s="6" t="s">
         <v>153</v>
       </c>
@@ -5113,7 +5141,7 @@
       <c r="G50" s="6"/>
       <c r="H50" s="6"/>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A51" s="14" t="s">
         <v>153</v>
       </c>
@@ -5131,7 +5159,7 @@
       <c r="G51" s="14"/>
       <c r="H51" s="14"/>
     </row>
-    <row r="52" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A52" s="6" t="s">
         <v>153</v>
       </c>
@@ -5149,7 +5177,7 @@
       <c r="G52" s="6"/>
       <c r="H52" s="6"/>
     </row>
-    <row r="53" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A53" s="14" t="s">
         <v>153</v>
       </c>
@@ -5167,7 +5195,7 @@
       <c r="G53" s="14"/>
       <c r="H53" s="14"/>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A54" s="6" t="s">
         <v>153</v>
       </c>
@@ -5185,7 +5213,7 @@
       <c r="G54" s="6"/>
       <c r="H54" s="6"/>
     </row>
-    <row r="55" spans="1:8" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8" ht="42.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A55" s="9"/>
       <c r="B55" s="9"/>
       <c r="C55" s="10" t="s">
@@ -5197,7 +5225,7 @@
       <c r="G55" s="9"/>
       <c r="H55" s="9"/>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A56" s="5" t="s">
         <v>169</v>
       </c>
@@ -5215,7 +5243,7 @@
       <c r="G56" s="5"/>
       <c r="H56" s="5"/>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A57" s="6" t="s">
         <v>169</v>
       </c>
@@ -5233,7 +5261,7 @@
       <c r="G57" s="6"/>
       <c r="H57" s="6"/>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A58" s="5" t="s">
         <v>169</v>
       </c>
@@ -5251,7 +5279,7 @@
       <c r="G58" s="5"/>
       <c r="H58" s="5"/>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A59" s="6" t="s">
         <v>169</v>
       </c>
@@ -5269,7 +5297,7 @@
       <c r="G59" s="6"/>
       <c r="H59" s="6"/>
     </row>
-    <row r="60" spans="1:8" ht="390" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:8" ht="377" x14ac:dyDescent="0.35">
       <c r="A60" s="5" t="s">
         <v>169</v>
       </c>
@@ -5287,7 +5315,7 @@
       <c r="G60" s="5"/>
       <c r="H60" s="5"/>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A61" s="6" t="s">
         <v>169</v>
       </c>
@@ -5305,7 +5333,7 @@
       <c r="G61" s="6"/>
       <c r="H61" s="6"/>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A62" s="5" t="s">
         <v>169</v>
       </c>
@@ -5325,7 +5353,7 @@
       <c r="G62" s="5"/>
       <c r="H62" s="5"/>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A63" s="6" t="s">
         <v>169</v>
       </c>
@@ -5345,7 +5373,7 @@
       <c r="G63" s="6"/>
       <c r="H63" s="6"/>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A64" s="5" t="s">
         <v>169</v>
       </c>
@@ -5363,7 +5391,7 @@
       <c r="G64" s="5"/>
       <c r="H64" s="5"/>
     </row>
-    <row r="65" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A65" s="6" t="s">
         <v>169</v>
       </c>
@@ -5383,7 +5411,7 @@
       <c r="G65" s="6"/>
       <c r="H65" s="6"/>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A66" s="5" t="s">
         <v>169</v>
       </c>
@@ -5401,7 +5429,7 @@
       <c r="G66" s="5"/>
       <c r="H66" s="5"/>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A67" s="6" t="s">
         <v>169</v>
       </c>
@@ -5419,7 +5447,7 @@
       <c r="G67" s="6"/>
       <c r="H67" s="6"/>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A68" s="5" t="s">
         <v>169</v>
       </c>
@@ -5437,7 +5465,7 @@
       <c r="G68" s="5"/>
       <c r="H68" s="5"/>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A69" s="6" t="s">
         <v>169</v>
       </c>
@@ -5455,7 +5483,7 @@
       <c r="G69" s="6"/>
       <c r="H69" s="6"/>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A70" s="5" t="s">
         <v>169</v>
       </c>
@@ -5473,7 +5501,7 @@
       <c r="G70" s="5"/>
       <c r="H70" s="5"/>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A71" s="6" t="s">
         <v>169</v>
       </c>
@@ -5491,7 +5519,7 @@
       <c r="G71" s="6"/>
       <c r="H71" s="6"/>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A72" s="5" t="s">
         <v>169</v>
       </c>
@@ -5511,7 +5539,7 @@
       <c r="G72" s="5"/>
       <c r="H72" s="5"/>
     </row>
-    <row r="73" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A73" s="6" t="s">
         <v>169</v>
       </c>
@@ -5531,7 +5559,7 @@
       <c r="G73" s="6"/>
       <c r="H73" s="6"/>
     </row>
-    <row r="74" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A74" s="5" t="s">
         <v>169</v>
       </c>
@@ -5551,7 +5579,7 @@
       <c r="G74" s="5"/>
       <c r="H74" s="5"/>
     </row>
-    <row r="75" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A75" s="6" t="s">
         <v>169</v>
       </c>
@@ -5571,7 +5599,7 @@
       <c r="G75" s="6"/>
       <c r="H75" s="6"/>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A76" s="5" t="s">
         <v>169</v>
       </c>
@@ -5589,7 +5617,7 @@
       <c r="G76" s="5"/>
       <c r="H76" s="5"/>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A77" s="6" t="s">
         <v>169</v>
       </c>
@@ -5607,7 +5635,7 @@
       <c r="G77" s="6"/>
       <c r="H77" s="6"/>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A78" s="5" t="s">
         <v>169</v>
       </c>
@@ -5625,7 +5653,7 @@
       <c r="G78" s="5"/>
       <c r="H78" s="5"/>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A79" s="6" t="s">
         <v>169</v>
       </c>
@@ -5643,7 +5671,7 @@
       <c r="G79" s="6"/>
       <c r="H79" s="6"/>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A80" s="5" t="s">
         <v>169</v>
       </c>
@@ -5661,7 +5689,7 @@
       <c r="G80" s="5"/>
       <c r="H80" s="5"/>
     </row>
-    <row r="81" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A81" s="6" t="s">
         <v>169</v>
       </c>
@@ -5677,7 +5705,7 @@
       <c r="G81" s="6"/>
       <c r="H81" s="6"/>
     </row>
-    <row r="82" spans="1:8" ht="255" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:8" ht="246.5" x14ac:dyDescent="0.35">
       <c r="A82" s="5" t="s">
         <v>169</v>
       </c>
@@ -5695,7 +5723,7 @@
       <c r="G82" s="5"/>
       <c r="H82" s="5"/>
     </row>
-    <row r="83" spans="1:8" ht="270" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:8" ht="261" x14ac:dyDescent="0.35">
       <c r="A83" s="6" t="s">
         <v>169</v>
       </c>
@@ -5713,7 +5741,7 @@
       <c r="G83" s="6"/>
       <c r="H83" s="6"/>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A84" s="5" t="s">
         <v>169</v>
       </c>
@@ -5731,7 +5759,7 @@
       <c r="G84" s="5"/>
       <c r="H84" s="5"/>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A85" s="6" t="s">
         <v>169</v>
       </c>
@@ -5749,7 +5777,7 @@
       <c r="G85" s="6"/>
       <c r="H85" s="6"/>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A86" s="5" t="s">
         <v>169</v>
       </c>
@@ -5769,7 +5797,7 @@
       <c r="G86" s="5"/>
       <c r="H86" s="5"/>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A87" s="6" t="s">
         <v>169</v>
       </c>
@@ -5789,7 +5817,7 @@
       <c r="G87" s="6"/>
       <c r="H87" s="6"/>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A88" s="5" t="s">
         <v>169</v>
       </c>
@@ -5809,7 +5837,7 @@
       <c r="G88" s="5"/>
       <c r="H88" s="5"/>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A89" s="6" t="s">
         <v>169</v>
       </c>
@@ -5829,7 +5857,7 @@
       <c r="G89" s="6"/>
       <c r="H89" s="6"/>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A90" s="5" t="s">
         <v>169</v>
       </c>
@@ -5849,7 +5877,7 @@
       <c r="G90" s="5"/>
       <c r="H90" s="5"/>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A91" s="6" t="s">
         <v>169</v>
       </c>
@@ -5869,7 +5897,7 @@
       <c r="G91" s="6"/>
       <c r="H91" s="6"/>
     </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A92" s="5" t="s">
         <v>169</v>
       </c>
@@ -5889,7 +5917,7 @@
       <c r="G92" s="5"/>
       <c r="H92" s="5"/>
     </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A93" s="6" t="s">
         <v>169</v>
       </c>
@@ -5909,7 +5937,7 @@
       <c r="G93" s="6"/>
       <c r="H93" s="6"/>
     </row>
-    <row r="94" spans="1:8" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:8" ht="62.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A94" s="31"/>
       <c r="B94" s="31"/>
       <c r="C94" s="31"/>
@@ -5921,7 +5949,7 @@
       <c r="G94" s="5"/>
       <c r="H94" s="5"/>
     </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A95" s="6" t="s">
         <v>169</v>
       </c>
@@ -5939,7 +5967,7 @@
       <c r="G95" s="5"/>
       <c r="H95" s="5"/>
     </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A96" s="5" t="s">
         <v>169</v>
       </c>
@@ -5959,7 +5987,7 @@
       <c r="G96" s="5"/>
       <c r="H96" s="5"/>
     </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A97" s="6" t="s">
         <v>169</v>
       </c>
@@ -5979,7 +6007,7 @@
       <c r="G97" s="5"/>
       <c r="H97" s="5"/>
     </row>
-    <row r="98" spans="1:8" ht="195" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:8" ht="188.5" x14ac:dyDescent="0.45">
       <c r="A98" s="5" t="s">
         <v>169</v>
       </c>
@@ -5997,7 +6025,7 @@
       <c r="G98" s="5"/>
       <c r="H98" s="5"/>
     </row>
-    <row r="99" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:8" ht="16.5" x14ac:dyDescent="0.45">
       <c r="A99" s="6" t="s">
         <v>169</v>
       </c>
@@ -6015,7 +6043,7 @@
       <c r="G99" s="5"/>
       <c r="H99" s="5"/>
     </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A100" s="5" t="s">
         <v>169</v>
       </c>
@@ -6035,7 +6063,7 @@
       <c r="G100" s="5"/>
       <c r="H100" s="5"/>
     </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A101" s="6" t="s">
         <v>169</v>
       </c>
@@ -6055,7 +6083,7 @@
       <c r="G101" s="5"/>
       <c r="H101" s="5"/>
     </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A102" s="5" t="s">
         <v>169</v>
       </c>
@@ -6075,7 +6103,7 @@
       <c r="G102" s="5"/>
       <c r="H102" s="5"/>
     </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A103" s="6" t="s">
         <v>169</v>
       </c>
@@ -6095,7 +6123,7 @@
       <c r="G103" s="5"/>
       <c r="H103" s="5"/>
     </row>
-    <row r="104" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A104" s="5" t="s">
         <v>169</v>
       </c>
@@ -6115,7 +6143,7 @@
       <c r="G104" s="5"/>
       <c r="H104" s="5"/>
     </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A105" s="6" t="s">
         <v>169</v>
       </c>
@@ -6135,7 +6163,7 @@
       <c r="G105" s="5"/>
       <c r="H105" s="5"/>
     </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A106" s="5" t="s">
         <v>169</v>
       </c>
@@ -6155,7 +6183,7 @@
       <c r="G106" s="5"/>
       <c r="H106" s="5"/>
     </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A107" s="6" t="s">
         <v>169</v>
       </c>
@@ -6175,7 +6203,7 @@
       <c r="G107" s="5"/>
       <c r="H107" s="5"/>
     </row>
-    <row r="108" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A108" s="5" t="s">
         <v>169</v>
       </c>
@@ -6195,7 +6223,7 @@
       <c r="G108" s="5"/>
       <c r="H108" s="5"/>
     </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A109" s="6" t="s">
         <v>169</v>
       </c>
@@ -6215,7 +6243,7 @@
       <c r="G109" s="5"/>
       <c r="H109" s="5"/>
     </row>
-    <row r="110" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A110" s="5" t="s">
         <v>169</v>
       </c>
@@ -6235,7 +6263,7 @@
       <c r="G110" s="5"/>
       <c r="H110" s="5"/>
     </row>
-    <row r="111" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A111" s="6" t="s">
         <v>169</v>
       </c>
@@ -6253,7 +6281,7 @@
       <c r="G111" s="5"/>
       <c r="H111" s="5"/>
     </row>
-    <row r="112" spans="1:8" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:8" ht="50.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A112" s="9"/>
       <c r="B112" s="9"/>
       <c r="C112" s="11" t="s">
@@ -6265,7 +6293,7 @@
       <c r="G112" s="9"/>
       <c r="H112" s="9"/>
     </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A113" s="5" t="s">
         <v>312</v>
       </c>
@@ -6283,7 +6311,7 @@
       <c r="G113" s="5"/>
       <c r="H113" s="5"/>
     </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A114" s="6" t="s">
         <v>312</v>
       </c>
@@ -6301,7 +6329,7 @@
       <c r="G114" s="6"/>
       <c r="H114" s="6"/>
     </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A115" s="5" t="s">
         <v>312</v>
       </c>
@@ -6319,7 +6347,7 @@
       <c r="G115" s="5"/>
       <c r="H115" s="5"/>
     </row>
-    <row r="116" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A116" s="6" t="s">
         <v>312</v>
       </c>
@@ -6339,7 +6367,7 @@
       <c r="G116" s="6"/>
       <c r="H116" s="6"/>
     </row>
-    <row r="117" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A117" s="5" t="s">
         <v>312</v>
       </c>
@@ -6359,7 +6387,7 @@
       <c r="G117" s="5"/>
       <c r="H117" s="5"/>
     </row>
-    <row r="118" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A118" s="6" t="s">
         <v>312</v>
       </c>
@@ -6379,7 +6407,7 @@
       <c r="G118" s="6"/>
       <c r="H118" s="6"/>
     </row>
-    <row r="119" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A119" s="5" t="s">
         <v>312</v>
       </c>
@@ -6399,7 +6427,7 @@
       <c r="G119" s="5"/>
       <c r="H119" s="5"/>
     </row>
-    <row r="120" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A120" s="6" t="s">
         <v>312</v>
       </c>
@@ -6419,7 +6447,7 @@
       <c r="G120" s="6"/>
       <c r="H120" s="6"/>
     </row>
-    <row r="121" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A121" s="5" t="s">
         <v>312</v>
       </c>
@@ -6439,7 +6467,7 @@
       <c r="G121" s="5"/>
       <c r="H121" s="5"/>
     </row>
-    <row r="122" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A122" s="6" t="s">
         <v>312</v>
       </c>
@@ -6457,7 +6485,7 @@
       <c r="G122" s="6"/>
       <c r="H122" s="6"/>
     </row>
-    <row r="123" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A123" s="5" t="s">
         <v>312</v>
       </c>
@@ -6475,7 +6503,7 @@
       <c r="G123" s="5"/>
       <c r="H123" s="5"/>
     </row>
-    <row r="124" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A124" s="6" t="s">
         <v>312</v>
       </c>
@@ -6493,7 +6521,7 @@
       <c r="G124" s="6"/>
       <c r="H124" s="6"/>
     </row>
-    <row r="125" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A125" s="5" t="s">
         <v>312</v>
       </c>
@@ -6511,7 +6539,7 @@
       <c r="G125" s="5"/>
       <c r="H125" s="5"/>
     </row>
-    <row r="126" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A126" s="6" t="s">
         <v>312</v>
       </c>
@@ -6529,7 +6557,7 @@
       <c r="G126" s="6"/>
       <c r="H126" s="6"/>
     </row>
-    <row r="127" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A127" s="5" t="s">
         <v>312</v>
       </c>
@@ -6549,7 +6577,7 @@
       <c r="G127" s="5"/>
       <c r="H127" s="5"/>
     </row>
-    <row r="128" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A128" s="6" t="s">
         <v>312</v>
       </c>
@@ -6567,7 +6595,7 @@
       <c r="G128" s="6"/>
       <c r="H128" s="6"/>
     </row>
-    <row r="129" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A129" s="5" t="s">
         <v>312</v>
       </c>
@@ -6585,7 +6613,7 @@
       <c r="G129" s="5"/>
       <c r="H129" s="5"/>
     </row>
-    <row r="130" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A130" s="6" t="s">
         <v>312</v>
       </c>
@@ -6603,7 +6631,7 @@
       <c r="G130" s="6"/>
       <c r="H130" s="6"/>
     </row>
-    <row r="131" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A131" s="5" t="s">
         <v>312</v>
       </c>
@@ -6623,7 +6651,7 @@
       <c r="G131" s="5"/>
       <c r="H131" s="5"/>
     </row>
-    <row r="132" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A132" s="6" t="s">
         <v>312</v>
       </c>
@@ -6641,7 +6669,7 @@
       <c r="G132" s="6"/>
       <c r="H132" s="6"/>
     </row>
-    <row r="133" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A133" s="5" t="s">
         <v>312</v>
       </c>
@@ -6661,7 +6689,7 @@
       <c r="G133" s="5"/>
       <c r="H133" s="5"/>
     </row>
-    <row r="134" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A134" s="6" t="s">
         <v>312</v>
       </c>
@@ -6679,7 +6707,7 @@
       <c r="G134" s="6"/>
       <c r="H134" s="6"/>
     </row>
-    <row r="135" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A135" s="5" t="s">
         <v>312</v>
       </c>
@@ -6695,7 +6723,7 @@
       <c r="G135" s="5"/>
       <c r="H135" s="5"/>
     </row>
-    <row r="136" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A136" s="6" t="s">
         <v>312</v>
       </c>
@@ -6713,7 +6741,7 @@
       <c r="G136" s="6"/>
       <c r="H136" s="6"/>
     </row>
-    <row r="137" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A137" s="5" t="s">
         <v>312</v>
       </c>
@@ -6731,7 +6759,7 @@
       <c r="G137" s="5"/>
       <c r="H137" s="5"/>
     </row>
-    <row r="138" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A138" s="6" t="s">
         <v>312</v>
       </c>
@@ -6751,7 +6779,7 @@
       <c r="G138" s="6"/>
       <c r="H138" s="6"/>
     </row>
-    <row r="139" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A139" s="5" t="s">
         <v>312</v>
       </c>
@@ -6771,7 +6799,7 @@
       <c r="G139" s="5"/>
       <c r="H139" s="5"/>
     </row>
-    <row r="140" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A140" s="6" t="s">
         <v>312</v>
       </c>
@@ -6791,7 +6819,7 @@
       <c r="G140" s="6"/>
       <c r="H140" s="6"/>
     </row>
-    <row r="141" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A141" s="5" t="s">
         <v>312</v>
       </c>
@@ -6811,7 +6839,7 @@
       <c r="G141" s="5"/>
       <c r="H141" s="5"/>
     </row>
-    <row r="142" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A142" s="6" t="s">
         <v>312</v>
       </c>
@@ -6831,7 +6859,7 @@
       <c r="G142" s="6"/>
       <c r="H142" s="6"/>
     </row>
-    <row r="143" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A143" s="5" t="s">
         <v>312</v>
       </c>
@@ -6851,7 +6879,7 @@
       <c r="G143" s="5"/>
       <c r="H143" s="5"/>
     </row>
-    <row r="144" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A144" s="6" t="s">
         <v>312</v>
       </c>
@@ -6871,7 +6899,7 @@
       <c r="G144" s="6"/>
       <c r="H144" s="6"/>
     </row>
-    <row r="145" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A145" s="5" t="s">
         <v>312</v>
       </c>
@@ -6891,7 +6919,7 @@
       <c r="G145" s="5"/>
       <c r="H145" s="5"/>
     </row>
-    <row r="146" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A146" s="6" t="s">
         <v>312</v>
       </c>
@@ -6911,7 +6939,7 @@
       <c r="G146" s="6"/>
       <c r="H146" s="6"/>
     </row>
-    <row r="147" spans="1:8" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:8" ht="47.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A147" s="9"/>
       <c r="B147" s="9"/>
       <c r="C147" s="10" t="s">
@@ -6923,7 +6951,7 @@
       <c r="G147" s="9"/>
       <c r="H147" s="9"/>
     </row>
-    <row r="148" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A148" s="5" t="s">
         <v>352</v>
       </c>
@@ -6943,7 +6971,7 @@
       <c r="G148" s="5"/>
       <c r="H148" s="5"/>
     </row>
-    <row r="149" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A149" s="6" t="s">
         <v>352</v>
       </c>
@@ -6963,7 +6991,7 @@
       <c r="G149" s="6"/>
       <c r="H149" s="6"/>
     </row>
-    <row r="150" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A150" s="5" t="s">
         <v>352</v>
       </c>
@@ -6983,7 +7011,7 @@
       <c r="G150" s="5"/>
       <c r="H150" s="5"/>
     </row>
-    <row r="151" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A151" s="6" t="s">
         <v>352</v>
       </c>
@@ -7003,7 +7031,7 @@
       <c r="G151" s="6"/>
       <c r="H151" s="6"/>
     </row>
-    <row r="152" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A152" s="5" t="s">
         <v>352</v>
       </c>
@@ -7023,7 +7051,7 @@
       <c r="G152" s="5"/>
       <c r="H152" s="5"/>
     </row>
-    <row r="153" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A153" s="6" t="s">
         <v>352</v>
       </c>
@@ -7043,7 +7071,7 @@
       <c r="G153" s="6"/>
       <c r="H153" s="6"/>
     </row>
-    <row r="154" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A154" s="5" t="s">
         <v>352</v>
       </c>
@@ -7063,7 +7091,7 @@
       <c r="G154" s="5"/>
       <c r="H154" s="5"/>
     </row>
-    <row r="155" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:8" ht="58" x14ac:dyDescent="0.35">
       <c r="A155" s="6" t="s">
         <v>352</v>
       </c>
@@ -7083,7 +7111,7 @@
       <c r="G155" s="6"/>
       <c r="H155" s="6"/>
     </row>
-    <row r="156" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A156" s="5" t="s">
         <v>352</v>
       </c>
@@ -7103,7 +7131,7 @@
       <c r="G156" s="5"/>
       <c r="H156" s="5"/>
     </row>
-    <row r="157" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A157" s="6" t="s">
         <v>352</v>
       </c>
@@ -7123,7 +7151,7 @@
       <c r="G157" s="6"/>
       <c r="H157" s="6"/>
     </row>
-    <row r="158" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A158" s="5" t="s">
         <v>352</v>
       </c>
@@ -7143,7 +7171,7 @@
       <c r="G158" s="5"/>
       <c r="H158" s="5"/>
     </row>
-    <row r="159" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A159" s="6" t="s">
         <v>352</v>
       </c>
@@ -7163,7 +7191,7 @@
       <c r="G159" s="6"/>
       <c r="H159" s="6"/>
     </row>
-    <row r="160" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A160" s="5" t="s">
         <v>352</v>
       </c>
@@ -7183,7 +7211,7 @@
       <c r="G160" s="5"/>
       <c r="H160" s="5"/>
     </row>
-    <row r="161" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A161" s="6" t="s">
         <v>352</v>
       </c>
@@ -7203,7 +7231,7 @@
       <c r="G161" s="6"/>
       <c r="H161" s="6"/>
     </row>
-    <row r="162" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:8" ht="58" x14ac:dyDescent="0.35">
       <c r="A162" s="5" t="s">
         <v>352</v>
       </c>
@@ -7223,7 +7251,7 @@
       <c r="G162" s="5"/>
       <c r="H162" s="5"/>
     </row>
-    <row r="163" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A163" s="6" t="s">
         <v>352</v>
       </c>
@@ -7243,7 +7271,7 @@
       <c r="G163" s="6"/>
       <c r="H163" s="6"/>
     </row>
-    <row r="164" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A164" s="5" t="s">
         <v>352</v>
       </c>
@@ -7263,7 +7291,7 @@
       <c r="G164" s="5"/>
       <c r="H164" s="5"/>
     </row>
-    <row r="165" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A165" s="6" t="s">
         <v>352</v>
       </c>
@@ -7283,7 +7311,7 @@
       <c r="G165" s="6"/>
       <c r="H165" s="6"/>
     </row>
-    <row r="166" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A166" s="14" t="s">
         <v>352</v>
       </c>
@@ -7303,7 +7331,7 @@
       <c r="G166" s="14"/>
       <c r="H166" s="14"/>
     </row>
-    <row r="167" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A167" s="6" t="s">
         <v>352</v>
       </c>
@@ -7323,7 +7351,7 @@
       <c r="G167" s="6"/>
       <c r="H167" s="6"/>
     </row>
-    <row r="168" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A168" s="14" t="s">
         <v>352</v>
       </c>
@@ -7343,7 +7371,7 @@
       <c r="G168" s="14"/>
       <c r="H168" s="14"/>
     </row>
-    <row r="169" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A169" s="6" t="s">
         <v>352</v>
       </c>
@@ -7363,7 +7391,7 @@
       <c r="G169" s="6"/>
       <c r="H169" s="6"/>
     </row>
-    <row r="170" spans="1:8" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:8" ht="48.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A170" s="10"/>
       <c r="B170" s="9"/>
       <c r="C170" s="10" t="s">
@@ -7375,7 +7403,7 @@
       <c r="G170" s="9"/>
       <c r="H170" s="9"/>
     </row>
-    <row r="171" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A171" s="5" t="s">
         <v>407</v>
       </c>
@@ -7393,7 +7421,7 @@
       <c r="G171" s="5"/>
       <c r="H171" s="5"/>
     </row>
-    <row r="172" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A172" s="6" t="s">
         <v>407</v>
       </c>
@@ -7409,7 +7437,7 @@
       <c r="G172" s="6"/>
       <c r="H172" s="6"/>
     </row>
-    <row r="173" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A173" s="5" t="s">
         <v>407</v>
       </c>
@@ -7427,7 +7455,7 @@
       <c r="G173" s="5"/>
       <c r="H173" s="5"/>
     </row>
-    <row r="174" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A174" s="6" t="s">
         <v>407</v>
       </c>
@@ -7447,7 +7475,7 @@
       <c r="G174" s="6"/>
       <c r="H174" s="6"/>
     </row>
-    <row r="175" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A175" s="5" t="s">
         <v>407</v>
       </c>
@@ -7465,7 +7493,7 @@
       <c r="G175" s="5"/>
       <c r="H175" s="5"/>
     </row>
-    <row r="176" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A176" s="6" t="s">
         <v>407</v>
       </c>
@@ -7483,7 +7511,7 @@
       <c r="G176" s="6"/>
       <c r="H176" s="6"/>
     </row>
-    <row r="177" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A177" s="5" t="s">
         <v>420</v>
       </c>
@@ -7501,7 +7529,7 @@
       <c r="G177" s="5"/>
       <c r="H177" s="5"/>
     </row>
-    <row r="178" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A178" s="6" t="s">
         <v>420</v>
       </c>
@@ -7517,7 +7545,7 @@
       <c r="G178" s="6"/>
       <c r="H178" s="6"/>
     </row>
-    <row r="179" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A179" s="5" t="s">
         <v>420</v>
       </c>
@@ -7537,7 +7565,7 @@
       <c r="G179" s="5"/>
       <c r="H179" s="5"/>
     </row>
-    <row r="180" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A180" s="6" t="s">
         <v>420</v>
       </c>
@@ -7555,7 +7583,7 @@
       <c r="G180" s="6"/>
       <c r="H180" s="6"/>
     </row>
-    <row r="181" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A181" s="5" t="s">
         <v>420</v>
       </c>
@@ -7573,7 +7601,7 @@
       <c r="G181" s="5"/>
       <c r="H181" s="5"/>
     </row>
-    <row r="182" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A182" s="6" t="s">
         <v>420</v>
       </c>
@@ -7591,7 +7619,7 @@
       <c r="G182" s="6"/>
       <c r="H182" s="6"/>
     </row>
-    <row r="183" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A183" s="5" t="s">
         <v>425</v>
       </c>
@@ -7609,7 +7637,7 @@
       <c r="G183" s="5"/>
       <c r="H183" s="5"/>
     </row>
-    <row r="184" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A184" s="6" t="s">
         <v>425</v>
       </c>
@@ -7625,7 +7653,7 @@
       <c r="G184" s="6"/>
       <c r="H184" s="6"/>
     </row>
-    <row r="185" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A185" s="5" t="s">
         <v>425</v>
       </c>
@@ -7641,7 +7669,7 @@
       <c r="G185" s="5"/>
       <c r="H185" s="5"/>
     </row>
-    <row r="186" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A186" s="6" t="s">
         <v>425</v>
       </c>
@@ -7659,7 +7687,7 @@
       <c r="G186" s="6"/>
       <c r="H186" s="6"/>
     </row>
-    <row r="187" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A187" s="5" t="s">
         <v>425</v>
       </c>
@@ -7675,7 +7703,7 @@
       <c r="G187" s="5"/>
       <c r="H187" s="5"/>
     </row>
-    <row r="188" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A188" s="6" t="s">
         <v>425</v>
       </c>
@@ -7693,7 +7721,7 @@
       <c r="G188" s="6"/>
       <c r="H188" s="6"/>
     </row>
-    <row r="189" spans="1:8" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:8" ht="55.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A189" s="9"/>
       <c r="B189" s="9"/>
       <c r="C189" s="10" t="s">
@@ -7705,7 +7733,7 @@
       <c r="G189" s="9"/>
       <c r="H189" s="9"/>
     </row>
-    <row r="190" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A190" s="5" t="s">
         <v>429</v>
       </c>
@@ -7725,7 +7753,7 @@
       <c r="G190" s="5"/>
       <c r="H190" s="5"/>
     </row>
-    <row r="191" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A191" s="6" t="s">
         <v>429</v>
       </c>
@@ -7745,7 +7773,7 @@
       <c r="G191" s="6"/>
       <c r="H191" s="6"/>
     </row>
-    <row r="192" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A192" s="5" t="s">
         <v>429</v>
       </c>
@@ -7765,7 +7793,7 @@
       <c r="G192" s="5"/>
       <c r="H192" s="5"/>
     </row>
-    <row r="193" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A193" s="6" t="s">
         <v>429</v>
       </c>
@@ -7785,7 +7813,7 @@
       <c r="G193" s="6"/>
       <c r="H193" s="6"/>
     </row>
-    <row r="194" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A194" s="5" t="s">
         <v>429</v>
       </c>
@@ -7805,7 +7833,7 @@
       <c r="G194" s="5"/>
       <c r="H194" s="5"/>
     </row>
-    <row r="195" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A195" s="6" t="s">
         <v>429</v>
       </c>
@@ -7825,7 +7853,7 @@
       <c r="G195" s="6"/>
       <c r="H195" s="6"/>
     </row>
-    <row r="196" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A196" s="5" t="s">
         <v>429</v>
       </c>
@@ -7845,7 +7873,7 @@
       <c r="G196" s="5"/>
       <c r="H196" s="5"/>
     </row>
-    <row r="197" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A197" s="6" t="s">
         <v>429</v>
       </c>
@@ -7865,7 +7893,7 @@
       <c r="G197" s="6"/>
       <c r="H197" s="6"/>
     </row>
-    <row r="198" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A198" s="5" t="s">
         <v>429</v>
       </c>
@@ -7885,7 +7913,7 @@
       <c r="G198" s="5"/>
       <c r="H198" s="5"/>
     </row>
-    <row r="199" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A199" s="6" t="s">
         <v>429</v>
       </c>
@@ -7905,7 +7933,7 @@
       <c r="G199" s="6"/>
       <c r="H199" s="6"/>
     </row>
-    <row r="200" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A200" s="5" t="s">
         <v>429</v>
       </c>
@@ -7925,7 +7953,7 @@
       <c r="G200" s="5"/>
       <c r="H200" s="5"/>
     </row>
-    <row r="201" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A201" s="6" t="s">
         <v>429</v>
       </c>
@@ -7945,7 +7973,7 @@
       <c r="G201" s="6"/>
       <c r="H201" s="6"/>
     </row>
-    <row r="202" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A202" s="5" t="s">
         <v>429</v>
       </c>
@@ -7965,7 +7993,7 @@
       <c r="G202" s="5"/>
       <c r="H202" s="5"/>
     </row>
-    <row r="203" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A203" s="6" t="s">
         <v>429</v>
       </c>
@@ -7987,7 +8015,7 @@
       <c r="G203" s="6"/>
       <c r="H203" s="6"/>
     </row>
-    <row r="204" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A204" s="5" t="s">
         <v>429</v>
       </c>
@@ -8007,7 +8035,7 @@
       <c r="G204" s="5"/>
       <c r="H204" s="5"/>
     </row>
-    <row r="205" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A205" s="9"/>
       <c r="B205" s="9"/>
       <c r="C205" s="10" t="s">
@@ -8019,7 +8047,7 @@
       <c r="G205" s="9"/>
       <c r="H205" s="9"/>
     </row>
-    <row r="206" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A206" s="5" t="s">
         <v>459</v>
       </c>
@@ -8037,7 +8065,7 @@
       <c r="G206" s="5"/>
       <c r="H206" s="5"/>
     </row>
-    <row r="207" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A207" s="6" t="s">
         <v>459</v>
       </c>
@@ -8055,7 +8083,7 @@
       <c r="G207" s="6"/>
       <c r="H207" s="6"/>
     </row>
-    <row r="208" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A208" s="5" t="s">
         <v>459</v>
       </c>
@@ -8073,7 +8101,7 @@
       <c r="G208" s="5"/>
       <c r="H208" s="5"/>
     </row>
-    <row r="209" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A209" s="6" t="s">
         <v>459</v>
       </c>
@@ -8091,7 +8119,7 @@
       <c r="G209" s="6"/>
       <c r="H209" s="6"/>
     </row>
-    <row r="210" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A210" s="14" t="s">
         <v>459</v>
       </c>
@@ -8109,7 +8137,7 @@
       <c r="G210" s="5"/>
       <c r="H210" s="5"/>
     </row>
-    <row r="211" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A211" s="6" t="s">
         <v>459</v>
       </c>
@@ -8127,7 +8155,7 @@
       <c r="G211" s="6"/>
       <c r="H211" s="6"/>
     </row>
-    <row r="212" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A212" s="14" t="s">
         <v>459</v>
       </c>
@@ -8143,7 +8171,7 @@
       <c r="G212" s="5"/>
       <c r="H212" s="5"/>
     </row>
-    <row r="213" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A213" s="6" t="s">
         <v>459</v>
       </c>
@@ -8161,7 +8189,7 @@
       <c r="G213" s="6"/>
       <c r="H213" s="6"/>
     </row>
-    <row r="214" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A214" s="5" t="s">
         <v>459</v>
       </c>
@@ -8179,7 +8207,7 @@
       <c r="G214" s="5"/>
       <c r="H214" s="5"/>
     </row>
-    <row r="215" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A215" s="6" t="s">
         <v>459</v>
       </c>
@@ -8197,7 +8225,7 @@
       <c r="G215" s="6"/>
       <c r="H215" s="6"/>
     </row>
-    <row r="216" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A216" s="14" t="s">
         <v>459</v>
       </c>
@@ -8215,7 +8243,7 @@
       <c r="G216" s="14"/>
       <c r="H216" s="14"/>
     </row>
-    <row r="217" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A217" s="6" t="s">
         <v>459</v>
       </c>
@@ -8233,7 +8261,7 @@
       <c r="G217" s="6"/>
       <c r="H217" s="6"/>
     </row>
-    <row r="218" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A218" s="14" t="s">
         <v>459</v>
       </c>
@@ -8251,7 +8279,7 @@
       <c r="G218" s="14"/>
       <c r="H218" s="14"/>
     </row>
-    <row r="219" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A219" s="6" t="s">
         <v>459</v>
       </c>
@@ -8269,7 +8297,7 @@
       <c r="G219" s="6"/>
       <c r="H219" s="6"/>
     </row>
-    <row r="220" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A220" s="5" t="s">
         <v>459</v>
       </c>
@@ -8287,7 +8315,7 @@
       <c r="G220" s="5"/>
       <c r="H220" s="5"/>
     </row>
-    <row r="221" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A221" s="6" t="s">
         <v>459</v>
       </c>
@@ -8305,7 +8333,7 @@
       <c r="G221" s="6"/>
       <c r="H221" s="6"/>
     </row>
-    <row r="222" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A222" s="5" t="s">
         <v>459</v>
       </c>
@@ -8321,7 +8349,7 @@
       <c r="G222" s="5"/>
       <c r="H222" s="5"/>
     </row>
-    <row r="223" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A223" s="6" t="s">
         <v>459</v>
       </c>
@@ -8337,7 +8365,7 @@
       <c r="G223" s="6"/>
       <c r="H223" s="6"/>
     </row>
-    <row r="224" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A224" s="5" t="s">
         <v>459</v>
       </c>
@@ -8353,7 +8381,7 @@
       <c r="G224" s="5"/>
       <c r="H224" s="5"/>
     </row>
-    <row r="225" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A225" s="6" t="s">
         <v>459</v>
       </c>
@@ -8369,7 +8397,7 @@
       <c r="G225" s="6"/>
       <c r="H225" s="6"/>
     </row>
-    <row r="226" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A226" s="5" t="s">
         <v>459</v>
       </c>
@@ -8385,7 +8413,7 @@
       <c r="G226" s="5"/>
       <c r="H226" s="5"/>
     </row>
-    <row r="227" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A227" s="6" t="s">
         <v>459</v>
       </c>
@@ -8401,7 +8429,7 @@
       <c r="G227" s="6"/>
       <c r="H227" s="6"/>
     </row>
-    <row r="228" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A228" s="5" t="s">
         <v>459</v>
       </c>
@@ -8417,7 +8445,7 @@
       <c r="G228" s="5"/>
       <c r="H228" s="5"/>
     </row>
-    <row r="229" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A229" s="6" t="s">
         <v>459</v>
       </c>
@@ -8457,17 +8485,17 @@
       <selection pane="bottomLeft" activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="55.5703125" customWidth="1"/>
-    <col min="3" max="3" width="42.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="39.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="48.7109375" customWidth="1"/>
-    <col min="6" max="6" width="50.42578125" customWidth="1"/>
-    <col min="7" max="7" width="46.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="55.54296875" customWidth="1"/>
+    <col min="3" max="3" width="42.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="39.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="48.7265625" customWidth="1"/>
+    <col min="6" max="6" width="50.453125" customWidth="1"/>
+    <col min="7" max="7" width="46.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="77.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="77.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="49" t="s">
         <v>788</v>
       </c>
@@ -8478,7 +8506,7 @@
       <c r="F1" s="49"/>
       <c r="G1" s="49"/>
     </row>
-    <row r="3" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="41" t="s">
         <v>798</v>
       </c>
@@ -8501,7 +8529,7 @@
         <v>683</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" s="36"/>
       <c r="B4" s="36"/>
       <c r="C4" s="37"/>
@@ -8510,7 +8538,7 @@
       <c r="F4" s="36"/>
       <c r="G4" s="36"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" s="39" t="s">
         <v>780</v>
       </c>
@@ -8521,7 +8549,7 @@
       <c r="F5" s="36"/>
       <c r="G5" s="36"/>
     </row>
-    <row r="6" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A6" s="43">
         <v>1</v>
       </c>
@@ -8538,7 +8566,7 @@
       <c r="F6" s="35"/>
       <c r="G6" s="34"/>
     </row>
-    <row r="7" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A7" s="43">
         <v>2</v>
       </c>
@@ -8555,7 +8583,7 @@
       <c r="F7" s="35"/>
       <c r="G7" s="34"/>
     </row>
-    <row r="8" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="58" x14ac:dyDescent="0.35">
       <c r="A8" s="43">
         <v>3</v>
       </c>
@@ -8572,7 +8600,7 @@
       <c r="F8" s="35"/>
       <c r="G8" s="34"/>
     </row>
-    <row r="9" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="58" x14ac:dyDescent="0.35">
       <c r="A9" s="43">
         <v>4</v>
       </c>
@@ -8589,7 +8617,7 @@
       <c r="F9" s="35"/>
       <c r="G9" s="34"/>
     </row>
-    <row r="10" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A10" s="43">
         <v>5</v>
       </c>
@@ -8606,7 +8634,7 @@
       <c r="F10" s="35"/>
       <c r="G10" s="34"/>
     </row>
-    <row r="11" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A11" s="43">
         <v>6</v>
       </c>
@@ -8623,7 +8651,7 @@
       <c r="F11" s="35"/>
       <c r="G11" s="34"/>
     </row>
-    <row r="12" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A12" s="43">
         <v>7</v>
       </c>
@@ -8640,7 +8668,7 @@
       <c r="F12" s="35"/>
       <c r="G12" s="34"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" s="45"/>
       <c r="B13" s="36"/>
       <c r="C13" s="37"/>
@@ -8649,7 +8677,7 @@
       <c r="F13" s="36"/>
       <c r="G13" s="36"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14" s="47" t="s">
         <v>781</v>
       </c>
@@ -8660,7 +8688,7 @@
       <c r="F14" s="36"/>
       <c r="G14" s="36"/>
     </row>
-    <row r="15" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A15" s="43">
         <v>1</v>
       </c>
@@ -8677,7 +8705,7 @@
       <c r="F15" s="35"/>
       <c r="G15" s="34"/>
     </row>
-    <row r="16" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A16" s="43">
         <v>2</v>
       </c>
@@ -8694,7 +8722,7 @@
       <c r="F16" s="35"/>
       <c r="G16" s="34"/>
     </row>
-    <row r="17" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A17" s="43">
         <v>3</v>
       </c>
@@ -8711,7 +8739,7 @@
       <c r="F17" s="35"/>
       <c r="G17" s="34"/>
     </row>
-    <row r="18" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A18" s="43">
         <v>4</v>
       </c>
@@ -8728,7 +8756,7 @@
       <c r="F18" s="35"/>
       <c r="G18" s="34"/>
     </row>
-    <row r="19" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A19" s="43">
         <v>5</v>
       </c>
@@ -8745,7 +8773,7 @@
       <c r="F19" s="40"/>
       <c r="G19" s="34"/>
     </row>
-    <row r="20" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A20" s="43">
         <v>6</v>
       </c>
@@ -8762,7 +8790,7 @@
       <c r="F20" s="35"/>
       <c r="G20" s="34"/>
     </row>
-    <row r="21" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A21" s="43">
         <v>6</v>
       </c>
@@ -8779,7 +8807,7 @@
       <c r="F21" s="35"/>
       <c r="G21" s="34"/>
     </row>
-    <row r="22" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A22" s="43">
         <v>7</v>
       </c>
@@ -8796,7 +8824,7 @@
       <c r="F22" s="40"/>
       <c r="G22" s="34"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A23" s="43">
         <v>8</v>
       </c>
@@ -8813,7 +8841,7 @@
       <c r="F23" s="40"/>
       <c r="G23" s="34"/>
     </row>
-    <row r="24" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A24" s="43">
         <v>9</v>
       </c>
@@ -8830,7 +8858,7 @@
       <c r="F24" s="35"/>
       <c r="G24" s="34"/>
     </row>
-    <row r="25" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" ht="58" x14ac:dyDescent="0.35">
       <c r="A25" s="43">
         <v>10</v>
       </c>
@@ -8847,7 +8875,7 @@
       <c r="F25" s="40"/>
       <c r="G25" s="34"/>
     </row>
-    <row r="26" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A26" s="43">
         <v>11</v>
       </c>
@@ -8864,7 +8892,7 @@
       <c r="F26" s="40"/>
       <c r="G26" s="34"/>
     </row>
-    <row r="27" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A27" s="43">
         <v>12</v>
       </c>
@@ -8881,7 +8909,7 @@
       <c r="F27" s="40"/>
       <c r="G27" s="34"/>
     </row>
-    <row r="28" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A28" s="43">
         <v>13</v>
       </c>
@@ -8898,7 +8926,7 @@
       <c r="F28" s="40"/>
       <c r="G28" s="34"/>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B29" s="36"/>
       <c r="C29" s="37"/>
       <c r="D29" s="36"/>
@@ -8923,16 +8951,16 @@
       <selection activeCell="D103" sqref="A103:XFD103"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="44.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="255.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="173.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="44.26953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="255.7265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="173.54296875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="44" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="26" x14ac:dyDescent="0.35">
       <c r="A1" s="15" t="s">
         <v>507</v>
       </c>
@@ -8949,7 +8977,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="16" t="s">
         <v>507</v>
       </c>
@@ -8966,7 +8994,7 @@
         <v>513</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="19" t="s">
         <v>507</v>
       </c>
@@ -8983,7 +9011,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="16"/>
       <c r="B4" s="17" t="s">
         <v>518</v>
@@ -8998,7 +9026,7 @@
         <v>513</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="19"/>
       <c r="B5" s="20" t="s">
         <v>71</v>
@@ -9013,7 +9041,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="53" t="s">
         <v>507</v>
       </c>
@@ -9030,7 +9058,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="53"/>
       <c r="B7" s="54"/>
       <c r="C7" s="54"/>
@@ -9039,7 +9067,7 @@
       </c>
       <c r="E7" s="55"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" s="53"/>
       <c r="B8" s="54"/>
       <c r="C8" s="54"/>
@@ -9048,7 +9076,7 @@
       </c>
       <c r="E8" s="55"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" s="19" t="s">
         <v>507</v>
       </c>
@@ -9065,7 +9093,7 @@
         <v>531</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" s="53" t="s">
         <v>507</v>
       </c>
@@ -9082,7 +9110,7 @@
         <v>535</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" s="53"/>
       <c r="B11" s="54"/>
       <c r="C11" s="54"/>
@@ -9091,7 +9119,7 @@
       </c>
       <c r="E11" s="55"/>
     </row>
-    <row r="12" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="50" t="s">
         <v>507</v>
       </c>
@@ -9108,7 +9136,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" s="50"/>
       <c r="B13" s="51"/>
       <c r="C13" s="51"/>
@@ -9117,7 +9145,7 @@
       </c>
       <c r="E13" s="52"/>
     </row>
-    <row r="14" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="16" t="s">
         <v>507</v>
       </c>
@@ -9134,7 +9162,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" s="19"/>
       <c r="B15" s="20" t="s">
         <v>544</v>
@@ -9149,7 +9177,7 @@
         <v>547</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" s="16"/>
       <c r="B16" s="17" t="s">
         <v>548</v>
@@ -9164,7 +9192,7 @@
         <v>547</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" s="19"/>
       <c r="B17" s="20" t="s">
         <v>550</v>
@@ -9179,7 +9207,7 @@
         <v>547</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" s="16"/>
       <c r="B18" s="17" t="s">
         <v>552</v>
@@ -9194,7 +9222,7 @@
         <v>547</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" s="19"/>
       <c r="B19" s="20" t="s">
         <v>177</v>
@@ -9209,7 +9237,7 @@
         <v>547</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" s="16"/>
       <c r="B20" s="17" t="s">
         <v>556</v>
@@ -9224,7 +9252,7 @@
         <v>547</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" s="19"/>
       <c r="B21" s="20" t="s">
         <v>558</v>
@@ -9239,7 +9267,7 @@
         <v>547</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" s="16"/>
       <c r="B22" s="17" t="s">
         <v>560</v>
@@ -9254,7 +9282,7 @@
         <v>547</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" s="19"/>
       <c r="B23" s="20" t="s">
         <v>562</v>
@@ -9269,7 +9297,7 @@
         <v>547</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="53"/>
       <c r="B24" s="54" t="s">
         <v>565</v>
@@ -9284,7 +9312,7 @@
         <v>568</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" s="53"/>
       <c r="B25" s="54"/>
       <c r="C25" s="54"/>
@@ -9293,7 +9321,7 @@
       </c>
       <c r="E25" s="55"/>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" s="50"/>
       <c r="B26" s="51" t="s">
         <v>570</v>
@@ -9308,7 +9336,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27" s="50"/>
       <c r="B27" s="51"/>
       <c r="C27" s="51"/>
@@ -9317,7 +9345,7 @@
       </c>
       <c r="E27" s="52"/>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28" s="53"/>
       <c r="B28" s="54" t="s">
         <v>575</v>
@@ -9332,7 +9360,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29" s="53"/>
       <c r="B29" s="54"/>
       <c r="C29" s="54"/>
@@ -9341,7 +9369,7 @@
       </c>
       <c r="E29" s="55"/>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A30" s="50"/>
       <c r="B30" s="51" t="s">
         <v>579</v>
@@ -9356,7 +9384,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A31" s="50"/>
       <c r="B31" s="51"/>
       <c r="C31" s="51"/>
@@ -9365,7 +9393,7 @@
       </c>
       <c r="E31" s="52"/>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A32" s="53"/>
       <c r="B32" s="54" t="s">
         <v>582</v>
@@ -9380,7 +9408,7 @@
         <v>585</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A33" s="53"/>
       <c r="B33" s="54"/>
       <c r="C33" s="54"/>
@@ -9389,7 +9417,7 @@
       </c>
       <c r="E33" s="55"/>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A34" s="50"/>
       <c r="B34" s="51" t="s">
         <v>587</v>
@@ -9404,7 +9432,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A35" s="50"/>
       <c r="B35" s="51"/>
       <c r="C35" s="51"/>
@@ -9413,7 +9441,7 @@
       </c>
       <c r="E35" s="52"/>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A36" s="16"/>
       <c r="B36" s="17" t="s">
         <v>592</v>
@@ -9428,7 +9456,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A37" s="50"/>
       <c r="B37" s="51" t="s">
         <v>594</v>
@@ -9443,7 +9471,7 @@
         <v>597</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A38" s="50"/>
       <c r="B38" s="51"/>
       <c r="C38" s="51"/>
@@ -9452,7 +9480,7 @@
       </c>
       <c r="E38" s="52"/>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A39" s="50"/>
       <c r="B39" s="51"/>
       <c r="C39" s="51"/>
@@ -9461,7 +9489,7 @@
       </c>
       <c r="E39" s="52"/>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A40" s="50"/>
       <c r="B40" s="51"/>
       <c r="C40" s="51"/>
@@ -9470,7 +9498,7 @@
       </c>
       <c r="E40" s="52"/>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A41" s="50"/>
       <c r="B41" s="51"/>
       <c r="C41" s="51"/>
@@ -9479,7 +9507,7 @@
       </c>
       <c r="E41" s="52"/>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A42" s="50"/>
       <c r="B42" s="51"/>
       <c r="C42" s="51"/>
@@ -9488,7 +9516,7 @@
       </c>
       <c r="E42" s="52"/>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A43" s="50"/>
       <c r="B43" s="51"/>
       <c r="C43" s="51"/>
@@ -9497,7 +9525,7 @@
       </c>
       <c r="E43" s="52"/>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A44" s="50"/>
       <c r="B44" s="51"/>
       <c r="C44" s="51"/>
@@ -9506,7 +9534,7 @@
       </c>
       <c r="E44" s="52"/>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A45" s="50"/>
       <c r="B45" s="51"/>
       <c r="C45" s="51"/>
@@ -9515,7 +9543,7 @@
       </c>
       <c r="E45" s="52"/>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A46" s="50"/>
       <c r="B46" s="51"/>
       <c r="C46" s="51"/>
@@ -9524,14 +9552,14 @@
       </c>
       <c r="E46" s="52"/>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A47" s="50"/>
       <c r="B47" s="51"/>
       <c r="C47" s="51"/>
       <c r="D47" s="3"/>
       <c r="E47" s="52"/>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A48" s="50"/>
       <c r="B48" s="51"/>
       <c r="C48" s="51"/>
@@ -9540,7 +9568,7 @@
       </c>
       <c r="E48" s="52"/>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A49" s="50"/>
       <c r="B49" s="51"/>
       <c r="C49" s="51"/>
@@ -9549,7 +9577,7 @@
       </c>
       <c r="E49" s="52"/>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A50" s="50"/>
       <c r="B50" s="51"/>
       <c r="C50" s="51"/>
@@ -9558,7 +9586,7 @@
       </c>
       <c r="E50" s="52"/>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A51" s="50"/>
       <c r="B51" s="51"/>
       <c r="C51" s="51"/>
@@ -9567,7 +9595,7 @@
       </c>
       <c r="E51" s="52"/>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A52" s="50"/>
       <c r="B52" s="51"/>
       <c r="C52" s="51"/>
@@ -9576,7 +9604,7 @@
       </c>
       <c r="E52" s="52"/>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A53" s="50"/>
       <c r="B53" s="51"/>
       <c r="C53" s="51"/>
@@ -9585,7 +9613,7 @@
       </c>
       <c r="E53" s="52"/>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A54" s="50"/>
       <c r="B54" s="51"/>
       <c r="C54" s="51"/>
@@ -9594,7 +9622,7 @@
       </c>
       <c r="E54" s="52"/>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A55" s="50"/>
       <c r="B55" s="51"/>
       <c r="C55" s="51"/>
@@ -9603,7 +9631,7 @@
       </c>
       <c r="E55" s="52"/>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A56" s="50"/>
       <c r="B56" s="51"/>
       <c r="C56" s="51"/>
@@ -9612,14 +9640,14 @@
       </c>
       <c r="E56" s="52"/>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A57" s="50"/>
       <c r="B57" s="51"/>
       <c r="C57" s="51"/>
       <c r="D57" s="3"/>
       <c r="E57" s="52"/>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A58" s="50"/>
       <c r="B58" s="51"/>
       <c r="C58" s="51"/>
@@ -9628,7 +9656,7 @@
       </c>
       <c r="E58" s="52"/>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A59" s="50"/>
       <c r="B59" s="51"/>
       <c r="C59" s="51"/>
@@ -9637,7 +9665,7 @@
       </c>
       <c r="E59" s="52"/>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A60" s="50"/>
       <c r="B60" s="51"/>
       <c r="C60" s="51"/>
@@ -9646,7 +9674,7 @@
       </c>
       <c r="E60" s="52"/>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A61" s="50"/>
       <c r="B61" s="51"/>
       <c r="C61" s="51"/>
@@ -9655,7 +9683,7 @@
       </c>
       <c r="E61" s="52"/>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A62" s="50"/>
       <c r="B62" s="51"/>
       <c r="C62" s="51"/>
@@ -9664,7 +9692,7 @@
       </c>
       <c r="E62" s="52"/>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A63" s="50"/>
       <c r="B63" s="51"/>
       <c r="C63" s="51"/>
@@ -9673,7 +9701,7 @@
       </c>
       <c r="E63" s="52"/>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A64" s="50"/>
       <c r="B64" s="51"/>
       <c r="C64" s="51"/>
@@ -9682,7 +9710,7 @@
       </c>
       <c r="E64" s="52"/>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A65" s="53"/>
       <c r="B65" s="54" t="s">
         <v>240</v>
@@ -9697,14 +9725,14 @@
         <v>547</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A66" s="53"/>
       <c r="B66" s="54"/>
       <c r="C66" s="54"/>
       <c r="D66" s="22"/>
       <c r="E66" s="55"/>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A67" s="53"/>
       <c r="B67" s="54"/>
       <c r="C67" s="54"/>
@@ -9713,7 +9741,7 @@
       </c>
       <c r="E67" s="55"/>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A68" s="53"/>
       <c r="B68" s="54"/>
       <c r="C68" s="54"/>
@@ -9722,7 +9750,7 @@
       </c>
       <c r="E68" s="55"/>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A69" s="53"/>
       <c r="B69" s="54"/>
       <c r="C69" s="54"/>
@@ -9731,7 +9759,7 @@
       </c>
       <c r="E69" s="55"/>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A70" s="53"/>
       <c r="B70" s="54"/>
       <c r="C70" s="54"/>
@@ -9740,7 +9768,7 @@
       </c>
       <c r="E70" s="55"/>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A71" s="53"/>
       <c r="B71" s="54"/>
       <c r="C71" s="54"/>
@@ -9749,7 +9777,7 @@
       </c>
       <c r="E71" s="55"/>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A72" s="53"/>
       <c r="B72" s="54"/>
       <c r="C72" s="54"/>
@@ -9758,7 +9786,7 @@
       </c>
       <c r="E72" s="55"/>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A73" s="53"/>
       <c r="B73" s="54"/>
       <c r="C73" s="54"/>
@@ -9767,7 +9795,7 @@
       </c>
       <c r="E73" s="55"/>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A74" s="53"/>
       <c r="B74" s="54"/>
       <c r="C74" s="54"/>
@@ -9776,7 +9804,7 @@
       </c>
       <c r="E74" s="55"/>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A75" s="53"/>
       <c r="B75" s="54"/>
       <c r="C75" s="54"/>
@@ -9785,7 +9813,7 @@
       </c>
       <c r="E75" s="55"/>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A76" s="53"/>
       <c r="B76" s="54"/>
       <c r="C76" s="54"/>
@@ -9794,7 +9822,7 @@
       </c>
       <c r="E76" s="55"/>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A77" s="53"/>
       <c r="B77" s="54"/>
       <c r="C77" s="54"/>
@@ -9803,7 +9831,7 @@
       </c>
       <c r="E77" s="55"/>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A78" s="53"/>
       <c r="B78" s="54"/>
       <c r="C78" s="54"/>
@@ -9812,7 +9840,7 @@
       </c>
       <c r="E78" s="55"/>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A79" s="53"/>
       <c r="B79" s="54"/>
       <c r="C79" s="54"/>
@@ -9821,7 +9849,7 @@
       </c>
       <c r="E79" s="55"/>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A80" s="50"/>
       <c r="B80" s="51" t="s">
         <v>237</v>
@@ -9836,14 +9864,14 @@
         <v>547</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A81" s="50"/>
       <c r="B81" s="51"/>
       <c r="C81" s="51"/>
       <c r="D81" s="3"/>
       <c r="E81" s="52"/>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A82" s="50"/>
       <c r="B82" s="51"/>
       <c r="C82" s="51"/>
@@ -9852,7 +9880,7 @@
       </c>
       <c r="E82" s="52"/>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A83" s="50"/>
       <c r="B83" s="51"/>
       <c r="C83" s="51"/>
@@ -9861,7 +9889,7 @@
       </c>
       <c r="E83" s="52"/>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A84" s="50"/>
       <c r="B84" s="51"/>
       <c r="C84" s="51"/>
@@ -9870,7 +9898,7 @@
       </c>
       <c r="E84" s="52"/>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A85" s="50"/>
       <c r="B85" s="51"/>
       <c r="C85" s="51"/>
@@ -9879,7 +9907,7 @@
       </c>
       <c r="E85" s="52"/>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A86" s="50"/>
       <c r="B86" s="51"/>
       <c r="C86" s="51"/>
@@ -9888,7 +9916,7 @@
       </c>
       <c r="E86" s="52"/>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A87" s="50"/>
       <c r="B87" s="51"/>
       <c r="C87" s="51"/>
@@ -9897,7 +9925,7 @@
       </c>
       <c r="E87" s="52"/>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A88" s="50"/>
       <c r="B88" s="51"/>
       <c r="C88" s="51"/>
@@ -9906,7 +9934,7 @@
       </c>
       <c r="E88" s="52"/>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A89" s="50"/>
       <c r="B89" s="51"/>
       <c r="C89" s="51"/>
@@ -9915,7 +9943,7 @@
       </c>
       <c r="E89" s="52"/>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A90" s="50"/>
       <c r="B90" s="51"/>
       <c r="C90" s="51"/>
@@ -9924,7 +9952,7 @@
       </c>
       <c r="E90" s="52"/>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A91" s="50"/>
       <c r="B91" s="51"/>
       <c r="C91" s="51"/>
@@ -9933,7 +9961,7 @@
       </c>
       <c r="E91" s="52"/>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A92" s="50"/>
       <c r="B92" s="51"/>
       <c r="C92" s="51"/>
@@ -9942,7 +9970,7 @@
       </c>
       <c r="E92" s="52"/>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A93" s="50"/>
       <c r="B93" s="51"/>
       <c r="C93" s="51"/>
@@ -9951,7 +9979,7 @@
       </c>
       <c r="E93" s="52"/>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A94" s="50"/>
       <c r="B94" s="51"/>
       <c r="C94" s="51"/>
@@ -9960,7 +9988,7 @@
       </c>
       <c r="E94" s="52"/>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A95" s="16"/>
       <c r="B95" s="17" t="s">
         <v>632</v>
@@ -9975,7 +10003,7 @@
         <v>547</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A96" s="19"/>
       <c r="B96" s="20" t="s">
         <v>77</v>
@@ -9990,7 +10018,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A97" s="16"/>
       <c r="B97" s="17" t="s">
         <v>636</v>
@@ -10005,7 +10033,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="98" spans="1:5" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:5" ht="13" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A98" s="50"/>
       <c r="B98" s="51" t="s">
         <v>124</v>
@@ -10020,7 +10048,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A99" s="50"/>
       <c r="B99" s="51"/>
       <c r="C99" s="51"/>
@@ -10029,7 +10057,7 @@
       </c>
       <c r="E99" s="52"/>
     </row>
-    <row r="100" spans="1:5" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:5" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A100" s="53"/>
       <c r="B100" s="54" t="s">
         <v>491</v>
@@ -10044,7 +10072,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A101" s="53"/>
       <c r="B101" s="54"/>
       <c r="C101" s="54"/>
@@ -10053,7 +10081,7 @@
       </c>
       <c r="E101" s="55"/>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A102" s="19"/>
       <c r="B102" s="20" t="s">
         <v>487</v>
@@ -10068,7 +10096,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="103" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:5" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A103" s="53"/>
       <c r="B103" s="54" t="s">
         <v>645</v>
@@ -10083,7 +10111,7 @@
         <v>547</v>
       </c>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A104" s="53"/>
       <c r="B104" s="54"/>
       <c r="C104" s="54"/>
@@ -10092,7 +10120,7 @@
       </c>
       <c r="E104" s="55"/>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A105" s="19"/>
       <c r="B105" s="20" t="s">
         <v>649</v>
@@ -10107,7 +10135,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A106" s="16"/>
       <c r="B106" s="17" t="s">
         <v>651</v>
@@ -10122,7 +10150,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A107" s="19"/>
       <c r="B107" s="20" t="s">
         <v>653</v>
@@ -10137,7 +10165,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A108" s="16"/>
       <c r="B108" s="17" t="s">
         <v>656</v>
@@ -10152,7 +10180,7 @@
         <v>547</v>
       </c>
     </row>
-    <row r="109" spans="1:5" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:5" ht="12.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A109" s="50"/>
       <c r="B109" s="51" t="s">
         <v>658</v>
@@ -10167,7 +10195,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="110" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A110" s="50"/>
       <c r="B110" s="51"/>
       <c r="C110" s="51"/>
@@ -10176,7 +10204,7 @@
       </c>
       <c r="E110" s="52"/>
     </row>
-    <row r="111" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A111" s="23"/>
       <c r="B111" s="24" t="s">
         <v>128</v>
@@ -10191,13 +10219,65 @@
         <v>663</v>
       </c>
     </row>
-    <row r="112" spans="1:5" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="113" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="114" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="115" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="116" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="112" spans="1:5" hidden="1" x14ac:dyDescent="0.35"/>
+    <row r="113" hidden="1" x14ac:dyDescent="0.35"/>
+    <row r="114" hidden="1" x14ac:dyDescent="0.35"/>
+    <row r="115" hidden="1" x14ac:dyDescent="0.35"/>
+    <row r="116" hidden="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <mergeCells count="64">
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="A6:A8"/>
+    <mergeCell ref="B6:B8"/>
+    <mergeCell ref="C6:C8"/>
+    <mergeCell ref="E6:E8"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="A24:A25"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="E24:E25"/>
+    <mergeCell ref="A26:A27"/>
+    <mergeCell ref="B26:B27"/>
+    <mergeCell ref="C26:C27"/>
+    <mergeCell ref="E26:E27"/>
+    <mergeCell ref="A28:A29"/>
+    <mergeCell ref="B28:B29"/>
+    <mergeCell ref="C28:C29"/>
+    <mergeCell ref="E28:E29"/>
+    <mergeCell ref="A30:A31"/>
+    <mergeCell ref="B30:B31"/>
+    <mergeCell ref="C30:C31"/>
+    <mergeCell ref="E30:E31"/>
+    <mergeCell ref="A32:A33"/>
+    <mergeCell ref="B32:B33"/>
+    <mergeCell ref="C32:C33"/>
+    <mergeCell ref="E32:E33"/>
+    <mergeCell ref="A34:A35"/>
+    <mergeCell ref="B34:B35"/>
+    <mergeCell ref="C34:C35"/>
+    <mergeCell ref="E34:E35"/>
+    <mergeCell ref="A37:A64"/>
+    <mergeCell ref="B37:B64"/>
+    <mergeCell ref="C37:C64"/>
+    <mergeCell ref="E37:E64"/>
+    <mergeCell ref="A65:A79"/>
+    <mergeCell ref="B65:B79"/>
+    <mergeCell ref="C65:C79"/>
+    <mergeCell ref="E65:E79"/>
+    <mergeCell ref="A80:A94"/>
+    <mergeCell ref="B80:B94"/>
+    <mergeCell ref="C80:C94"/>
+    <mergeCell ref="E80:E94"/>
+    <mergeCell ref="A98:A99"/>
+    <mergeCell ref="B98:B99"/>
+    <mergeCell ref="C98:C99"/>
+    <mergeCell ref="E98:E99"/>
     <mergeCell ref="A109:A110"/>
     <mergeCell ref="B109:B110"/>
     <mergeCell ref="C109:C110"/>
@@ -10210,106 +10290,12 @@
     <mergeCell ref="B103:B104"/>
     <mergeCell ref="C103:C104"/>
     <mergeCell ref="E103:E104"/>
-    <mergeCell ref="A80:A94"/>
-    <mergeCell ref="B80:B94"/>
-    <mergeCell ref="C80:C94"/>
-    <mergeCell ref="E80:E94"/>
-    <mergeCell ref="A98:A99"/>
-    <mergeCell ref="B98:B99"/>
-    <mergeCell ref="C98:C99"/>
-    <mergeCell ref="E98:E99"/>
-    <mergeCell ref="A37:A64"/>
-    <mergeCell ref="B37:B64"/>
-    <mergeCell ref="C37:C64"/>
-    <mergeCell ref="E37:E64"/>
-    <mergeCell ref="A65:A79"/>
-    <mergeCell ref="B65:B79"/>
-    <mergeCell ref="C65:C79"/>
-    <mergeCell ref="E65:E79"/>
-    <mergeCell ref="A32:A33"/>
-    <mergeCell ref="B32:B33"/>
-    <mergeCell ref="C32:C33"/>
-    <mergeCell ref="E32:E33"/>
-    <mergeCell ref="A34:A35"/>
-    <mergeCell ref="B34:B35"/>
-    <mergeCell ref="C34:C35"/>
-    <mergeCell ref="E34:E35"/>
-    <mergeCell ref="A28:A29"/>
-    <mergeCell ref="B28:B29"/>
-    <mergeCell ref="C28:C29"/>
-    <mergeCell ref="E28:E29"/>
-    <mergeCell ref="A30:A31"/>
-    <mergeCell ref="B30:B31"/>
-    <mergeCell ref="C30:C31"/>
-    <mergeCell ref="E30:E31"/>
-    <mergeCell ref="A24:A25"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="C24:C25"/>
-    <mergeCell ref="E24:E25"/>
-    <mergeCell ref="A26:A27"/>
-    <mergeCell ref="B26:B27"/>
-    <mergeCell ref="C26:C27"/>
-    <mergeCell ref="E26:E27"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="A6:A8"/>
-    <mergeCell ref="B6:B8"/>
-    <mergeCell ref="C6:C8"/>
-    <mergeCell ref="E6:E8"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="E10:E11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="cea7764e-6bf9-427d-be15-e74097e0a61c">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <SharedWithUsers xmlns="fb9ea31f-0ab8-44ff-80d1-5777f6d9d945">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-    <MediaLengthInSeconds xmlns="cea7764e-6bf9-427d-be15-e74097e0a61c" xsi:nil="true"/>
-    <Sign_x002d_off_x0020_status xmlns="cea7764e-6bf9-427d-be15-e74097e0a61c" xsi:nil="true"/>
-    <Title_x0020_URL xmlns="cea7764e-6bf9-427d-be15-e74097e0a61c">
-      <Url xsi:nil="true"/>
-      <Description xsi:nil="true"/>
-    </Title_x0020_URL>
-    <Mail_x0020_Sent xmlns="cea7764e-6bf9-427d-be15-e74097e0a61c">false</Mail_x0020_Sent>
-    <_Flow_SignoffStatus xmlns="cea7764e-6bf9-427d-be15-e74097e0a61c" xsi:nil="true"/>
-    <State xmlns="cea7764e-6bf9-427d-be15-e74097e0a61c">Open</State>
-    <Comments xmlns="cea7764e-6bf9-427d-be15-e74097e0a61c" xsi:nil="true"/>
-    <Lead_x0020_Signoff xmlns="cea7764e-6bf9-427d-be15-e74097e0a61c">false</Lead_x0020_Signoff>
-    <Title_x0020_ID xmlns="cea7764e-6bf9-427d-be15-e74097e0a61c" xsi:nil="true"/>
-    <TranslatedLang xmlns="cea7764e-6bf9-427d-be15-e74097e0a61c" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010039A62E282DDA434E979CD3E03185182E" ma:contentTypeVersion="33" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="a6c69cf93bfe1fca5d0e373365e7fdfc">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="cea7764e-6bf9-427d-be15-e74097e0a61c" xmlns:ns3="fb9ea31f-0ab8-44ff-80d1-5777f6d9d945" xmlns:ns4="230e9df3-be65-4c73-a93b-d1236ebd677e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="62cb4c6faf5eab163d0c8ea23c8ff408" ns1:_="" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -10651,34 +10637,49 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E53D8182-34C2-4EE5-8FD0-D750C3EB0900}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="fb9ea31f-0ab8-44ff-80d1-5777f6d9d945"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
-    <ds:schemaRef ds:uri="cea7764e-6bf9-427d-be15-e74097e0a61c"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3F377113-5718-41B1-A1CE-B96F830D3573}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="cea7764e-6bf9-427d-be15-e74097e0a61c">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <SharedWithUsers xmlns="fb9ea31f-0ab8-44ff-80d1-5777f6d9d945">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+    <MediaLengthInSeconds xmlns="cea7764e-6bf9-427d-be15-e74097e0a61c" xsi:nil="true"/>
+    <Sign_x002d_off_x0020_status xmlns="cea7764e-6bf9-427d-be15-e74097e0a61c" xsi:nil="true"/>
+    <Title_x0020_URL xmlns="cea7764e-6bf9-427d-be15-e74097e0a61c">
+      <Url xsi:nil="true"/>
+      <Description xsi:nil="true"/>
+    </Title_x0020_URL>
+    <Mail_x0020_Sent xmlns="cea7764e-6bf9-427d-be15-e74097e0a61c">false</Mail_x0020_Sent>
+    <_Flow_SignoffStatus xmlns="cea7764e-6bf9-427d-be15-e74097e0a61c" xsi:nil="true"/>
+    <State xmlns="cea7764e-6bf9-427d-be15-e74097e0a61c">Open</State>
+    <Comments xmlns="cea7764e-6bf9-427d-be15-e74097e0a61c" xsi:nil="true"/>
+    <Lead_x0020_Signoff xmlns="cea7764e-6bf9-427d-be15-e74097e0a61c">false</Lead_x0020_Signoff>
+    <Title_x0020_ID xmlns="cea7764e-6bf9-427d-be15-e74097e0a61c" xsi:nil="true"/>
+    <TranslatedLang xmlns="cea7764e-6bf9-427d-be15-e74097e0a61c" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{23B9621B-458A-4676-8042-F53348150B3A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -10699,6 +10700,33 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3F377113-5718-41B1-A1CE-B96F830D3573}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E53D8182-34C2-4EE5-8FD0-D750C3EB0900}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="fb9ea31f-0ab8-44ff-80d1-5777f6d9d945"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
+    <ds:schemaRef ds:uri="cea7764e-6bf9-427d-be15-e74097e0a61c"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{87867195-f2b8-4ac2-b0b6-6bb73cb33afc}" enabled="1" method="Privileged" siteId="{72f988bf-86f1-41af-91ab-2d7cd011db47}" contentBits="0" removed="0"/>

</xml_diff>

<commit_message>
feat: security management group (#140)
* feat: security management group

* Update docs/content/accelerator/userguide/2_start/terraform-azuredevops.md

Co-authored-by: Matt White <16320656+matt-FFFFFF@users.noreply.github.com>

* Update docs/content/accelerator/userguide/2_start/terraform-github.md

Co-authored-by: Matt White <16320656+matt-FFFFFF@users.noreply.github.com>

* Update docs/content/accelerator/userguide/2_start/terraform-local.md

Co-authored-by: Matt White <16320656+matt-FFFFFF@users.noreply.github.com>

* improve release notes

---------

Co-authored-by: Matt White <16320656+matt-FFFFFF@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/docs/static/examples/tf/accelerator/config/checklist.xlsx
+++ b/docs/static/examples/tf/accelerator/config/checklist.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\Azure-Landing-Zones\docs\static\examples\tf\accelerator\config\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jaredholgate\Code\azure-landing-zones\docs\static\examples\tf\accelerator\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AAF9BDE-F5B8-4497-AF3D-23E3B3919670}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29446722-CE5D-4CA6-97DF-6F4B77F3077C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" tabRatio="415" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" tabRatio="415" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Accelerator - Bootstrap" sheetId="13" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1408" uniqueCount="805">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1412" uniqueCount="807">
   <si>
     <t>Description</t>
   </si>
@@ -2589,6 +2589,12 @@
   </si>
   <si>
     <t>"mgmt"</t>
+  </si>
+  <si>
+    <t>Security subscription id</t>
+  </si>
+  <si>
+    <t>The subscription id for the security subscription</t>
   </si>
 </sst>
 </file>
@@ -2881,7 +2887,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -3043,6 +3049,9 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3399,24 +3408,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D33EA6D-E1B5-4751-908D-ADA676A42D17}">
-  <dimension ref="A1:G45"/>
+  <dimension ref="A1:G46"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="7.85546875" style="42" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="42.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="39.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.81640625" style="42" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="42.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="39.81640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="38" customWidth="1"/>
-    <col min="5" max="5" width="50.42578125" customWidth="1"/>
-    <col min="6" max="7" width="46.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="50.453125" customWidth="1"/>
+    <col min="6" max="7" width="46.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="77.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="77.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="48" t="s">
         <v>787</v>
       </c>
@@ -3427,7 +3436,7 @@
       <c r="F1" s="48"/>
       <c r="G1" s="48"/>
     </row>
-    <row r="3" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="44" t="s">
         <v>790</v>
       </c>
@@ -3450,7 +3459,7 @@
         <v>683</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A4" s="43">
         <v>1</v>
       </c>
@@ -3469,7 +3478,7 @@
       <c r="F4" s="38"/>
       <c r="G4" s="34"/>
     </row>
-    <row r="5" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A5" s="43">
         <v>2</v>
       </c>
@@ -3488,7 +3497,7 @@
       <c r="F5" s="35"/>
       <c r="G5" s="34"/>
     </row>
-    <row r="6" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="87" x14ac:dyDescent="0.35">
       <c r="A6" s="43">
         <v>3</v>
       </c>
@@ -3507,7 +3516,7 @@
       <c r="F6" s="35"/>
       <c r="G6" s="34"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" s="45"/>
       <c r="B7" s="36"/>
       <c r="C7" s="37"/>
@@ -3516,7 +3525,7 @@
       <c r="F7" s="36"/>
       <c r="G7" s="36"/>
     </row>
-    <row r="8" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" s="43">
         <v>4</v>
       </c>
@@ -3537,7 +3546,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A9" s="43">
         <v>5</v>
       </c>
@@ -3558,7 +3567,7 @@
         <v>684</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A10" s="43">
         <v>6</v>
       </c>
@@ -3579,7 +3588,7 @@
       </c>
       <c r="G10" s="34"/>
     </row>
-    <row r="11" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A11" s="43">
         <v>7</v>
       </c>
@@ -3598,7 +3607,7 @@
       <c r="F11" s="35"/>
       <c r="G11" s="34"/>
     </row>
-    <row r="12" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A12" s="43">
         <v>7</v>
       </c>
@@ -3617,7 +3626,7 @@
       <c r="F12" s="35"/>
       <c r="G12" s="34"/>
     </row>
-    <row r="13" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A13" s="43">
         <v>7</v>
       </c>
@@ -3636,152 +3645,150 @@
       <c r="F13" s="35"/>
       <c r="G13" s="34"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="45"/>
-      <c r="B14" s="36"/>
-      <c r="C14" s="37"/>
-      <c r="D14" s="36"/>
-      <c r="E14" s="37"/>
-      <c r="F14" s="36"/>
-      <c r="G14" s="36"/>
-    </row>
-    <row r="15" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="43">
+    <row r="14" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A14" s="43">
+        <v>7</v>
+      </c>
+      <c r="B14" s="34" t="s">
+        <v>805</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>806</v>
+      </c>
+      <c r="D14" s="34" t="s">
+        <v>504</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>688</v>
+      </c>
+      <c r="F14" s="56"/>
+      <c r="G14" s="34"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A15" s="45"/>
+      <c r="B15" s="36"/>
+      <c r="C15" s="37"/>
+      <c r="D15" s="36"/>
+      <c r="E15" s="37"/>
+      <c r="F15" s="36"/>
+      <c r="G15" s="36"/>
+    </row>
+    <row r="16" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A16" s="43">
         <v>8</v>
       </c>
-      <c r="B15" s="34" t="s">
+      <c r="B16" s="34" t="s">
         <v>695</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="C16" s="1" t="s">
         <v>696</v>
       </c>
-      <c r="D15" s="34" t="s">
+      <c r="D16" s="34" t="s">
         <v>46</v>
       </c>
-      <c r="E15" s="1" t="s">
+      <c r="E16" s="1" t="s">
         <v>697</v>
       </c>
-      <c r="F15" s="40" t="s">
+      <c r="F16" s="40" t="s">
         <v>44</v>
       </c>
-      <c r="G15" s="34"/>
-    </row>
-    <row r="16" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="43">
-        <v>9</v>
-      </c>
-      <c r="B16" s="34" t="s">
-        <v>698</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>699</v>
-      </c>
-      <c r="D16" s="34" t="s">
-        <v>47</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>700</v>
-      </c>
-      <c r="F16" s="35" t="s">
-        <v>16</v>
-      </c>
       <c r="G16" s="34"/>
     </row>
-    <row r="17" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A17" s="43">
         <v>9</v>
       </c>
       <c r="B17" s="34" t="s">
-        <v>803</v>
+        <v>698</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>701</v>
+        <v>699</v>
       </c>
       <c r="D17" s="34" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>700</v>
       </c>
       <c r="F17" s="35" t="s">
-        <v>804</v>
+        <v>16</v>
       </c>
       <c r="G17" s="34"/>
     </row>
-    <row r="18" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A18" s="43">
         <v>9</v>
       </c>
       <c r="B18" s="34" t="s">
+        <v>803</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>701</v>
+      </c>
+      <c r="D18" s="34" t="s">
+        <v>49</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>700</v>
+      </c>
+      <c r="F18" s="35" t="s">
+        <v>804</v>
+      </c>
+      <c r="G18" s="34"/>
+    </row>
+    <row r="19" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A19" s="43">
+        <v>9</v>
+      </c>
+      <c r="B19" s="34" t="s">
         <v>703</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="C19" s="1" t="s">
         <v>704</v>
       </c>
-      <c r="D18" s="34" t="s">
+      <c r="D19" s="34" t="s">
         <v>50</v>
       </c>
-      <c r="E18" s="1" t="s">
+      <c r="E19" s="1" t="s">
         <v>702</v>
       </c>
-      <c r="F18" s="35">
+      <c r="F19" s="35">
         <v>1</v>
       </c>
-      <c r="G18" s="34"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="45"/>
-      <c r="B19" s="36"/>
-      <c r="C19" s="37"/>
-      <c r="D19" s="36"/>
-      <c r="E19" s="37"/>
-      <c r="F19" s="36"/>
-      <c r="G19" s="36"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="46"/>
-      <c r="B20" s="39" t="s">
-        <v>717</v>
-      </c>
+      <c r="G19" s="34"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A20" s="45"/>
+      <c r="B20" s="36"/>
       <c r="C20" s="37"/>
       <c r="D20" s="36"/>
       <c r="E20" s="37"/>
       <c r="F20" s="36"/>
       <c r="G20" s="36"/>
     </row>
-    <row r="21" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A21" s="43">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A21" s="46"/>
+      <c r="B21" s="39" t="s">
+        <v>717</v>
+      </c>
+      <c r="C21" s="37"/>
+      <c r="D21" s="36"/>
+      <c r="E21" s="37"/>
+      <c r="F21" s="36"/>
+      <c r="G21" s="36"/>
+    </row>
+    <row r="22" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A22" s="43">
         <v>11</v>
       </c>
-      <c r="B21" s="34" t="s">
+      <c r="B22" s="34" t="s">
         <v>719</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="C22" s="1" t="s">
         <v>720</v>
       </c>
-      <c r="D21" s="34" t="s">
+      <c r="D22" s="34" t="s">
         <v>45</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>711</v>
-      </c>
-      <c r="F21" s="40" t="s">
-        <v>123</v>
-      </c>
-      <c r="G21" s="34"/>
-    </row>
-    <row r="22" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A22" s="43">
-        <v>10</v>
-      </c>
-      <c r="B22" s="34" t="s">
-        <v>721</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>723</v>
-      </c>
-      <c r="D22" s="34" t="s">
-        <v>53</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>711</v>
@@ -3791,380 +3798,380 @@
       </c>
       <c r="G22" s="34"/>
     </row>
-    <row r="23" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A23" s="43"/>
+    <row r="23" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A23" s="43">
+        <v>10</v>
+      </c>
       <c r="B23" s="34" t="s">
-        <v>724</v>
+        <v>721</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>725</v>
+        <v>723</v>
       </c>
       <c r="D23" s="34" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E23" s="1" t="s">
         <v>711</v>
       </c>
       <c r="F23" s="40" t="s">
+        <v>123</v>
+      </c>
+      <c r="G23" s="34"/>
+    </row>
+    <row r="24" spans="1:7" ht="58" x14ac:dyDescent="0.35">
+      <c r="A24" s="43"/>
+      <c r="B24" s="34" t="s">
+        <v>724</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>725</v>
+      </c>
+      <c r="D24" s="34" t="s">
+        <v>54</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>711</v>
+      </c>
+      <c r="F24" s="40" t="s">
         <v>133</v>
       </c>
-      <c r="G23" s="34"/>
-    </row>
-    <row r="24" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A24" s="43">
-        <v>11</v>
-      </c>
-      <c r="B24" s="34" t="s">
-        <v>726</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>727</v>
-      </c>
-      <c r="D24" s="34" t="s">
-        <v>55</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>728</v>
-      </c>
-      <c r="F24" s="35"/>
-      <c r="G24" s="34" t="s">
-        <v>729</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="G24" s="34"/>
+    </row>
+    <row r="25" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A25" s="43">
         <v>11</v>
       </c>
       <c r="B25" s="34" t="s">
+        <v>726</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>727</v>
+      </c>
+      <c r="D25" s="34" t="s">
+        <v>55</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>728</v>
+      </c>
+      <c r="F25" s="35"/>
+      <c r="G25" s="34" t="s">
+        <v>729</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A26" s="43">
+        <v>11</v>
+      </c>
+      <c r="B26" s="34" t="s">
         <v>722</v>
       </c>
-      <c r="C25" s="1" t="s">
+      <c r="C26" s="1" t="s">
         <v>730</v>
       </c>
-      <c r="D25" s="34" t="s">
+      <c r="D26" s="34" t="s">
         <v>56</v>
       </c>
-      <c r="E25" s="1" t="s">
+      <c r="E26" s="1" t="s">
         <v>711</v>
       </c>
-      <c r="F25" s="40" t="s">
+      <c r="F26" s="40" t="s">
         <v>123</v>
       </c>
-      <c r="G25" s="34"/>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="45"/>
-      <c r="B26" s="36"/>
-      <c r="C26" s="37"/>
-      <c r="D26" s="36"/>
-      <c r="E26" s="37"/>
-      <c r="F26" s="36"/>
-      <c r="G26" s="36"/>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="46"/>
-      <c r="B27" s="39" t="s">
-        <v>716</v>
-      </c>
+      <c r="G26" s="34"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A27" s="45"/>
+      <c r="B27" s="36"/>
       <c r="C27" s="37"/>
       <c r="D27" s="36"/>
       <c r="E27" s="37"/>
       <c r="F27" s="36"/>
       <c r="G27" s="36"/>
     </row>
-    <row r="28" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A28" s="43">
-        <v>11</v>
-      </c>
-      <c r="B28" s="34" t="s">
-        <v>731</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>738</v>
-      </c>
-      <c r="D28" s="34" t="s">
-        <v>57</v>
-      </c>
-      <c r="E28" s="1"/>
-      <c r="F28" s="35"/>
-      <c r="G28" s="34"/>
-    </row>
-    <row r="29" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A28" s="46"/>
+      <c r="B28" s="39" t="s">
+        <v>716</v>
+      </c>
+      <c r="C28" s="37"/>
+      <c r="D28" s="36"/>
+      <c r="E28" s="37"/>
+      <c r="F28" s="36"/>
+      <c r="G28" s="36"/>
+    </row>
+    <row r="29" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A29" s="43">
         <v>11</v>
       </c>
       <c r="B29" s="34" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>737</v>
+        <v>738</v>
       </c>
       <c r="D29" s="34" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E29" s="1"/>
       <c r="F29" s="35"/>
       <c r="G29" s="34"/>
     </row>
-    <row r="30" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A30" s="43">
         <v>11</v>
       </c>
       <c r="B30" s="34" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>736</v>
+        <v>737</v>
       </c>
       <c r="D30" s="34" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E30" s="1"/>
       <c r="F30" s="35"/>
       <c r="G30" s="34"/>
     </row>
-    <row r="31" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A31" s="43">
         <v>11</v>
       </c>
       <c r="B31" s="34" t="s">
-        <v>735</v>
+        <v>733</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>739</v>
+        <v>736</v>
       </c>
       <c r="D31" s="34" t="s">
-        <v>60</v>
-      </c>
-      <c r="E31" s="1" t="s">
-        <v>711</v>
-      </c>
-      <c r="F31" s="40" t="s">
-        <v>133</v>
-      </c>
+        <v>59</v>
+      </c>
+      <c r="E31" s="1"/>
+      <c r="F31" s="35"/>
       <c r="G31" s="34"/>
     </row>
-    <row r="32" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A32" s="43">
         <v>11</v>
       </c>
       <c r="B32" s="34" t="s">
-        <v>740</v>
+        <v>735</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>741</v>
+        <v>739</v>
       </c>
       <c r="D32" s="34" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E32" s="1" t="s">
         <v>711</v>
       </c>
       <c r="F32" s="40" t="s">
-        <v>123</v>
+        <v>133</v>
       </c>
       <c r="G32" s="34"/>
     </row>
-    <row r="33" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" ht="58" x14ac:dyDescent="0.35">
       <c r="A33" s="43">
         <v>11</v>
       </c>
       <c r="B33" s="34" t="s">
+        <v>740</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>741</v>
+      </c>
+      <c r="D33" s="34" t="s">
+        <v>61</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>711</v>
+      </c>
+      <c r="F33" s="40" t="s">
+        <v>123</v>
+      </c>
+      <c r="G33" s="34"/>
+    </row>
+    <row r="34" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A34" s="43">
+        <v>11</v>
+      </c>
+      <c r="B34" s="34" t="s">
         <v>734</v>
       </c>
-      <c r="C33" s="1" t="s">
+      <c r="C34" s="1" t="s">
         <v>742</v>
       </c>
-      <c r="D33" s="34" t="s">
+      <c r="D34" s="34" t="s">
         <v>62</v>
       </c>
-      <c r="E33" s="1"/>
-      <c r="F33" s="35"/>
-      <c r="G33" s="34"/>
-    </row>
-    <row r="34" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A34" s="43">
+      <c r="E34" s="1"/>
+      <c r="F34" s="35"/>
+      <c r="G34" s="34"/>
+    </row>
+    <row r="35" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A35" s="43">
         <v>10</v>
       </c>
-      <c r="B34" s="34" t="s">
+      <c r="B35" s="34" t="s">
         <v>743</v>
       </c>
-      <c r="C34" s="1" t="s">
+      <c r="C35" s="1" t="s">
         <v>744</v>
       </c>
-      <c r="D34" s="34" t="s">
+      <c r="D35" s="34" t="s">
         <v>52</v>
       </c>
-      <c r="E34" s="1"/>
-      <c r="F34" s="40" t="s">
+      <c r="E35" s="1"/>
+      <c r="F35" s="40" t="s">
         <v>123</v>
       </c>
-      <c r="G34" s="34"/>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" s="45"/>
-      <c r="B35" s="36"/>
-      <c r="C35" s="37"/>
-      <c r="D35" s="36"/>
-      <c r="E35" s="37"/>
-      <c r="F35" s="36"/>
-      <c r="G35" s="36"/>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" s="46"/>
-      <c r="B36" s="39" t="s">
-        <v>718</v>
-      </c>
+      <c r="G35" s="34"/>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A36" s="45"/>
+      <c r="B36" s="36"/>
       <c r="C36" s="37"/>
       <c r="D36" s="36"/>
       <c r="E36" s="37"/>
       <c r="F36" s="36"/>
       <c r="G36" s="36"/>
     </row>
-    <row r="37" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A37" s="43">
-        <v>11</v>
-      </c>
-      <c r="B37" s="34" t="s">
-        <v>752</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>750</v>
-      </c>
-      <c r="D37" s="34" t="s">
-        <v>63</v>
-      </c>
-      <c r="E37" s="1"/>
-      <c r="F37" s="35"/>
-      <c r="G37" s="34"/>
-    </row>
-    <row r="38" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A37" s="46"/>
+      <c r="B37" s="39" t="s">
+        <v>718</v>
+      </c>
+      <c r="C37" s="37"/>
+      <c r="D37" s="36"/>
+      <c r="E37" s="37"/>
+      <c r="F37" s="36"/>
+      <c r="G37" s="36"/>
+    </row>
+    <row r="38" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A38" s="43">
         <v>11</v>
       </c>
       <c r="B38" s="34" t="s">
-        <v>751</v>
+        <v>752</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>749</v>
+        <v>750</v>
       </c>
       <c r="D38" s="34" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E38" s="1"/>
       <c r="F38" s="35"/>
       <c r="G38" s="34"/>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A39" s="43">
         <v>11</v>
       </c>
       <c r="B39" s="34" t="s">
-        <v>747</v>
+        <v>751</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>748</v>
+        <v>749</v>
       </c>
       <c r="D39" s="34" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E39" s="1"/>
       <c r="F39" s="35"/>
       <c r="G39" s="34"/>
     </row>
-    <row r="40" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A40" s="43">
+        <v>11</v>
+      </c>
+      <c r="B40" s="34" t="s">
+        <v>747</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>748</v>
+      </c>
+      <c r="D40" s="34" t="s">
+        <v>65</v>
+      </c>
+      <c r="E40" s="1"/>
+      <c r="F40" s="35"/>
+      <c r="G40" s="34"/>
+    </row>
+    <row r="41" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A41" s="43">
         <v>10</v>
       </c>
-      <c r="B40" s="34" t="s">
+      <c r="B41" s="34" t="s">
         <v>745</v>
       </c>
-      <c r="C40" s="1" t="s">
+      <c r="C41" s="1" t="s">
         <v>746</v>
       </c>
-      <c r="D40" s="34" t="s">
+      <c r="D41" s="34" t="s">
         <v>506</v>
       </c>
-      <c r="E40" s="1"/>
-      <c r="F40" s="40" t="s">
+      <c r="E41" s="1"/>
+      <c r="F41" s="40" t="s">
         <v>123</v>
       </c>
-      <c r="G40" s="34"/>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41" s="45"/>
-      <c r="B41" s="36"/>
-      <c r="C41" s="37"/>
-      <c r="D41" s="36"/>
-      <c r="E41" s="37"/>
-      <c r="F41" s="36"/>
-      <c r="G41" s="36"/>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A42" s="46"/>
-      <c r="B42" s="39" t="s">
-        <v>705</v>
-      </c>
+      <c r="G41" s="34"/>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A42" s="45"/>
+      <c r="B42" s="36"/>
       <c r="C42" s="37"/>
       <c r="D42" s="36"/>
       <c r="E42" s="37"/>
       <c r="F42" s="36"/>
       <c r="G42" s="36"/>
     </row>
-    <row r="43" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A43" s="43">
-        <v>11</v>
-      </c>
-      <c r="B43" s="34" t="s">
-        <v>706</v>
-      </c>
-      <c r="C43" s="1" t="s">
-        <v>707</v>
-      </c>
-      <c r="D43" s="34" t="s">
-        <v>66</v>
-      </c>
-      <c r="E43" s="1" t="s">
-        <v>708</v>
-      </c>
-      <c r="F43" s="40" t="s">
-        <v>44</v>
-      </c>
-      <c r="G43" s="34"/>
-    </row>
-    <row r="44" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A43" s="46"/>
+      <c r="B43" s="39" t="s">
+        <v>705</v>
+      </c>
+      <c r="C43" s="37"/>
+      <c r="D43" s="36"/>
+      <c r="E43" s="37"/>
+      <c r="F43" s="36"/>
+      <c r="G43" s="36"/>
+    </row>
+    <row r="44" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A44" s="43">
         <v>11</v>
       </c>
       <c r="B44" s="34" t="s">
-        <v>709</v>
+        <v>706</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>710</v>
+        <v>707</v>
       </c>
       <c r="D44" s="34" t="s">
-        <v>712</v>
+        <v>66</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>711</v>
+        <v>708</v>
       </c>
       <c r="F44" s="40" t="s">
-        <v>123</v>
+        <v>44</v>
       </c>
       <c r="G44" s="34"/>
     </row>
-    <row r="45" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A45" s="43">
         <v>11</v>
       </c>
       <c r="B45" s="34" t="s">
-        <v>713</v>
+        <v>709</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>715</v>
+        <v>710</v>
       </c>
       <c r="D45" s="34" t="s">
-        <v>714</v>
+        <v>712</v>
       </c>
       <c r="E45" s="1" t="s">
         <v>711</v>
@@ -4173,6 +4180,27 @@
         <v>123</v>
       </c>
       <c r="G45" s="34"/>
+    </row>
+    <row r="46" spans="1:7" ht="58" x14ac:dyDescent="0.35">
+      <c r="A46" s="43">
+        <v>11</v>
+      </c>
+      <c r="B46" s="34" t="s">
+        <v>713</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>715</v>
+      </c>
+      <c r="D46" s="34" t="s">
+        <v>714</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>711</v>
+      </c>
+      <c r="F46" s="40" t="s">
+        <v>123</v>
+      </c>
+      <c r="G46" s="34"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -4187,25 +4215,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA5559C7-55D7-4845-9950-8EEEDB97C0FA}">
   <dimension ref="A1:H229"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A35" sqref="A35:XFD35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="41.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="47.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="74.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="93.85546875" style="4" customWidth="1"/>
-    <col min="5" max="5" width="38.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="41.1796875" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="47.81640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="74.26953125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="93.81640625" style="4" customWidth="1"/>
+    <col min="5" max="5" width="38.26953125" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="34" style="2" customWidth="1"/>
-    <col min="7" max="7" width="18.28515625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="18.26953125" style="2" customWidth="1"/>
     <col min="8" max="8" width="21" style="2" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="2"/>
+    <col min="9" max="16384" width="9.1796875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="52.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="26" x14ac:dyDescent="0.35">
       <c r="A1" s="12" t="s">
         <v>7</v>
       </c>
@@ -4231,7 +4259,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="43.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="9"/>
       <c r="B2" s="9"/>
       <c r="C2" s="10" t="s">
@@ -4243,7 +4271,7 @@
       <c r="G2" s="9"/>
       <c r="H2" s="9"/>
     </row>
-    <row r="3" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
         <v>13</v>
       </c>
@@ -4263,7 +4291,7 @@
       <c r="G3" s="5"/>
       <c r="H3" s="5"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="s">
         <v>13</v>
       </c>
@@ -4281,7 +4309,7 @@
       <c r="G4" s="5"/>
       <c r="H4" s="5"/>
     </row>
-    <row r="5" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
         <v>13</v>
       </c>
@@ -4301,7 +4329,7 @@
       <c r="G5" s="5"/>
       <c r="H5" s="5"/>
     </row>
-    <row r="6" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="s">
         <v>13</v>
       </c>
@@ -4319,7 +4347,7 @@
       <c r="G6" s="5"/>
       <c r="H6" s="5"/>
     </row>
-    <row r="7" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A7" s="5" t="s">
         <v>13</v>
       </c>
@@ -4337,7 +4365,7 @@
       <c r="G7" s="5"/>
       <c r="H7" s="5"/>
     </row>
-    <row r="8" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A8" s="5" t="s">
         <v>13</v>
       </c>
@@ -4355,7 +4383,7 @@
       <c r="G8" s="5"/>
       <c r="H8" s="5"/>
     </row>
-    <row r="9" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A9" s="5" t="s">
         <v>13</v>
       </c>
@@ -4375,7 +4403,7 @@
       <c r="G9" s="5"/>
       <c r="H9" s="5"/>
     </row>
-    <row r="10" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A10" s="5" t="s">
         <v>13</v>
       </c>
@@ -4395,7 +4423,7 @@
       <c r="G10" s="5"/>
       <c r="H10" s="5"/>
     </row>
-    <row r="11" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" s="5" t="s">
         <v>13</v>
       </c>
@@ -4413,7 +4441,7 @@
       <c r="G11" s="5"/>
       <c r="H11" s="5"/>
     </row>
-    <row r="12" spans="1:8" ht="51" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" ht="51" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="9"/>
       <c r="B12" s="7"/>
       <c r="C12" s="10" t="s">
@@ -4425,7 +4453,7 @@
       <c r="G12" s="8"/>
       <c r="H12" s="8"/>
     </row>
-    <row r="13" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A13" s="5" t="s">
         <v>67</v>
       </c>
@@ -4443,7 +4471,7 @@
       <c r="G13" s="5"/>
       <c r="H13" s="5"/>
     </row>
-    <row r="14" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A14" s="6" t="s">
         <v>67</v>
       </c>
@@ -4461,7 +4489,7 @@
       <c r="G14" s="6"/>
       <c r="H14" s="6"/>
     </row>
-    <row r="15" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A15" s="5" t="s">
         <v>67</v>
       </c>
@@ -4479,7 +4507,7 @@
       <c r="G15" s="5"/>
       <c r="H15" s="5"/>
     </row>
-    <row r="16" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A16" s="6" t="s">
         <v>67</v>
       </c>
@@ -4497,7 +4525,7 @@
       <c r="G16" s="6"/>
       <c r="H16" s="6"/>
     </row>
-    <row r="17" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A17" s="5" t="s">
         <v>67</v>
       </c>
@@ -4515,7 +4543,7 @@
       <c r="G17" s="5"/>
       <c r="H17" s="5"/>
     </row>
-    <row r="18" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A18" s="5" t="s">
         <v>67</v>
       </c>
@@ -4533,7 +4561,7 @@
       <c r="G18" s="6"/>
       <c r="H18" s="6"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A19" s="14" t="s">
         <v>67</v>
       </c>
@@ -4551,7 +4579,7 @@
       <c r="G19" s="14"/>
       <c r="H19" s="14"/>
     </row>
-    <row r="20" spans="1:8" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" ht="50.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="9"/>
       <c r="B20" s="7"/>
       <c r="C20" s="10" t="s">
@@ -4563,7 +4591,7 @@
       <c r="G20" s="8"/>
       <c r="H20" s="8"/>
     </row>
-    <row r="21" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A21" s="5" t="s">
         <v>84</v>
       </c>
@@ -4581,7 +4609,7 @@
       <c r="G21" s="5"/>
       <c r="H21" s="5"/>
     </row>
-    <row r="22" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A22" s="6" t="s">
         <v>87</v>
       </c>
@@ -4599,7 +4627,7 @@
       <c r="G22" s="6"/>
       <c r="H22" s="6"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A23" s="5" t="s">
         <v>87</v>
       </c>
@@ -4617,7 +4645,7 @@
       <c r="G23" s="5"/>
       <c r="H23" s="5"/>
     </row>
-    <row r="24" spans="1:8" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" ht="66.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="9"/>
       <c r="B24" s="9"/>
       <c r="C24" s="10" t="s">
@@ -4629,7 +4657,7 @@
       <c r="G24" s="7"/>
       <c r="H24" s="9"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A25" s="6" t="s">
         <v>90</v>
       </c>
@@ -4649,7 +4677,7 @@
       <c r="G25" s="6"/>
       <c r="H25" s="6"/>
     </row>
-    <row r="26" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A26" s="5" t="s">
         <v>90</v>
       </c>
@@ -4669,7 +4697,7 @@
       <c r="G26" s="5"/>
       <c r="H26" s="5"/>
     </row>
-    <row r="27" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A27" s="6" t="s">
         <v>90</v>
       </c>
@@ -4689,7 +4717,7 @@
       <c r="G27" s="6"/>
       <c r="H27" s="6"/>
     </row>
-    <row r="28" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A28" s="14" t="s">
         <v>90</v>
       </c>
@@ -4707,7 +4735,7 @@
       <c r="G28" s="14"/>
       <c r="H28" s="14"/>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A29" s="6" t="s">
         <v>90</v>
       </c>
@@ -4725,7 +4753,7 @@
       <c r="G29" s="6"/>
       <c r="H29" s="6"/>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A30" s="14" t="s">
         <v>90</v>
       </c>
@@ -4745,7 +4773,7 @@
       <c r="G30" s="14"/>
       <c r="H30" s="14"/>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A31" s="6" t="s">
         <v>90</v>
       </c>
@@ -4763,7 +4791,7 @@
       <c r="G31" s="6"/>
       <c r="H31" s="6"/>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A32" s="14" t="s">
         <v>90</v>
       </c>
@@ -4781,7 +4809,7 @@
       <c r="G32" s="14"/>
       <c r="H32" s="14"/>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A33" s="6" t="s">
         <v>90</v>
       </c>
@@ -4799,7 +4827,7 @@
       <c r="G33" s="6"/>
       <c r="H33" s="6"/>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A34" s="14" t="s">
         <v>90</v>
       </c>
@@ -4817,7 +4845,7 @@
       <c r="G34" s="14"/>
       <c r="H34" s="14"/>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A35" s="14" t="s">
         <v>90</v>
       </c>
@@ -4835,7 +4863,7 @@
       <c r="G35" s="14"/>
       <c r="H35" s="14"/>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A36" s="6" t="s">
         <v>90</v>
       </c>
@@ -4853,7 +4881,7 @@
       <c r="G36" s="6"/>
       <c r="H36" s="6"/>
     </row>
-    <row r="37" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A37" s="14" t="s">
         <v>90</v>
       </c>
@@ -4871,7 +4899,7 @@
       <c r="G37" s="14"/>
       <c r="H37" s="14"/>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A38" s="6" t="s">
         <v>90</v>
       </c>
@@ -4891,7 +4919,7 @@
       <c r="G38" s="6"/>
       <c r="H38" s="6"/>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A39" s="5" t="s">
         <v>90</v>
       </c>
@@ -4911,7 +4939,7 @@
       <c r="G39" s="5"/>
       <c r="H39" s="5"/>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A40" s="6" t="s">
         <v>90</v>
       </c>
@@ -4931,7 +4959,7 @@
       <c r="G40" s="6"/>
       <c r="H40" s="6"/>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A41" s="5" t="s">
         <v>90</v>
       </c>
@@ -4951,7 +4979,7 @@
       <c r="G41" s="5"/>
       <c r="H41" s="5"/>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A42" s="6" t="s">
         <v>90</v>
       </c>
@@ -4971,7 +4999,7 @@
       <c r="G42" s="6"/>
       <c r="H42" s="6"/>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A43" s="5" t="s">
         <v>90</v>
       </c>
@@ -4991,7 +5019,7 @@
       <c r="G43" s="5"/>
       <c r="H43" s="5"/>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A44" s="6" t="s">
         <v>90</v>
       </c>
@@ -5011,7 +5039,7 @@
       <c r="G44" s="6"/>
       <c r="H44" s="6"/>
     </row>
-    <row r="45" spans="1:8" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" ht="48.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A45" s="9"/>
       <c r="B45" s="9"/>
       <c r="C45" s="10" t="s">
@@ -5023,7 +5051,7 @@
       <c r="G45" s="9"/>
       <c r="H45" s="9"/>
     </row>
-    <row r="46" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A46" s="6" t="s">
         <v>153</v>
       </c>
@@ -5041,7 +5069,7 @@
       <c r="G46" s="6"/>
       <c r="H46" s="6"/>
     </row>
-    <row r="47" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A47" s="5" t="s">
         <v>153</v>
       </c>
@@ -5059,7 +5087,7 @@
       <c r="G47" s="5"/>
       <c r="H47" s="5"/>
     </row>
-    <row r="48" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A48" s="6" t="s">
         <v>153</v>
       </c>
@@ -5077,7 +5105,7 @@
       <c r="G48" s="6"/>
       <c r="H48" s="6"/>
     </row>
-    <row r="49" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A49" s="14" t="s">
         <v>153</v>
       </c>
@@ -5095,7 +5123,7 @@
       <c r="G49" s="14"/>
       <c r="H49" s="14"/>
     </row>
-    <row r="50" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A50" s="6" t="s">
         <v>153</v>
       </c>
@@ -5113,7 +5141,7 @@
       <c r="G50" s="6"/>
       <c r="H50" s="6"/>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A51" s="14" t="s">
         <v>153</v>
       </c>
@@ -5131,7 +5159,7 @@
       <c r="G51" s="14"/>
       <c r="H51" s="14"/>
     </row>
-    <row r="52" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A52" s="6" t="s">
         <v>153</v>
       </c>
@@ -5149,7 +5177,7 @@
       <c r="G52" s="6"/>
       <c r="H52" s="6"/>
     </row>
-    <row r="53" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A53" s="14" t="s">
         <v>153</v>
       </c>
@@ -5167,7 +5195,7 @@
       <c r="G53" s="14"/>
       <c r="H53" s="14"/>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A54" s="6" t="s">
         <v>153</v>
       </c>
@@ -5185,7 +5213,7 @@
       <c r="G54" s="6"/>
       <c r="H54" s="6"/>
     </row>
-    <row r="55" spans="1:8" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8" ht="42.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A55" s="9"/>
       <c r="B55" s="9"/>
       <c r="C55" s="10" t="s">
@@ -5197,7 +5225,7 @@
       <c r="G55" s="9"/>
       <c r="H55" s="9"/>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A56" s="5" t="s">
         <v>169</v>
       </c>
@@ -5215,7 +5243,7 @@
       <c r="G56" s="5"/>
       <c r="H56" s="5"/>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A57" s="6" t="s">
         <v>169</v>
       </c>
@@ -5233,7 +5261,7 @@
       <c r="G57" s="6"/>
       <c r="H57" s="6"/>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A58" s="5" t="s">
         <v>169</v>
       </c>
@@ -5251,7 +5279,7 @@
       <c r="G58" s="5"/>
       <c r="H58" s="5"/>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A59" s="6" t="s">
         <v>169</v>
       </c>
@@ -5269,7 +5297,7 @@
       <c r="G59" s="6"/>
       <c r="H59" s="6"/>
     </row>
-    <row r="60" spans="1:8" ht="390" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:8" ht="377" x14ac:dyDescent="0.35">
       <c r="A60" s="5" t="s">
         <v>169</v>
       </c>
@@ -5287,7 +5315,7 @@
       <c r="G60" s="5"/>
       <c r="H60" s="5"/>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A61" s="6" t="s">
         <v>169</v>
       </c>
@@ -5305,7 +5333,7 @@
       <c r="G61" s="6"/>
       <c r="H61" s="6"/>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A62" s="5" t="s">
         <v>169</v>
       </c>
@@ -5325,7 +5353,7 @@
       <c r="G62" s="5"/>
       <c r="H62" s="5"/>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A63" s="6" t="s">
         <v>169</v>
       </c>
@@ -5345,7 +5373,7 @@
       <c r="G63" s="6"/>
       <c r="H63" s="6"/>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A64" s="5" t="s">
         <v>169</v>
       </c>
@@ -5363,7 +5391,7 @@
       <c r="G64" s="5"/>
       <c r="H64" s="5"/>
     </row>
-    <row r="65" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A65" s="6" t="s">
         <v>169</v>
       </c>
@@ -5383,7 +5411,7 @@
       <c r="G65" s="6"/>
       <c r="H65" s="6"/>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A66" s="5" t="s">
         <v>169</v>
       </c>
@@ -5401,7 +5429,7 @@
       <c r="G66" s="5"/>
       <c r="H66" s="5"/>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A67" s="6" t="s">
         <v>169</v>
       </c>
@@ -5419,7 +5447,7 @@
       <c r="G67" s="6"/>
       <c r="H67" s="6"/>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A68" s="5" t="s">
         <v>169</v>
       </c>
@@ -5437,7 +5465,7 @@
       <c r="G68" s="5"/>
       <c r="H68" s="5"/>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A69" s="6" t="s">
         <v>169</v>
       </c>
@@ -5455,7 +5483,7 @@
       <c r="G69" s="6"/>
       <c r="H69" s="6"/>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A70" s="5" t="s">
         <v>169</v>
       </c>
@@ -5473,7 +5501,7 @@
       <c r="G70" s="5"/>
       <c r="H70" s="5"/>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A71" s="6" t="s">
         <v>169</v>
       </c>
@@ -5491,7 +5519,7 @@
       <c r="G71" s="6"/>
       <c r="H71" s="6"/>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A72" s="5" t="s">
         <v>169</v>
       </c>
@@ -5511,7 +5539,7 @@
       <c r="G72" s="5"/>
       <c r="H72" s="5"/>
     </row>
-    <row r="73" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A73" s="6" t="s">
         <v>169</v>
       </c>
@@ -5531,7 +5559,7 @@
       <c r="G73" s="6"/>
       <c r="H73" s="6"/>
     </row>
-    <row r="74" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A74" s="5" t="s">
         <v>169</v>
       </c>
@@ -5551,7 +5579,7 @@
       <c r="G74" s="5"/>
       <c r="H74" s="5"/>
     </row>
-    <row r="75" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A75" s="6" t="s">
         <v>169</v>
       </c>
@@ -5571,7 +5599,7 @@
       <c r="G75" s="6"/>
       <c r="H75" s="6"/>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A76" s="5" t="s">
         <v>169</v>
       </c>
@@ -5589,7 +5617,7 @@
       <c r="G76" s="5"/>
       <c r="H76" s="5"/>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A77" s="6" t="s">
         <v>169</v>
       </c>
@@ -5607,7 +5635,7 @@
       <c r="G77" s="6"/>
       <c r="H77" s="6"/>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A78" s="5" t="s">
         <v>169</v>
       </c>
@@ -5625,7 +5653,7 @@
       <c r="G78" s="5"/>
       <c r="H78" s="5"/>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A79" s="6" t="s">
         <v>169</v>
       </c>
@@ -5643,7 +5671,7 @@
       <c r="G79" s="6"/>
       <c r="H79" s="6"/>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A80" s="5" t="s">
         <v>169</v>
       </c>
@@ -5661,7 +5689,7 @@
       <c r="G80" s="5"/>
       <c r="H80" s="5"/>
     </row>
-    <row r="81" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A81" s="6" t="s">
         <v>169</v>
       </c>
@@ -5677,7 +5705,7 @@
       <c r="G81" s="6"/>
       <c r="H81" s="6"/>
     </row>
-    <row r="82" spans="1:8" ht="255" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:8" ht="246.5" x14ac:dyDescent="0.35">
       <c r="A82" s="5" t="s">
         <v>169</v>
       </c>
@@ -5695,7 +5723,7 @@
       <c r="G82" s="5"/>
       <c r="H82" s="5"/>
     </row>
-    <row r="83" spans="1:8" ht="270" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:8" ht="261" x14ac:dyDescent="0.35">
       <c r="A83" s="6" t="s">
         <v>169</v>
       </c>
@@ -5713,7 +5741,7 @@
       <c r="G83" s="6"/>
       <c r="H83" s="6"/>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A84" s="5" t="s">
         <v>169</v>
       </c>
@@ -5731,7 +5759,7 @@
       <c r="G84" s="5"/>
       <c r="H84" s="5"/>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A85" s="6" t="s">
         <v>169</v>
       </c>
@@ -5749,7 +5777,7 @@
       <c r="G85" s="6"/>
       <c r="H85" s="6"/>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A86" s="5" t="s">
         <v>169</v>
       </c>
@@ -5769,7 +5797,7 @@
       <c r="G86" s="5"/>
       <c r="H86" s="5"/>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A87" s="6" t="s">
         <v>169</v>
       </c>
@@ -5789,7 +5817,7 @@
       <c r="G87" s="6"/>
       <c r="H87" s="6"/>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A88" s="5" t="s">
         <v>169</v>
       </c>
@@ -5809,7 +5837,7 @@
       <c r="G88" s="5"/>
       <c r="H88" s="5"/>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A89" s="6" t="s">
         <v>169</v>
       </c>
@@ -5829,7 +5857,7 @@
       <c r="G89" s="6"/>
       <c r="H89" s="6"/>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A90" s="5" t="s">
         <v>169</v>
       </c>
@@ -5849,7 +5877,7 @@
       <c r="G90" s="5"/>
       <c r="H90" s="5"/>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A91" s="6" t="s">
         <v>169</v>
       </c>
@@ -5869,7 +5897,7 @@
       <c r="G91" s="6"/>
       <c r="H91" s="6"/>
     </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A92" s="5" t="s">
         <v>169</v>
       </c>
@@ -5889,7 +5917,7 @@
       <c r="G92" s="5"/>
       <c r="H92" s="5"/>
     </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A93" s="6" t="s">
         <v>169</v>
       </c>
@@ -5909,7 +5937,7 @@
       <c r="G93" s="6"/>
       <c r="H93" s="6"/>
     </row>
-    <row r="94" spans="1:8" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:8" ht="62.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A94" s="31"/>
       <c r="B94" s="31"/>
       <c r="C94" s="31"/>
@@ -5921,7 +5949,7 @@
       <c r="G94" s="5"/>
       <c r="H94" s="5"/>
     </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A95" s="6" t="s">
         <v>169</v>
       </c>
@@ -5939,7 +5967,7 @@
       <c r="G95" s="5"/>
       <c r="H95" s="5"/>
     </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A96" s="5" t="s">
         <v>169</v>
       </c>
@@ -5959,7 +5987,7 @@
       <c r="G96" s="5"/>
       <c r="H96" s="5"/>
     </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A97" s="6" t="s">
         <v>169</v>
       </c>
@@ -5979,7 +6007,7 @@
       <c r="G97" s="5"/>
       <c r="H97" s="5"/>
     </row>
-    <row r="98" spans="1:8" ht="195" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:8" ht="188.5" x14ac:dyDescent="0.45">
       <c r="A98" s="5" t="s">
         <v>169</v>
       </c>
@@ -5997,7 +6025,7 @@
       <c r="G98" s="5"/>
       <c r="H98" s="5"/>
     </row>
-    <row r="99" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:8" ht="16.5" x14ac:dyDescent="0.45">
       <c r="A99" s="6" t="s">
         <v>169</v>
       </c>
@@ -6015,7 +6043,7 @@
       <c r="G99" s="5"/>
       <c r="H99" s="5"/>
     </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A100" s="5" t="s">
         <v>169</v>
       </c>
@@ -6035,7 +6063,7 @@
       <c r="G100" s="5"/>
       <c r="H100" s="5"/>
     </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A101" s="6" t="s">
         <v>169</v>
       </c>
@@ -6055,7 +6083,7 @@
       <c r="G101" s="5"/>
       <c r="H101" s="5"/>
     </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A102" s="5" t="s">
         <v>169</v>
       </c>
@@ -6075,7 +6103,7 @@
       <c r="G102" s="5"/>
       <c r="H102" s="5"/>
     </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A103" s="6" t="s">
         <v>169</v>
       </c>
@@ -6095,7 +6123,7 @@
       <c r="G103" s="5"/>
       <c r="H103" s="5"/>
     </row>
-    <row r="104" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A104" s="5" t="s">
         <v>169</v>
       </c>
@@ -6115,7 +6143,7 @@
       <c r="G104" s="5"/>
       <c r="H104" s="5"/>
     </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A105" s="6" t="s">
         <v>169</v>
       </c>
@@ -6135,7 +6163,7 @@
       <c r="G105" s="5"/>
       <c r="H105" s="5"/>
     </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A106" s="5" t="s">
         <v>169</v>
       </c>
@@ -6155,7 +6183,7 @@
       <c r="G106" s="5"/>
       <c r="H106" s="5"/>
     </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A107" s="6" t="s">
         <v>169</v>
       </c>
@@ -6175,7 +6203,7 @@
       <c r="G107" s="5"/>
       <c r="H107" s="5"/>
     </row>
-    <row r="108" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A108" s="5" t="s">
         <v>169</v>
       </c>
@@ -6195,7 +6223,7 @@
       <c r="G108" s="5"/>
       <c r="H108" s="5"/>
     </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A109" s="6" t="s">
         <v>169</v>
       </c>
@@ -6215,7 +6243,7 @@
       <c r="G109" s="5"/>
       <c r="H109" s="5"/>
     </row>
-    <row r="110" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A110" s="5" t="s">
         <v>169</v>
       </c>
@@ -6235,7 +6263,7 @@
       <c r="G110" s="5"/>
       <c r="H110" s="5"/>
     </row>
-    <row r="111" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A111" s="6" t="s">
         <v>169</v>
       </c>
@@ -6253,7 +6281,7 @@
       <c r="G111" s="5"/>
       <c r="H111" s="5"/>
     </row>
-    <row r="112" spans="1:8" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:8" ht="50.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A112" s="9"/>
       <c r="B112" s="9"/>
       <c r="C112" s="11" t="s">
@@ -6265,7 +6293,7 @@
       <c r="G112" s="9"/>
       <c r="H112" s="9"/>
     </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A113" s="5" t="s">
         <v>312</v>
       </c>
@@ -6283,7 +6311,7 @@
       <c r="G113" s="5"/>
       <c r="H113" s="5"/>
     </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A114" s="6" t="s">
         <v>312</v>
       </c>
@@ -6301,7 +6329,7 @@
       <c r="G114" s="6"/>
       <c r="H114" s="6"/>
     </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A115" s="5" t="s">
         <v>312</v>
       </c>
@@ -6319,7 +6347,7 @@
       <c r="G115" s="5"/>
       <c r="H115" s="5"/>
     </row>
-    <row r="116" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A116" s="6" t="s">
         <v>312</v>
       </c>
@@ -6339,7 +6367,7 @@
       <c r="G116" s="6"/>
       <c r="H116" s="6"/>
     </row>
-    <row r="117" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A117" s="5" t="s">
         <v>312</v>
       </c>
@@ -6359,7 +6387,7 @@
       <c r="G117" s="5"/>
       <c r="H117" s="5"/>
     </row>
-    <row r="118" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A118" s="6" t="s">
         <v>312</v>
       </c>
@@ -6379,7 +6407,7 @@
       <c r="G118" s="6"/>
       <c r="H118" s="6"/>
     </row>
-    <row r="119" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A119" s="5" t="s">
         <v>312</v>
       </c>
@@ -6399,7 +6427,7 @@
       <c r="G119" s="5"/>
       <c r="H119" s="5"/>
     </row>
-    <row r="120" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A120" s="6" t="s">
         <v>312</v>
       </c>
@@ -6419,7 +6447,7 @@
       <c r="G120" s="6"/>
       <c r="H120" s="6"/>
     </row>
-    <row r="121" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A121" s="5" t="s">
         <v>312</v>
       </c>
@@ -6439,7 +6467,7 @@
       <c r="G121" s="5"/>
       <c r="H121" s="5"/>
     </row>
-    <row r="122" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A122" s="6" t="s">
         <v>312</v>
       </c>
@@ -6457,7 +6485,7 @@
       <c r="G122" s="6"/>
       <c r="H122" s="6"/>
     </row>
-    <row r="123" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A123" s="5" t="s">
         <v>312</v>
       </c>
@@ -6475,7 +6503,7 @@
       <c r="G123" s="5"/>
       <c r="H123" s="5"/>
     </row>
-    <row r="124" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A124" s="6" t="s">
         <v>312</v>
       </c>
@@ -6493,7 +6521,7 @@
       <c r="G124" s="6"/>
       <c r="H124" s="6"/>
     </row>
-    <row r="125" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A125" s="5" t="s">
         <v>312</v>
       </c>
@@ -6511,7 +6539,7 @@
       <c r="G125" s="5"/>
       <c r="H125" s="5"/>
     </row>
-    <row r="126" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A126" s="6" t="s">
         <v>312</v>
       </c>
@@ -6529,7 +6557,7 @@
       <c r="G126" s="6"/>
       <c r="H126" s="6"/>
     </row>
-    <row r="127" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A127" s="5" t="s">
         <v>312</v>
       </c>
@@ -6549,7 +6577,7 @@
       <c r="G127" s="5"/>
       <c r="H127" s="5"/>
     </row>
-    <row r="128" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A128" s="6" t="s">
         <v>312</v>
       </c>
@@ -6567,7 +6595,7 @@
       <c r="G128" s="6"/>
       <c r="H128" s="6"/>
     </row>
-    <row r="129" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A129" s="5" t="s">
         <v>312</v>
       </c>
@@ -6585,7 +6613,7 @@
       <c r="G129" s="5"/>
       <c r="H129" s="5"/>
     </row>
-    <row r="130" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A130" s="6" t="s">
         <v>312</v>
       </c>
@@ -6603,7 +6631,7 @@
       <c r="G130" s="6"/>
       <c r="H130" s="6"/>
     </row>
-    <row r="131" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A131" s="5" t="s">
         <v>312</v>
       </c>
@@ -6623,7 +6651,7 @@
       <c r="G131" s="5"/>
       <c r="H131" s="5"/>
     </row>
-    <row r="132" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A132" s="6" t="s">
         <v>312</v>
       </c>
@@ -6641,7 +6669,7 @@
       <c r="G132" s="6"/>
       <c r="H132" s="6"/>
     </row>
-    <row r="133" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A133" s="5" t="s">
         <v>312</v>
       </c>
@@ -6661,7 +6689,7 @@
       <c r="G133" s="5"/>
       <c r="H133" s="5"/>
     </row>
-    <row r="134" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A134" s="6" t="s">
         <v>312</v>
       </c>
@@ -6679,7 +6707,7 @@
       <c r="G134" s="6"/>
       <c r="H134" s="6"/>
     </row>
-    <row r="135" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A135" s="5" t="s">
         <v>312</v>
       </c>
@@ -6695,7 +6723,7 @@
       <c r="G135" s="5"/>
       <c r="H135" s="5"/>
     </row>
-    <row r="136" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A136" s="6" t="s">
         <v>312</v>
       </c>
@@ -6713,7 +6741,7 @@
       <c r="G136" s="6"/>
       <c r="H136" s="6"/>
     </row>
-    <row r="137" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A137" s="5" t="s">
         <v>312</v>
       </c>
@@ -6731,7 +6759,7 @@
       <c r="G137" s="5"/>
       <c r="H137" s="5"/>
     </row>
-    <row r="138" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A138" s="6" t="s">
         <v>312</v>
       </c>
@@ -6751,7 +6779,7 @@
       <c r="G138" s="6"/>
       <c r="H138" s="6"/>
     </row>
-    <row r="139" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A139" s="5" t="s">
         <v>312</v>
       </c>
@@ -6771,7 +6799,7 @@
       <c r="G139" s="5"/>
       <c r="H139" s="5"/>
     </row>
-    <row r="140" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A140" s="6" t="s">
         <v>312</v>
       </c>
@@ -6791,7 +6819,7 @@
       <c r="G140" s="6"/>
       <c r="H140" s="6"/>
     </row>
-    <row r="141" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A141" s="5" t="s">
         <v>312</v>
       </c>
@@ -6811,7 +6839,7 @@
       <c r="G141" s="5"/>
       <c r="H141" s="5"/>
     </row>
-    <row r="142" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A142" s="6" t="s">
         <v>312</v>
       </c>
@@ -6831,7 +6859,7 @@
       <c r="G142" s="6"/>
       <c r="H142" s="6"/>
     </row>
-    <row r="143" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A143" s="5" t="s">
         <v>312</v>
       </c>
@@ -6851,7 +6879,7 @@
       <c r="G143" s="5"/>
       <c r="H143" s="5"/>
     </row>
-    <row r="144" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A144" s="6" t="s">
         <v>312</v>
       </c>
@@ -6871,7 +6899,7 @@
       <c r="G144" s="6"/>
       <c r="H144" s="6"/>
     </row>
-    <row r="145" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A145" s="5" t="s">
         <v>312</v>
       </c>
@@ -6891,7 +6919,7 @@
       <c r="G145" s="5"/>
       <c r="H145" s="5"/>
     </row>
-    <row r="146" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A146" s="6" t="s">
         <v>312</v>
       </c>
@@ -6911,7 +6939,7 @@
       <c r="G146" s="6"/>
       <c r="H146" s="6"/>
     </row>
-    <row r="147" spans="1:8" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:8" ht="47.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A147" s="9"/>
       <c r="B147" s="9"/>
       <c r="C147" s="10" t="s">
@@ -6923,7 +6951,7 @@
       <c r="G147" s="9"/>
       <c r="H147" s="9"/>
     </row>
-    <row r="148" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A148" s="5" t="s">
         <v>352</v>
       </c>
@@ -6943,7 +6971,7 @@
       <c r="G148" s="5"/>
       <c r="H148" s="5"/>
     </row>
-    <row r="149" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A149" s="6" t="s">
         <v>352</v>
       </c>
@@ -6963,7 +6991,7 @@
       <c r="G149" s="6"/>
       <c r="H149" s="6"/>
     </row>
-    <row r="150" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A150" s="5" t="s">
         <v>352</v>
       </c>
@@ -6983,7 +7011,7 @@
       <c r="G150" s="5"/>
       <c r="H150" s="5"/>
     </row>
-    <row r="151" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A151" s="6" t="s">
         <v>352</v>
       </c>
@@ -7003,7 +7031,7 @@
       <c r="G151" s="6"/>
       <c r="H151" s="6"/>
     </row>
-    <row r="152" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A152" s="5" t="s">
         <v>352</v>
       </c>
@@ -7023,7 +7051,7 @@
       <c r="G152" s="5"/>
       <c r="H152" s="5"/>
     </row>
-    <row r="153" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A153" s="6" t="s">
         <v>352</v>
       </c>
@@ -7043,7 +7071,7 @@
       <c r="G153" s="6"/>
       <c r="H153" s="6"/>
     </row>
-    <row r="154" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A154" s="5" t="s">
         <v>352</v>
       </c>
@@ -7063,7 +7091,7 @@
       <c r="G154" s="5"/>
       <c r="H154" s="5"/>
     </row>
-    <row r="155" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:8" ht="58" x14ac:dyDescent="0.35">
       <c r="A155" s="6" t="s">
         <v>352</v>
       </c>
@@ -7083,7 +7111,7 @@
       <c r="G155" s="6"/>
       <c r="H155" s="6"/>
     </row>
-    <row r="156" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A156" s="5" t="s">
         <v>352</v>
       </c>
@@ -7103,7 +7131,7 @@
       <c r="G156" s="5"/>
       <c r="H156" s="5"/>
     </row>
-    <row r="157" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A157" s="6" t="s">
         <v>352</v>
       </c>
@@ -7123,7 +7151,7 @@
       <c r="G157" s="6"/>
       <c r="H157" s="6"/>
     </row>
-    <row r="158" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A158" s="5" t="s">
         <v>352</v>
       </c>
@@ -7143,7 +7171,7 @@
       <c r="G158" s="5"/>
       <c r="H158" s="5"/>
     </row>
-    <row r="159" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A159" s="6" t="s">
         <v>352</v>
       </c>
@@ -7163,7 +7191,7 @@
       <c r="G159" s="6"/>
       <c r="H159" s="6"/>
     </row>
-    <row r="160" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A160" s="5" t="s">
         <v>352</v>
       </c>
@@ -7183,7 +7211,7 @@
       <c r="G160" s="5"/>
       <c r="H160" s="5"/>
     </row>
-    <row r="161" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A161" s="6" t="s">
         <v>352</v>
       </c>
@@ -7203,7 +7231,7 @@
       <c r="G161" s="6"/>
       <c r="H161" s="6"/>
     </row>
-    <row r="162" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:8" ht="58" x14ac:dyDescent="0.35">
       <c r="A162" s="5" t="s">
         <v>352</v>
       </c>
@@ -7223,7 +7251,7 @@
       <c r="G162" s="5"/>
       <c r="H162" s="5"/>
     </row>
-    <row r="163" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A163" s="6" t="s">
         <v>352</v>
       </c>
@@ -7243,7 +7271,7 @@
       <c r="G163" s="6"/>
       <c r="H163" s="6"/>
     </row>
-    <row r="164" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A164" s="5" t="s">
         <v>352</v>
       </c>
@@ -7263,7 +7291,7 @@
       <c r="G164" s="5"/>
       <c r="H164" s="5"/>
     </row>
-    <row r="165" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A165" s="6" t="s">
         <v>352</v>
       </c>
@@ -7283,7 +7311,7 @@
       <c r="G165" s="6"/>
       <c r="H165" s="6"/>
     </row>
-    <row r="166" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A166" s="14" t="s">
         <v>352</v>
       </c>
@@ -7303,7 +7331,7 @@
       <c r="G166" s="14"/>
       <c r="H166" s="14"/>
     </row>
-    <row r="167" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A167" s="6" t="s">
         <v>352</v>
       </c>
@@ -7323,7 +7351,7 @@
       <c r="G167" s="6"/>
       <c r="H167" s="6"/>
     </row>
-    <row r="168" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A168" s="14" t="s">
         <v>352</v>
       </c>
@@ -7343,7 +7371,7 @@
       <c r="G168" s="14"/>
       <c r="H168" s="14"/>
     </row>
-    <row r="169" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A169" s="6" t="s">
         <v>352</v>
       </c>
@@ -7363,7 +7391,7 @@
       <c r="G169" s="6"/>
       <c r="H169" s="6"/>
     </row>
-    <row r="170" spans="1:8" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:8" ht="48.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A170" s="10"/>
       <c r="B170" s="9"/>
       <c r="C170" s="10" t="s">
@@ -7375,7 +7403,7 @@
       <c r="G170" s="9"/>
       <c r="H170" s="9"/>
     </row>
-    <row r="171" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A171" s="5" t="s">
         <v>407</v>
       </c>
@@ -7393,7 +7421,7 @@
       <c r="G171" s="5"/>
       <c r="H171" s="5"/>
     </row>
-    <row r="172" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A172" s="6" t="s">
         <v>407</v>
       </c>
@@ -7409,7 +7437,7 @@
       <c r="G172" s="6"/>
       <c r="H172" s="6"/>
     </row>
-    <row r="173" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A173" s="5" t="s">
         <v>407</v>
       </c>
@@ -7427,7 +7455,7 @@
       <c r="G173" s="5"/>
       <c r="H173" s="5"/>
     </row>
-    <row r="174" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A174" s="6" t="s">
         <v>407</v>
       </c>
@@ -7447,7 +7475,7 @@
       <c r="G174" s="6"/>
       <c r="H174" s="6"/>
     </row>
-    <row r="175" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A175" s="5" t="s">
         <v>407</v>
       </c>
@@ -7465,7 +7493,7 @@
       <c r="G175" s="5"/>
       <c r="H175" s="5"/>
     </row>
-    <row r="176" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A176" s="6" t="s">
         <v>407</v>
       </c>
@@ -7483,7 +7511,7 @@
       <c r="G176" s="6"/>
       <c r="H176" s="6"/>
     </row>
-    <row r="177" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A177" s="5" t="s">
         <v>420</v>
       </c>
@@ -7501,7 +7529,7 @@
       <c r="G177" s="5"/>
       <c r="H177" s="5"/>
     </row>
-    <row r="178" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A178" s="6" t="s">
         <v>420</v>
       </c>
@@ -7517,7 +7545,7 @@
       <c r="G178" s="6"/>
       <c r="H178" s="6"/>
     </row>
-    <row r="179" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A179" s="5" t="s">
         <v>420</v>
       </c>
@@ -7537,7 +7565,7 @@
       <c r="G179" s="5"/>
       <c r="H179" s="5"/>
     </row>
-    <row r="180" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A180" s="6" t="s">
         <v>420</v>
       </c>
@@ -7555,7 +7583,7 @@
       <c r="G180" s="6"/>
       <c r="H180" s="6"/>
     </row>
-    <row r="181" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A181" s="5" t="s">
         <v>420</v>
       </c>
@@ -7573,7 +7601,7 @@
       <c r="G181" s="5"/>
       <c r="H181" s="5"/>
     </row>
-    <row r="182" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A182" s="6" t="s">
         <v>420</v>
       </c>
@@ -7591,7 +7619,7 @@
       <c r="G182" s="6"/>
       <c r="H182" s="6"/>
     </row>
-    <row r="183" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A183" s="5" t="s">
         <v>425</v>
       </c>
@@ -7609,7 +7637,7 @@
       <c r="G183" s="5"/>
       <c r="H183" s="5"/>
     </row>
-    <row r="184" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A184" s="6" t="s">
         <v>425</v>
       </c>
@@ -7625,7 +7653,7 @@
       <c r="G184" s="6"/>
       <c r="H184" s="6"/>
     </row>
-    <row r="185" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A185" s="5" t="s">
         <v>425</v>
       </c>
@@ -7641,7 +7669,7 @@
       <c r="G185" s="5"/>
       <c r="H185" s="5"/>
     </row>
-    <row r="186" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A186" s="6" t="s">
         <v>425</v>
       </c>
@@ -7659,7 +7687,7 @@
       <c r="G186" s="6"/>
       <c r="H186" s="6"/>
     </row>
-    <row r="187" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A187" s="5" t="s">
         <v>425</v>
       </c>
@@ -7675,7 +7703,7 @@
       <c r="G187" s="5"/>
       <c r="H187" s="5"/>
     </row>
-    <row r="188" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A188" s="6" t="s">
         <v>425</v>
       </c>
@@ -7693,7 +7721,7 @@
       <c r="G188" s="6"/>
       <c r="H188" s="6"/>
     </row>
-    <row r="189" spans="1:8" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:8" ht="55.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A189" s="9"/>
       <c r="B189" s="9"/>
       <c r="C189" s="10" t="s">
@@ -7705,7 +7733,7 @@
       <c r="G189" s="9"/>
       <c r="H189" s="9"/>
     </row>
-    <row r="190" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A190" s="5" t="s">
         <v>429</v>
       </c>
@@ -7725,7 +7753,7 @@
       <c r="G190" s="5"/>
       <c r="H190" s="5"/>
     </row>
-    <row r="191" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A191" s="6" t="s">
         <v>429</v>
       </c>
@@ -7745,7 +7773,7 @@
       <c r="G191" s="6"/>
       <c r="H191" s="6"/>
     </row>
-    <row r="192" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A192" s="5" t="s">
         <v>429</v>
       </c>
@@ -7765,7 +7793,7 @@
       <c r="G192" s="5"/>
       <c r="H192" s="5"/>
     </row>
-    <row r="193" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A193" s="6" t="s">
         <v>429</v>
       </c>
@@ -7785,7 +7813,7 @@
       <c r="G193" s="6"/>
       <c r="H193" s="6"/>
     </row>
-    <row r="194" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A194" s="5" t="s">
         <v>429</v>
       </c>
@@ -7805,7 +7833,7 @@
       <c r="G194" s="5"/>
       <c r="H194" s="5"/>
     </row>
-    <row r="195" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A195" s="6" t="s">
         <v>429</v>
       </c>
@@ -7825,7 +7853,7 @@
       <c r="G195" s="6"/>
       <c r="H195" s="6"/>
     </row>
-    <row r="196" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A196" s="5" t="s">
         <v>429</v>
       </c>
@@ -7845,7 +7873,7 @@
       <c r="G196" s="5"/>
       <c r="H196" s="5"/>
     </row>
-    <row r="197" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A197" s="6" t="s">
         <v>429</v>
       </c>
@@ -7865,7 +7893,7 @@
       <c r="G197" s="6"/>
       <c r="H197" s="6"/>
     </row>
-    <row r="198" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A198" s="5" t="s">
         <v>429</v>
       </c>
@@ -7885,7 +7913,7 @@
       <c r="G198" s="5"/>
       <c r="H198" s="5"/>
     </row>
-    <row r="199" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A199" s="6" t="s">
         <v>429</v>
       </c>
@@ -7905,7 +7933,7 @@
       <c r="G199" s="6"/>
       <c r="H199" s="6"/>
     </row>
-    <row r="200" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A200" s="5" t="s">
         <v>429</v>
       </c>
@@ -7925,7 +7953,7 @@
       <c r="G200" s="5"/>
       <c r="H200" s="5"/>
     </row>
-    <row r="201" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A201" s="6" t="s">
         <v>429</v>
       </c>
@@ -7945,7 +7973,7 @@
       <c r="G201" s="6"/>
       <c r="H201" s="6"/>
     </row>
-    <row r="202" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A202" s="5" t="s">
         <v>429</v>
       </c>
@@ -7965,7 +7993,7 @@
       <c r="G202" s="5"/>
       <c r="H202" s="5"/>
     </row>
-    <row r="203" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A203" s="6" t="s">
         <v>429</v>
       </c>
@@ -7987,7 +8015,7 @@
       <c r="G203" s="6"/>
       <c r="H203" s="6"/>
     </row>
-    <row r="204" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A204" s="5" t="s">
         <v>429</v>
       </c>
@@ -8007,7 +8035,7 @@
       <c r="G204" s="5"/>
       <c r="H204" s="5"/>
     </row>
-    <row r="205" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A205" s="9"/>
       <c r="B205" s="9"/>
       <c r="C205" s="10" t="s">
@@ -8019,7 +8047,7 @@
       <c r="G205" s="9"/>
       <c r="H205" s="9"/>
     </row>
-    <row r="206" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A206" s="5" t="s">
         <v>459</v>
       </c>
@@ -8037,7 +8065,7 @@
       <c r="G206" s="5"/>
       <c r="H206" s="5"/>
     </row>
-    <row r="207" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A207" s="6" t="s">
         <v>459</v>
       </c>
@@ -8055,7 +8083,7 @@
       <c r="G207" s="6"/>
       <c r="H207" s="6"/>
     </row>
-    <row r="208" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A208" s="5" t="s">
         <v>459</v>
       </c>
@@ -8073,7 +8101,7 @@
       <c r="G208" s="5"/>
       <c r="H208" s="5"/>
     </row>
-    <row r="209" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A209" s="6" t="s">
         <v>459</v>
       </c>
@@ -8091,7 +8119,7 @@
       <c r="G209" s="6"/>
       <c r="H209" s="6"/>
     </row>
-    <row r="210" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A210" s="14" t="s">
         <v>459</v>
       </c>
@@ -8109,7 +8137,7 @@
       <c r="G210" s="5"/>
       <c r="H210" s="5"/>
     </row>
-    <row r="211" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A211" s="6" t="s">
         <v>459</v>
       </c>
@@ -8127,7 +8155,7 @@
       <c r="G211" s="6"/>
       <c r="H211" s="6"/>
     </row>
-    <row r="212" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A212" s="14" t="s">
         <v>459</v>
       </c>
@@ -8143,7 +8171,7 @@
       <c r="G212" s="5"/>
       <c r="H212" s="5"/>
     </row>
-    <row r="213" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A213" s="6" t="s">
         <v>459</v>
       </c>
@@ -8161,7 +8189,7 @@
       <c r="G213" s="6"/>
       <c r="H213" s="6"/>
     </row>
-    <row r="214" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A214" s="5" t="s">
         <v>459</v>
       </c>
@@ -8179,7 +8207,7 @@
       <c r="G214" s="5"/>
       <c r="H214" s="5"/>
     </row>
-    <row r="215" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A215" s="6" t="s">
         <v>459</v>
       </c>
@@ -8197,7 +8225,7 @@
       <c r="G215" s="6"/>
       <c r="H215" s="6"/>
     </row>
-    <row r="216" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A216" s="14" t="s">
         <v>459</v>
       </c>
@@ -8215,7 +8243,7 @@
       <c r="G216" s="14"/>
       <c r="H216" s="14"/>
     </row>
-    <row r="217" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A217" s="6" t="s">
         <v>459</v>
       </c>
@@ -8233,7 +8261,7 @@
       <c r="G217" s="6"/>
       <c r="H217" s="6"/>
     </row>
-    <row r="218" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A218" s="14" t="s">
         <v>459</v>
       </c>
@@ -8251,7 +8279,7 @@
       <c r="G218" s="14"/>
       <c r="H218" s="14"/>
     </row>
-    <row r="219" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A219" s="6" t="s">
         <v>459</v>
       </c>
@@ -8269,7 +8297,7 @@
       <c r="G219" s="6"/>
       <c r="H219" s="6"/>
     </row>
-    <row r="220" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A220" s="5" t="s">
         <v>459</v>
       </c>
@@ -8287,7 +8315,7 @@
       <c r="G220" s="5"/>
       <c r="H220" s="5"/>
     </row>
-    <row r="221" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A221" s="6" t="s">
         <v>459</v>
       </c>
@@ -8305,7 +8333,7 @@
       <c r="G221" s="6"/>
       <c r="H221" s="6"/>
     </row>
-    <row r="222" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A222" s="5" t="s">
         <v>459</v>
       </c>
@@ -8321,7 +8349,7 @@
       <c r="G222" s="5"/>
       <c r="H222" s="5"/>
     </row>
-    <row r="223" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A223" s="6" t="s">
         <v>459</v>
       </c>
@@ -8337,7 +8365,7 @@
       <c r="G223" s="6"/>
       <c r="H223" s="6"/>
     </row>
-    <row r="224" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A224" s="5" t="s">
         <v>459</v>
       </c>
@@ -8353,7 +8381,7 @@
       <c r="G224" s="5"/>
       <c r="H224" s="5"/>
     </row>
-    <row r="225" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A225" s="6" t="s">
         <v>459</v>
       </c>
@@ -8369,7 +8397,7 @@
       <c r="G225" s="6"/>
       <c r="H225" s="6"/>
     </row>
-    <row r="226" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A226" s="5" t="s">
         <v>459</v>
       </c>
@@ -8385,7 +8413,7 @@
       <c r="G226" s="5"/>
       <c r="H226" s="5"/>
     </row>
-    <row r="227" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A227" s="6" t="s">
         <v>459</v>
       </c>
@@ -8401,7 +8429,7 @@
       <c r="G227" s="6"/>
       <c r="H227" s="6"/>
     </row>
-    <row r="228" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A228" s="5" t="s">
         <v>459</v>
       </c>
@@ -8417,7 +8445,7 @@
       <c r="G228" s="5"/>
       <c r="H228" s="5"/>
     </row>
-    <row r="229" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A229" s="6" t="s">
         <v>459</v>
       </c>
@@ -8457,17 +8485,17 @@
       <selection pane="bottomLeft" activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="55.5703125" customWidth="1"/>
-    <col min="3" max="3" width="42.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="39.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="48.7109375" customWidth="1"/>
-    <col min="6" max="6" width="50.42578125" customWidth="1"/>
-    <col min="7" max="7" width="46.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="55.54296875" customWidth="1"/>
+    <col min="3" max="3" width="42.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="39.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="48.7265625" customWidth="1"/>
+    <col min="6" max="6" width="50.453125" customWidth="1"/>
+    <col min="7" max="7" width="46.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="77.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="77.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="49" t="s">
         <v>788</v>
       </c>
@@ -8478,7 +8506,7 @@
       <c r="F1" s="49"/>
       <c r="G1" s="49"/>
     </row>
-    <row r="3" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="41" t="s">
         <v>798</v>
       </c>
@@ -8501,7 +8529,7 @@
         <v>683</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" s="36"/>
       <c r="B4" s="36"/>
       <c r="C4" s="37"/>
@@ -8510,7 +8538,7 @@
       <c r="F4" s="36"/>
       <c r="G4" s="36"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" s="39" t="s">
         <v>780</v>
       </c>
@@ -8521,7 +8549,7 @@
       <c r="F5" s="36"/>
       <c r="G5" s="36"/>
     </row>
-    <row r="6" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A6" s="43">
         <v>1</v>
       </c>
@@ -8538,7 +8566,7 @@
       <c r="F6" s="35"/>
       <c r="G6" s="34"/>
     </row>
-    <row r="7" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A7" s="43">
         <v>2</v>
       </c>
@@ -8555,7 +8583,7 @@
       <c r="F7" s="35"/>
       <c r="G7" s="34"/>
     </row>
-    <row r="8" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="58" x14ac:dyDescent="0.35">
       <c r="A8" s="43">
         <v>3</v>
       </c>
@@ -8572,7 +8600,7 @@
       <c r="F8" s="35"/>
       <c r="G8" s="34"/>
     </row>
-    <row r="9" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="58" x14ac:dyDescent="0.35">
       <c r="A9" s="43">
         <v>4</v>
       </c>
@@ -8589,7 +8617,7 @@
       <c r="F9" s="35"/>
       <c r="G9" s="34"/>
     </row>
-    <row r="10" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A10" s="43">
         <v>5</v>
       </c>
@@ -8606,7 +8634,7 @@
       <c r="F10" s="35"/>
       <c r="G10" s="34"/>
     </row>
-    <row r="11" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A11" s="43">
         <v>6</v>
       </c>
@@ -8623,7 +8651,7 @@
       <c r="F11" s="35"/>
       <c r="G11" s="34"/>
     </row>
-    <row r="12" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A12" s="43">
         <v>7</v>
       </c>
@@ -8640,7 +8668,7 @@
       <c r="F12" s="35"/>
       <c r="G12" s="34"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" s="45"/>
       <c r="B13" s="36"/>
       <c r="C13" s="37"/>
@@ -8649,7 +8677,7 @@
       <c r="F13" s="36"/>
       <c r="G13" s="36"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14" s="47" t="s">
         <v>781</v>
       </c>
@@ -8660,7 +8688,7 @@
       <c r="F14" s="36"/>
       <c r="G14" s="36"/>
     </row>
-    <row r="15" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A15" s="43">
         <v>1</v>
       </c>
@@ -8677,7 +8705,7 @@
       <c r="F15" s="35"/>
       <c r="G15" s="34"/>
     </row>
-    <row r="16" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A16" s="43">
         <v>2</v>
       </c>
@@ -8694,7 +8722,7 @@
       <c r="F16" s="35"/>
       <c r="G16" s="34"/>
     </row>
-    <row r="17" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A17" s="43">
         <v>3</v>
       </c>
@@ -8711,7 +8739,7 @@
       <c r="F17" s="35"/>
       <c r="G17" s="34"/>
     </row>
-    <row r="18" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A18" s="43">
         <v>4</v>
       </c>
@@ -8728,7 +8756,7 @@
       <c r="F18" s="35"/>
       <c r="G18" s="34"/>
     </row>
-    <row r="19" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A19" s="43">
         <v>5</v>
       </c>
@@ -8745,7 +8773,7 @@
       <c r="F19" s="40"/>
       <c r="G19" s="34"/>
     </row>
-    <row r="20" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A20" s="43">
         <v>6</v>
       </c>
@@ -8762,7 +8790,7 @@
       <c r="F20" s="35"/>
       <c r="G20" s="34"/>
     </row>
-    <row r="21" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A21" s="43">
         <v>6</v>
       </c>
@@ -8779,7 +8807,7 @@
       <c r="F21" s="35"/>
       <c r="G21" s="34"/>
     </row>
-    <row r="22" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A22" s="43">
         <v>7</v>
       </c>
@@ -8796,7 +8824,7 @@
       <c r="F22" s="40"/>
       <c r="G22" s="34"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A23" s="43">
         <v>8</v>
       </c>
@@ -8813,7 +8841,7 @@
       <c r="F23" s="40"/>
       <c r="G23" s="34"/>
     </row>
-    <row r="24" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A24" s="43">
         <v>9</v>
       </c>
@@ -8830,7 +8858,7 @@
       <c r="F24" s="35"/>
       <c r="G24" s="34"/>
     </row>
-    <row r="25" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" ht="58" x14ac:dyDescent="0.35">
       <c r="A25" s="43">
         <v>10</v>
       </c>
@@ -8847,7 +8875,7 @@
       <c r="F25" s="40"/>
       <c r="G25" s="34"/>
     </row>
-    <row r="26" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A26" s="43">
         <v>11</v>
       </c>
@@ -8864,7 +8892,7 @@
       <c r="F26" s="40"/>
       <c r="G26" s="34"/>
     </row>
-    <row r="27" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A27" s="43">
         <v>12</v>
       </c>
@@ -8881,7 +8909,7 @@
       <c r="F27" s="40"/>
       <c r="G27" s="34"/>
     </row>
-    <row r="28" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A28" s="43">
         <v>13</v>
       </c>
@@ -8898,7 +8926,7 @@
       <c r="F28" s="40"/>
       <c r="G28" s="34"/>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B29" s="36"/>
       <c r="C29" s="37"/>
       <c r="D29" s="36"/>
@@ -8923,16 +8951,16 @@
       <selection activeCell="D103" sqref="A103:XFD103"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="44.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="255.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="173.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="44.26953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="255.7265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="173.54296875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="44" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="26" x14ac:dyDescent="0.35">
       <c r="A1" s="15" t="s">
         <v>507</v>
       </c>
@@ -8949,7 +8977,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="16" t="s">
         <v>507</v>
       </c>
@@ -8966,7 +8994,7 @@
         <v>513</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="19" t="s">
         <v>507</v>
       </c>
@@ -8983,7 +9011,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="16"/>
       <c r="B4" s="17" t="s">
         <v>518</v>
@@ -8998,7 +9026,7 @@
         <v>513</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="19"/>
       <c r="B5" s="20" t="s">
         <v>71</v>
@@ -9013,7 +9041,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="53" t="s">
         <v>507</v>
       </c>
@@ -9030,7 +9058,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="53"/>
       <c r="B7" s="54"/>
       <c r="C7" s="54"/>
@@ -9039,7 +9067,7 @@
       </c>
       <c r="E7" s="55"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" s="53"/>
       <c r="B8" s="54"/>
       <c r="C8" s="54"/>
@@ -9048,7 +9076,7 @@
       </c>
       <c r="E8" s="55"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" s="19" t="s">
         <v>507</v>
       </c>
@@ -9065,7 +9093,7 @@
         <v>531</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" s="53" t="s">
         <v>507</v>
       </c>
@@ -9082,7 +9110,7 @@
         <v>535</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" s="53"/>
       <c r="B11" s="54"/>
       <c r="C11" s="54"/>
@@ -9091,7 +9119,7 @@
       </c>
       <c r="E11" s="55"/>
     </row>
-    <row r="12" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="50" t="s">
         <v>507</v>
       </c>
@@ -9108,7 +9136,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" s="50"/>
       <c r="B13" s="51"/>
       <c r="C13" s="51"/>
@@ -9117,7 +9145,7 @@
       </c>
       <c r="E13" s="52"/>
     </row>
-    <row r="14" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="16" t="s">
         <v>507</v>
       </c>
@@ -9134,7 +9162,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" s="19"/>
       <c r="B15" s="20" t="s">
         <v>544</v>
@@ -9149,7 +9177,7 @@
         <v>547</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" s="16"/>
       <c r="B16" s="17" t="s">
         <v>548</v>
@@ -9164,7 +9192,7 @@
         <v>547</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" s="19"/>
       <c r="B17" s="20" t="s">
         <v>550</v>
@@ -9179,7 +9207,7 @@
         <v>547</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" s="16"/>
       <c r="B18" s="17" t="s">
         <v>552</v>
@@ -9194,7 +9222,7 @@
         <v>547</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" s="19"/>
       <c r="B19" s="20" t="s">
         <v>177</v>
@@ -9209,7 +9237,7 @@
         <v>547</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" s="16"/>
       <c r="B20" s="17" t="s">
         <v>556</v>
@@ -9224,7 +9252,7 @@
         <v>547</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" s="19"/>
       <c r="B21" s="20" t="s">
         <v>558</v>
@@ -9239,7 +9267,7 @@
         <v>547</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" s="16"/>
       <c r="B22" s="17" t="s">
         <v>560</v>
@@ -9254,7 +9282,7 @@
         <v>547</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" s="19"/>
       <c r="B23" s="20" t="s">
         <v>562</v>
@@ -9269,7 +9297,7 @@
         <v>547</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="53"/>
       <c r="B24" s="54" t="s">
         <v>565</v>
@@ -9284,7 +9312,7 @@
         <v>568</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" s="53"/>
       <c r="B25" s="54"/>
       <c r="C25" s="54"/>
@@ -9293,7 +9321,7 @@
       </c>
       <c r="E25" s="55"/>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" s="50"/>
       <c r="B26" s="51" t="s">
         <v>570</v>
@@ -9308,7 +9336,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27" s="50"/>
       <c r="B27" s="51"/>
       <c r="C27" s="51"/>
@@ -9317,7 +9345,7 @@
       </c>
       <c r="E27" s="52"/>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28" s="53"/>
       <c r="B28" s="54" t="s">
         <v>575</v>
@@ -9332,7 +9360,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29" s="53"/>
       <c r="B29" s="54"/>
       <c r="C29" s="54"/>
@@ -9341,7 +9369,7 @@
       </c>
       <c r="E29" s="55"/>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A30" s="50"/>
       <c r="B30" s="51" t="s">
         <v>579</v>
@@ -9356,7 +9384,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A31" s="50"/>
       <c r="B31" s="51"/>
       <c r="C31" s="51"/>
@@ -9365,7 +9393,7 @@
       </c>
       <c r="E31" s="52"/>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A32" s="53"/>
       <c r="B32" s="54" t="s">
         <v>582</v>
@@ -9380,7 +9408,7 @@
         <v>585</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A33" s="53"/>
       <c r="B33" s="54"/>
       <c r="C33" s="54"/>
@@ -9389,7 +9417,7 @@
       </c>
       <c r="E33" s="55"/>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A34" s="50"/>
       <c r="B34" s="51" t="s">
         <v>587</v>
@@ -9404,7 +9432,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A35" s="50"/>
       <c r="B35" s="51"/>
       <c r="C35" s="51"/>
@@ -9413,7 +9441,7 @@
       </c>
       <c r="E35" s="52"/>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A36" s="16"/>
       <c r="B36" s="17" t="s">
         <v>592</v>
@@ -9428,7 +9456,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A37" s="50"/>
       <c r="B37" s="51" t="s">
         <v>594</v>
@@ -9443,7 +9471,7 @@
         <v>597</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A38" s="50"/>
       <c r="B38" s="51"/>
       <c r="C38" s="51"/>
@@ -9452,7 +9480,7 @@
       </c>
       <c r="E38" s="52"/>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A39" s="50"/>
       <c r="B39" s="51"/>
       <c r="C39" s="51"/>
@@ -9461,7 +9489,7 @@
       </c>
       <c r="E39" s="52"/>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A40" s="50"/>
       <c r="B40" s="51"/>
       <c r="C40" s="51"/>
@@ -9470,7 +9498,7 @@
       </c>
       <c r="E40" s="52"/>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A41" s="50"/>
       <c r="B41" s="51"/>
       <c r="C41" s="51"/>
@@ -9479,7 +9507,7 @@
       </c>
       <c r="E41" s="52"/>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A42" s="50"/>
       <c r="B42" s="51"/>
       <c r="C42" s="51"/>
@@ -9488,7 +9516,7 @@
       </c>
       <c r="E42" s="52"/>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A43" s="50"/>
       <c r="B43" s="51"/>
       <c r="C43" s="51"/>
@@ -9497,7 +9525,7 @@
       </c>
       <c r="E43" s="52"/>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A44" s="50"/>
       <c r="B44" s="51"/>
       <c r="C44" s="51"/>
@@ -9506,7 +9534,7 @@
       </c>
       <c r="E44" s="52"/>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A45" s="50"/>
       <c r="B45" s="51"/>
       <c r="C45" s="51"/>
@@ -9515,7 +9543,7 @@
       </c>
       <c r="E45" s="52"/>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A46" s="50"/>
       <c r="B46" s="51"/>
       <c r="C46" s="51"/>
@@ -9524,14 +9552,14 @@
       </c>
       <c r="E46" s="52"/>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A47" s="50"/>
       <c r="B47" s="51"/>
       <c r="C47" s="51"/>
       <c r="D47" s="3"/>
       <c r="E47" s="52"/>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A48" s="50"/>
       <c r="B48" s="51"/>
       <c r="C48" s="51"/>
@@ -9540,7 +9568,7 @@
       </c>
       <c r="E48" s="52"/>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A49" s="50"/>
       <c r="B49" s="51"/>
       <c r="C49" s="51"/>
@@ -9549,7 +9577,7 @@
       </c>
       <c r="E49" s="52"/>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A50" s="50"/>
       <c r="B50" s="51"/>
       <c r="C50" s="51"/>
@@ -9558,7 +9586,7 @@
       </c>
       <c r="E50" s="52"/>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A51" s="50"/>
       <c r="B51" s="51"/>
       <c r="C51" s="51"/>
@@ -9567,7 +9595,7 @@
       </c>
       <c r="E51" s="52"/>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A52" s="50"/>
       <c r="B52" s="51"/>
       <c r="C52" s="51"/>
@@ -9576,7 +9604,7 @@
       </c>
       <c r="E52" s="52"/>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A53" s="50"/>
       <c r="B53" s="51"/>
       <c r="C53" s="51"/>
@@ -9585,7 +9613,7 @@
       </c>
       <c r="E53" s="52"/>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A54" s="50"/>
       <c r="B54" s="51"/>
       <c r="C54" s="51"/>
@@ -9594,7 +9622,7 @@
       </c>
       <c r="E54" s="52"/>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A55" s="50"/>
       <c r="B55" s="51"/>
       <c r="C55" s="51"/>
@@ -9603,7 +9631,7 @@
       </c>
       <c r="E55" s="52"/>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A56" s="50"/>
       <c r="B56" s="51"/>
       <c r="C56" s="51"/>
@@ -9612,14 +9640,14 @@
       </c>
       <c r="E56" s="52"/>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A57" s="50"/>
       <c r="B57" s="51"/>
       <c r="C57" s="51"/>
       <c r="D57" s="3"/>
       <c r="E57" s="52"/>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A58" s="50"/>
       <c r="B58" s="51"/>
       <c r="C58" s="51"/>
@@ -9628,7 +9656,7 @@
       </c>
       <c r="E58" s="52"/>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A59" s="50"/>
       <c r="B59" s="51"/>
       <c r="C59" s="51"/>
@@ -9637,7 +9665,7 @@
       </c>
       <c r="E59" s="52"/>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A60" s="50"/>
       <c r="B60" s="51"/>
       <c r="C60" s="51"/>
@@ -9646,7 +9674,7 @@
       </c>
       <c r="E60" s="52"/>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A61" s="50"/>
       <c r="B61" s="51"/>
       <c r="C61" s="51"/>
@@ -9655,7 +9683,7 @@
       </c>
       <c r="E61" s="52"/>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A62" s="50"/>
       <c r="B62" s="51"/>
       <c r="C62" s="51"/>
@@ -9664,7 +9692,7 @@
       </c>
       <c r="E62" s="52"/>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A63" s="50"/>
       <c r="B63" s="51"/>
       <c r="C63" s="51"/>
@@ -9673,7 +9701,7 @@
       </c>
       <c r="E63" s="52"/>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A64" s="50"/>
       <c r="B64" s="51"/>
       <c r="C64" s="51"/>
@@ -9682,7 +9710,7 @@
       </c>
       <c r="E64" s="52"/>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A65" s="53"/>
       <c r="B65" s="54" t="s">
         <v>240</v>
@@ -9697,14 +9725,14 @@
         <v>547</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A66" s="53"/>
       <c r="B66" s="54"/>
       <c r="C66" s="54"/>
       <c r="D66" s="22"/>
       <c r="E66" s="55"/>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A67" s="53"/>
       <c r="B67" s="54"/>
       <c r="C67" s="54"/>
@@ -9713,7 +9741,7 @@
       </c>
       <c r="E67" s="55"/>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A68" s="53"/>
       <c r="B68" s="54"/>
       <c r="C68" s="54"/>
@@ -9722,7 +9750,7 @@
       </c>
       <c r="E68" s="55"/>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A69" s="53"/>
       <c r="B69" s="54"/>
       <c r="C69" s="54"/>
@@ -9731,7 +9759,7 @@
       </c>
       <c r="E69" s="55"/>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A70" s="53"/>
       <c r="B70" s="54"/>
       <c r="C70" s="54"/>
@@ -9740,7 +9768,7 @@
       </c>
       <c r="E70" s="55"/>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A71" s="53"/>
       <c r="B71" s="54"/>
       <c r="C71" s="54"/>
@@ -9749,7 +9777,7 @@
       </c>
       <c r="E71" s="55"/>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A72" s="53"/>
       <c r="B72" s="54"/>
       <c r="C72" s="54"/>
@@ -9758,7 +9786,7 @@
       </c>
       <c r="E72" s="55"/>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A73" s="53"/>
       <c r="B73" s="54"/>
       <c r="C73" s="54"/>
@@ -9767,7 +9795,7 @@
       </c>
       <c r="E73" s="55"/>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A74" s="53"/>
       <c r="B74" s="54"/>
       <c r="C74" s="54"/>
@@ -9776,7 +9804,7 @@
       </c>
       <c r="E74" s="55"/>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A75" s="53"/>
       <c r="B75" s="54"/>
       <c r="C75" s="54"/>
@@ -9785,7 +9813,7 @@
       </c>
       <c r="E75" s="55"/>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A76" s="53"/>
       <c r="B76" s="54"/>
       <c r="C76" s="54"/>
@@ -9794,7 +9822,7 @@
       </c>
       <c r="E76" s="55"/>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A77" s="53"/>
       <c r="B77" s="54"/>
       <c r="C77" s="54"/>
@@ -9803,7 +9831,7 @@
       </c>
       <c r="E77" s="55"/>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A78" s="53"/>
       <c r="B78" s="54"/>
       <c r="C78" s="54"/>
@@ -9812,7 +9840,7 @@
       </c>
       <c r="E78" s="55"/>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A79" s="53"/>
       <c r="B79" s="54"/>
       <c r="C79" s="54"/>
@@ -9821,7 +9849,7 @@
       </c>
       <c r="E79" s="55"/>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A80" s="50"/>
       <c r="B80" s="51" t="s">
         <v>237</v>
@@ -9836,14 +9864,14 @@
         <v>547</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A81" s="50"/>
       <c r="B81" s="51"/>
       <c r="C81" s="51"/>
       <c r="D81" s="3"/>
       <c r="E81" s="52"/>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A82" s="50"/>
       <c r="B82" s="51"/>
       <c r="C82" s="51"/>
@@ -9852,7 +9880,7 @@
       </c>
       <c r="E82" s="52"/>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A83" s="50"/>
       <c r="B83" s="51"/>
       <c r="C83" s="51"/>
@@ -9861,7 +9889,7 @@
       </c>
       <c r="E83" s="52"/>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A84" s="50"/>
       <c r="B84" s="51"/>
       <c r="C84" s="51"/>
@@ -9870,7 +9898,7 @@
       </c>
       <c r="E84" s="52"/>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A85" s="50"/>
       <c r="B85" s="51"/>
       <c r="C85" s="51"/>
@@ -9879,7 +9907,7 @@
       </c>
       <c r="E85" s="52"/>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A86" s="50"/>
       <c r="B86" s="51"/>
       <c r="C86" s="51"/>
@@ -9888,7 +9916,7 @@
       </c>
       <c r="E86" s="52"/>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A87" s="50"/>
       <c r="B87" s="51"/>
       <c r="C87" s="51"/>
@@ -9897,7 +9925,7 @@
       </c>
       <c r="E87" s="52"/>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A88" s="50"/>
       <c r="B88" s="51"/>
       <c r="C88" s="51"/>
@@ -9906,7 +9934,7 @@
       </c>
       <c r="E88" s="52"/>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A89" s="50"/>
       <c r="B89" s="51"/>
       <c r="C89" s="51"/>
@@ -9915,7 +9943,7 @@
       </c>
       <c r="E89" s="52"/>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A90" s="50"/>
       <c r="B90" s="51"/>
       <c r="C90" s="51"/>
@@ -9924,7 +9952,7 @@
       </c>
       <c r="E90" s="52"/>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A91" s="50"/>
       <c r="B91" s="51"/>
       <c r="C91" s="51"/>
@@ -9933,7 +9961,7 @@
       </c>
       <c r="E91" s="52"/>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A92" s="50"/>
       <c r="B92" s="51"/>
       <c r="C92" s="51"/>
@@ -9942,7 +9970,7 @@
       </c>
       <c r="E92" s="52"/>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A93" s="50"/>
       <c r="B93" s="51"/>
       <c r="C93" s="51"/>
@@ -9951,7 +9979,7 @@
       </c>
       <c r="E93" s="52"/>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A94" s="50"/>
       <c r="B94" s="51"/>
       <c r="C94" s="51"/>
@@ -9960,7 +9988,7 @@
       </c>
       <c r="E94" s="52"/>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A95" s="16"/>
       <c r="B95" s="17" t="s">
         <v>632</v>
@@ -9975,7 +10003,7 @@
         <v>547</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A96" s="19"/>
       <c r="B96" s="20" t="s">
         <v>77</v>
@@ -9990,7 +10018,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A97" s="16"/>
       <c r="B97" s="17" t="s">
         <v>636</v>
@@ -10005,7 +10033,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="98" spans="1:5" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:5" ht="13" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A98" s="50"/>
       <c r="B98" s="51" t="s">
         <v>124</v>
@@ -10020,7 +10048,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A99" s="50"/>
       <c r="B99" s="51"/>
       <c r="C99" s="51"/>
@@ -10029,7 +10057,7 @@
       </c>
       <c r="E99" s="52"/>
     </row>
-    <row r="100" spans="1:5" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:5" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A100" s="53"/>
       <c r="B100" s="54" t="s">
         <v>491</v>
@@ -10044,7 +10072,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A101" s="53"/>
       <c r="B101" s="54"/>
       <c r="C101" s="54"/>
@@ -10053,7 +10081,7 @@
       </c>
       <c r="E101" s="55"/>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A102" s="19"/>
       <c r="B102" s="20" t="s">
         <v>487</v>
@@ -10068,7 +10096,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="103" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:5" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A103" s="53"/>
       <c r="B103" s="54" t="s">
         <v>645</v>
@@ -10083,7 +10111,7 @@
         <v>547</v>
       </c>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A104" s="53"/>
       <c r="B104" s="54"/>
       <c r="C104" s="54"/>
@@ -10092,7 +10120,7 @@
       </c>
       <c r="E104" s="55"/>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A105" s="19"/>
       <c r="B105" s="20" t="s">
         <v>649</v>
@@ -10107,7 +10135,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A106" s="16"/>
       <c r="B106" s="17" t="s">
         <v>651</v>
@@ -10122,7 +10150,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A107" s="19"/>
       <c r="B107" s="20" t="s">
         <v>653</v>
@@ -10137,7 +10165,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A108" s="16"/>
       <c r="B108" s="17" t="s">
         <v>656</v>
@@ -10152,7 +10180,7 @@
         <v>547</v>
       </c>
     </row>
-    <row r="109" spans="1:5" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:5" ht="12.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A109" s="50"/>
       <c r="B109" s="51" t="s">
         <v>658</v>
@@ -10167,7 +10195,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="110" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A110" s="50"/>
       <c r="B110" s="51"/>
       <c r="C110" s="51"/>
@@ -10176,7 +10204,7 @@
       </c>
       <c r="E110" s="52"/>
     </row>
-    <row r="111" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A111" s="23"/>
       <c r="B111" s="24" t="s">
         <v>128</v>
@@ -10191,13 +10219,65 @@
         <v>663</v>
       </c>
     </row>
-    <row r="112" spans="1:5" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="113" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="114" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="115" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="116" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="112" spans="1:5" hidden="1" x14ac:dyDescent="0.35"/>
+    <row r="113" hidden="1" x14ac:dyDescent="0.35"/>
+    <row r="114" hidden="1" x14ac:dyDescent="0.35"/>
+    <row r="115" hidden="1" x14ac:dyDescent="0.35"/>
+    <row r="116" hidden="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <mergeCells count="64">
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="A6:A8"/>
+    <mergeCell ref="B6:B8"/>
+    <mergeCell ref="C6:C8"/>
+    <mergeCell ref="E6:E8"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="A24:A25"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="E24:E25"/>
+    <mergeCell ref="A26:A27"/>
+    <mergeCell ref="B26:B27"/>
+    <mergeCell ref="C26:C27"/>
+    <mergeCell ref="E26:E27"/>
+    <mergeCell ref="A28:A29"/>
+    <mergeCell ref="B28:B29"/>
+    <mergeCell ref="C28:C29"/>
+    <mergeCell ref="E28:E29"/>
+    <mergeCell ref="A30:A31"/>
+    <mergeCell ref="B30:B31"/>
+    <mergeCell ref="C30:C31"/>
+    <mergeCell ref="E30:E31"/>
+    <mergeCell ref="A32:A33"/>
+    <mergeCell ref="B32:B33"/>
+    <mergeCell ref="C32:C33"/>
+    <mergeCell ref="E32:E33"/>
+    <mergeCell ref="A34:A35"/>
+    <mergeCell ref="B34:B35"/>
+    <mergeCell ref="C34:C35"/>
+    <mergeCell ref="E34:E35"/>
+    <mergeCell ref="A37:A64"/>
+    <mergeCell ref="B37:B64"/>
+    <mergeCell ref="C37:C64"/>
+    <mergeCell ref="E37:E64"/>
+    <mergeCell ref="A65:A79"/>
+    <mergeCell ref="B65:B79"/>
+    <mergeCell ref="C65:C79"/>
+    <mergeCell ref="E65:E79"/>
+    <mergeCell ref="A80:A94"/>
+    <mergeCell ref="B80:B94"/>
+    <mergeCell ref="C80:C94"/>
+    <mergeCell ref="E80:E94"/>
+    <mergeCell ref="A98:A99"/>
+    <mergeCell ref="B98:B99"/>
+    <mergeCell ref="C98:C99"/>
+    <mergeCell ref="E98:E99"/>
     <mergeCell ref="A109:A110"/>
     <mergeCell ref="B109:B110"/>
     <mergeCell ref="C109:C110"/>
@@ -10210,106 +10290,12 @@
     <mergeCell ref="B103:B104"/>
     <mergeCell ref="C103:C104"/>
     <mergeCell ref="E103:E104"/>
-    <mergeCell ref="A80:A94"/>
-    <mergeCell ref="B80:B94"/>
-    <mergeCell ref="C80:C94"/>
-    <mergeCell ref="E80:E94"/>
-    <mergeCell ref="A98:A99"/>
-    <mergeCell ref="B98:B99"/>
-    <mergeCell ref="C98:C99"/>
-    <mergeCell ref="E98:E99"/>
-    <mergeCell ref="A37:A64"/>
-    <mergeCell ref="B37:B64"/>
-    <mergeCell ref="C37:C64"/>
-    <mergeCell ref="E37:E64"/>
-    <mergeCell ref="A65:A79"/>
-    <mergeCell ref="B65:B79"/>
-    <mergeCell ref="C65:C79"/>
-    <mergeCell ref="E65:E79"/>
-    <mergeCell ref="A32:A33"/>
-    <mergeCell ref="B32:B33"/>
-    <mergeCell ref="C32:C33"/>
-    <mergeCell ref="E32:E33"/>
-    <mergeCell ref="A34:A35"/>
-    <mergeCell ref="B34:B35"/>
-    <mergeCell ref="C34:C35"/>
-    <mergeCell ref="E34:E35"/>
-    <mergeCell ref="A28:A29"/>
-    <mergeCell ref="B28:B29"/>
-    <mergeCell ref="C28:C29"/>
-    <mergeCell ref="E28:E29"/>
-    <mergeCell ref="A30:A31"/>
-    <mergeCell ref="B30:B31"/>
-    <mergeCell ref="C30:C31"/>
-    <mergeCell ref="E30:E31"/>
-    <mergeCell ref="A24:A25"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="C24:C25"/>
-    <mergeCell ref="E24:E25"/>
-    <mergeCell ref="A26:A27"/>
-    <mergeCell ref="B26:B27"/>
-    <mergeCell ref="C26:C27"/>
-    <mergeCell ref="E26:E27"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="A6:A8"/>
-    <mergeCell ref="B6:B8"/>
-    <mergeCell ref="C6:C8"/>
-    <mergeCell ref="E6:E8"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="E10:E11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="cea7764e-6bf9-427d-be15-e74097e0a61c">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <SharedWithUsers xmlns="fb9ea31f-0ab8-44ff-80d1-5777f6d9d945">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-    <MediaLengthInSeconds xmlns="cea7764e-6bf9-427d-be15-e74097e0a61c" xsi:nil="true"/>
-    <Sign_x002d_off_x0020_status xmlns="cea7764e-6bf9-427d-be15-e74097e0a61c" xsi:nil="true"/>
-    <Title_x0020_URL xmlns="cea7764e-6bf9-427d-be15-e74097e0a61c">
-      <Url xsi:nil="true"/>
-      <Description xsi:nil="true"/>
-    </Title_x0020_URL>
-    <Mail_x0020_Sent xmlns="cea7764e-6bf9-427d-be15-e74097e0a61c">false</Mail_x0020_Sent>
-    <_Flow_SignoffStatus xmlns="cea7764e-6bf9-427d-be15-e74097e0a61c" xsi:nil="true"/>
-    <State xmlns="cea7764e-6bf9-427d-be15-e74097e0a61c">Open</State>
-    <Comments xmlns="cea7764e-6bf9-427d-be15-e74097e0a61c" xsi:nil="true"/>
-    <Lead_x0020_Signoff xmlns="cea7764e-6bf9-427d-be15-e74097e0a61c">false</Lead_x0020_Signoff>
-    <Title_x0020_ID xmlns="cea7764e-6bf9-427d-be15-e74097e0a61c" xsi:nil="true"/>
-    <TranslatedLang xmlns="cea7764e-6bf9-427d-be15-e74097e0a61c" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010039A62E282DDA434E979CD3E03185182E" ma:contentTypeVersion="33" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="a6c69cf93bfe1fca5d0e373365e7fdfc">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="cea7764e-6bf9-427d-be15-e74097e0a61c" xmlns:ns3="fb9ea31f-0ab8-44ff-80d1-5777f6d9d945" xmlns:ns4="230e9df3-be65-4c73-a93b-d1236ebd677e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="62cb4c6faf5eab163d0c8ea23c8ff408" ns1:_="" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -10651,34 +10637,49 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E53D8182-34C2-4EE5-8FD0-D750C3EB0900}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="fb9ea31f-0ab8-44ff-80d1-5777f6d9d945"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
-    <ds:schemaRef ds:uri="cea7764e-6bf9-427d-be15-e74097e0a61c"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3F377113-5718-41B1-A1CE-B96F830D3573}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="cea7764e-6bf9-427d-be15-e74097e0a61c">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <SharedWithUsers xmlns="fb9ea31f-0ab8-44ff-80d1-5777f6d9d945">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+    <MediaLengthInSeconds xmlns="cea7764e-6bf9-427d-be15-e74097e0a61c" xsi:nil="true"/>
+    <Sign_x002d_off_x0020_status xmlns="cea7764e-6bf9-427d-be15-e74097e0a61c" xsi:nil="true"/>
+    <Title_x0020_URL xmlns="cea7764e-6bf9-427d-be15-e74097e0a61c">
+      <Url xsi:nil="true"/>
+      <Description xsi:nil="true"/>
+    </Title_x0020_URL>
+    <Mail_x0020_Sent xmlns="cea7764e-6bf9-427d-be15-e74097e0a61c">false</Mail_x0020_Sent>
+    <_Flow_SignoffStatus xmlns="cea7764e-6bf9-427d-be15-e74097e0a61c" xsi:nil="true"/>
+    <State xmlns="cea7764e-6bf9-427d-be15-e74097e0a61c">Open</State>
+    <Comments xmlns="cea7764e-6bf9-427d-be15-e74097e0a61c" xsi:nil="true"/>
+    <Lead_x0020_Signoff xmlns="cea7764e-6bf9-427d-be15-e74097e0a61c">false</Lead_x0020_Signoff>
+    <Title_x0020_ID xmlns="cea7764e-6bf9-427d-be15-e74097e0a61c" xsi:nil="true"/>
+    <TranslatedLang xmlns="cea7764e-6bf9-427d-be15-e74097e0a61c" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{23B9621B-458A-4676-8042-F53348150B3A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -10699,6 +10700,33 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3F377113-5718-41B1-A1CE-B96F830D3573}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E53D8182-34C2-4EE5-8FD0-D750C3EB0900}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="fb9ea31f-0ab8-44ff-80d1-5777f6d9d945"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
+    <ds:schemaRef ds:uri="cea7764e-6bf9-427d-be15-e74097e0a61c"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{87867195-f2b8-4ac2-b0b6-6bb73cb33afc}" enabled="1" method="Privileged" siteId="{72f988bf-86f1-41af-91ab-2d7cd011db47}" contentBits="0" removed="0"/>

</xml_diff>

<commit_message>
docs: github fine grained token
</commit_message>
<xml_diff>
--- a/docs/static/examples/tf/accelerator/config/checklist.xlsx
+++ b/docs/static/examples/tf/accelerator/config/checklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jaredholgate\Code\azure-landing-zones\docs\static\examples\tf\accelerator\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E572CE07-DCF0-44EF-A0F8-300B49B72DEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45CFA1FB-225C-46AB-9470-C6E08B523B56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" tabRatio="415" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1171" uniqueCount="650">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1177" uniqueCount="654">
   <si>
     <t>Description</t>
   </si>
@@ -2123,6 +2123,18 @@
   </si>
   <si>
     <t>The subscription id for the security subscription</t>
+  </si>
+  <si>
+    <t>Zero Trust Security</t>
+  </si>
+  <si>
+    <t>Do you want to configure Zero Trust Security?</t>
+  </si>
+  <si>
+    <t>Sovereign Landing Zone</t>
+  </si>
+  <si>
+    <t>Do you want to configure Sovereign Landing Zone controls?</t>
   </si>
 </sst>
 </file>
@@ -2339,7 +2351,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -2450,6 +2462,9 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -7876,7 +7891,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE440EAA-007A-486E-B4E3-7FE7599AA545}">
-  <dimension ref="A1:G29"/>
+  <dimension ref="A1:G31"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
@@ -8324,13 +8339,47 @@
       <c r="F28" s="28"/>
       <c r="G28" s="22"/>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="B29" s="24"/>
-      <c r="C29" s="25"/>
-      <c r="D29" s="24"/>
-      <c r="E29" s="25"/>
-      <c r="F29" s="24"/>
-      <c r="G29" s="24"/>
+    <row r="29" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A29" s="31">
+        <v>14</v>
+      </c>
+      <c r="B29" s="22" t="s">
+        <v>650</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>651</v>
+      </c>
+      <c r="D29" s="22"/>
+      <c r="E29" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F29" s="39"/>
+      <c r="G29" s="22"/>
+    </row>
+    <row r="30" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A30" s="31">
+        <v>15</v>
+      </c>
+      <c r="B30" s="22" t="s">
+        <v>652</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>653</v>
+      </c>
+      <c r="D30" s="22"/>
+      <c r="E30" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F30" s="39"/>
+      <c r="G30" s="22"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B31" s="24"/>
+      <c r="C31" s="25"/>
+      <c r="D31" s="24"/>
+      <c r="E31" s="25"/>
+      <c r="F31" s="24"/>
+      <c r="G31" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -8375,15 +8424,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010039A62E282DDA434E979CD3E03185182E" ma:contentTypeVersion="33" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="a6c69cf93bfe1fca5d0e373365e7fdfc">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="cea7764e-6bf9-427d-be15-e74097e0a61c" xmlns:ns3="fb9ea31f-0ab8-44ff-80d1-5777f6d9d945" xmlns:ns4="230e9df3-be65-4c73-a93b-d1236ebd677e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="62cb4c6faf5eab163d0c8ea23c8ff408" ns1:_="" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -8725,6 +8765,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E53D8182-34C2-4EE5-8FD0-D750C3EB0900}">
   <ds:schemaRefs>
@@ -8745,14 +8794,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3F377113-5718-41B1-A1CE-B96F830D3573}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{23B9621B-458A-4676-8042-F53348150B3A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -8773,6 +8814,14 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3F377113-5718-41B1-A1CE-B96F830D3573}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{87867195-f2b8-4ac2-b0b6-6bb73cb33afc}" enabled="1" method="Privileged" siteId="{72f988bf-86f1-41af-91ab-2d7cd011db47}" contentBits="0" removed="0"/>

</xml_diff>

<commit_message>
docs: github fine grained token (#149)
* docs: github fine grained token

* fix required permissions

* fix expiration date
</commit_message>
<xml_diff>
--- a/docs/static/examples/tf/accelerator/config/checklist.xlsx
+++ b/docs/static/examples/tf/accelerator/config/checklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jaredholgate\Code\azure-landing-zones\docs\static\examples\tf\accelerator\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E572CE07-DCF0-44EF-A0F8-300B49B72DEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45CFA1FB-225C-46AB-9470-C6E08B523B56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" tabRatio="415" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1171" uniqueCount="650">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1177" uniqueCount="654">
   <si>
     <t>Description</t>
   </si>
@@ -2123,6 +2123,18 @@
   </si>
   <si>
     <t>The subscription id for the security subscription</t>
+  </si>
+  <si>
+    <t>Zero Trust Security</t>
+  </si>
+  <si>
+    <t>Do you want to configure Zero Trust Security?</t>
+  </si>
+  <si>
+    <t>Sovereign Landing Zone</t>
+  </si>
+  <si>
+    <t>Do you want to configure Sovereign Landing Zone controls?</t>
   </si>
 </sst>
 </file>
@@ -2339,7 +2351,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -2450,6 +2462,9 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -7876,7 +7891,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE440EAA-007A-486E-B4E3-7FE7599AA545}">
-  <dimension ref="A1:G29"/>
+  <dimension ref="A1:G31"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
@@ -8324,13 +8339,47 @@
       <c r="F28" s="28"/>
       <c r="G28" s="22"/>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="B29" s="24"/>
-      <c r="C29" s="25"/>
-      <c r="D29" s="24"/>
-      <c r="E29" s="25"/>
-      <c r="F29" s="24"/>
-      <c r="G29" s="24"/>
+    <row r="29" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A29" s="31">
+        <v>14</v>
+      </c>
+      <c r="B29" s="22" t="s">
+        <v>650</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>651</v>
+      </c>
+      <c r="D29" s="22"/>
+      <c r="E29" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F29" s="39"/>
+      <c r="G29" s="22"/>
+    </row>
+    <row r="30" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A30" s="31">
+        <v>15</v>
+      </c>
+      <c r="B30" s="22" t="s">
+        <v>652</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>653</v>
+      </c>
+      <c r="D30" s="22"/>
+      <c r="E30" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F30" s="39"/>
+      <c r="G30" s="22"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B31" s="24"/>
+      <c r="C31" s="25"/>
+      <c r="D31" s="24"/>
+      <c r="E31" s="25"/>
+      <c r="F31" s="24"/>
+      <c r="G31" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -8375,15 +8424,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010039A62E282DDA434E979CD3E03185182E" ma:contentTypeVersion="33" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="a6c69cf93bfe1fca5d0e373365e7fdfc">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="cea7764e-6bf9-427d-be15-e74097e0a61c" xmlns:ns3="fb9ea31f-0ab8-44ff-80d1-5777f6d9d945" xmlns:ns4="230e9df3-be65-4c73-a93b-d1236ebd677e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="62cb4c6faf5eab163d0c8ea23c8ff408" ns1:_="" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -8725,6 +8765,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E53D8182-34C2-4EE5-8FD0-D750C3EB0900}">
   <ds:schemaRefs>
@@ -8745,14 +8794,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3F377113-5718-41B1-A1CE-B96F830D3573}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{23B9621B-458A-4676-8042-F53348150B3A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -8773,6 +8814,14 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3F377113-5718-41B1-A1CE-B96F830D3573}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{87867195-f2b8-4ac2-b0b6-6bb73cb33afc}" enabled="1" method="Privileged" siteId="{72f988bf-86f1-41af-91ab-2d7cd011db47}" contentBits="0" removed="0"/>

</xml_diff>

<commit_message>
docs refactor and simplification
</commit_message>
<xml_diff>
--- a/docs/static/examples/tf/accelerator/config/checklist.xlsx
+++ b/docs/static/examples/tf/accelerator/config/checklist.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29530"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jaredholgate\Code\azure-landing-zones\docs\static\examples\tf\accelerator\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45CFA1FB-225C-46AB-9470-C6E08B523B56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{485682DB-19D0-41B6-A7CF-DFC0C69DD288}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" tabRatio="415" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Accelerator - Bootstrap" sheetId="13" r:id="rId1"/>
     <sheet name="Accelerator - Bicep" sheetId="5" r:id="rId2"/>
-    <sheet name="Accelerator - Terraform - ALZ" sheetId="14" r:id="rId3"/>
+    <sheet name="Accelerator - Terraform" sheetId="14" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -2457,14 +2457,14 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2839,15 +2839,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="77.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="38" t="s">
         <v>630</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
-      <c r="G1" s="37"/>
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
+      <c r="G1" s="38"/>
     </row>
     <row r="3" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="32" t="s">
@@ -7909,15 +7909,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="77.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="39" t="s">
         <v>631</v>
       </c>
-      <c r="B1" s="38"/>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="38"/>
-      <c r="G1" s="38"/>
+      <c r="B1" s="39"/>
+      <c r="C1" s="39"/>
+      <c r="D1" s="39"/>
+      <c r="E1" s="39"/>
+      <c r="F1" s="39"/>
+      <c r="G1" s="39"/>
     </row>
     <row r="3" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="29" t="s">
@@ -8353,7 +8353,7 @@
       <c r="E29" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F29" s="39"/>
+      <c r="F29" s="37"/>
       <c r="G29" s="22"/>
     </row>
     <row r="30" spans="1:7" ht="29" x14ac:dyDescent="0.35">
@@ -8370,7 +8370,7 @@
       <c r="E30" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F30" s="39"/>
+      <c r="F30" s="37"/>
       <c r="G30" s="22"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.35">
@@ -8391,36 +8391,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="cea7764e-6bf9-427d-be15-e74097e0a61c">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <SharedWithUsers xmlns="fb9ea31f-0ab8-44ff-80d1-5777f6d9d945">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-    <MediaLengthInSeconds xmlns="cea7764e-6bf9-427d-be15-e74097e0a61c" xsi:nil="true"/>
-    <Sign_x002d_off_x0020_status xmlns="cea7764e-6bf9-427d-be15-e74097e0a61c" xsi:nil="true"/>
-    <Title_x0020_URL xmlns="cea7764e-6bf9-427d-be15-e74097e0a61c">
-      <Url xsi:nil="true"/>
-      <Description xsi:nil="true"/>
-    </Title_x0020_URL>
-    <Mail_x0020_Sent xmlns="cea7764e-6bf9-427d-be15-e74097e0a61c">false</Mail_x0020_Sent>
-    <_Flow_SignoffStatus xmlns="cea7764e-6bf9-427d-be15-e74097e0a61c" xsi:nil="true"/>
-    <State xmlns="cea7764e-6bf9-427d-be15-e74097e0a61c">Open</State>
-    <Comments xmlns="cea7764e-6bf9-427d-be15-e74097e0a61c" xsi:nil="true"/>
-    <Lead_x0020_Signoff xmlns="cea7764e-6bf9-427d-be15-e74097e0a61c">false</Lead_x0020_Signoff>
-    <Title_x0020_ID xmlns="cea7764e-6bf9-427d-be15-e74097e0a61c" xsi:nil="true"/>
-    <TranslatedLang xmlns="cea7764e-6bf9-427d-be15-e74097e0a61c" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -8766,29 +8742,42 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="cea7764e-6bf9-427d-be15-e74097e0a61c">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <SharedWithUsers xmlns="fb9ea31f-0ab8-44ff-80d1-5777f6d9d945">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+    <MediaLengthInSeconds xmlns="cea7764e-6bf9-427d-be15-e74097e0a61c" xsi:nil="true"/>
+    <Sign_x002d_off_x0020_status xmlns="cea7764e-6bf9-427d-be15-e74097e0a61c" xsi:nil="true"/>
+    <Title_x0020_URL xmlns="cea7764e-6bf9-427d-be15-e74097e0a61c">
+      <Url xsi:nil="true"/>
+      <Description xsi:nil="true"/>
+    </Title_x0020_URL>
+    <Mail_x0020_Sent xmlns="cea7764e-6bf9-427d-be15-e74097e0a61c">false</Mail_x0020_Sent>
+    <_Flow_SignoffStatus xmlns="cea7764e-6bf9-427d-be15-e74097e0a61c" xsi:nil="true"/>
+    <State xmlns="cea7764e-6bf9-427d-be15-e74097e0a61c">Open</State>
+    <Comments xmlns="cea7764e-6bf9-427d-be15-e74097e0a61c" xsi:nil="true"/>
+    <Lead_x0020_Signoff xmlns="cea7764e-6bf9-427d-be15-e74097e0a61c">false</Lead_x0020_Signoff>
+    <Title_x0020_ID xmlns="cea7764e-6bf9-427d-be15-e74097e0a61c" xsi:nil="true"/>
+    <TranslatedLang xmlns="cea7764e-6bf9-427d-be15-e74097e0a61c" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E53D8182-34C2-4EE5-8FD0-D750C3EB0900}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3F377113-5718-41B1-A1CE-B96F830D3573}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="fb9ea31f-0ab8-44ff-80d1-5777f6d9d945"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
-    <ds:schemaRef ds:uri="cea7764e-6bf9-427d-be15-e74097e0a61c"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -8815,9 +8804,20 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3F377113-5718-41B1-A1CE-B96F830D3573}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E53D8182-34C2-4EE5-8FD0-D750C3EB0900}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="fb9ea31f-0ab8-44ff-80d1-5777f6d9d945"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
+    <ds:schemaRef ds:uri="cea7764e-6bf9-427d-be15-e74097e0a61c"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
docs: simplify terraform (#164)
* docs: simplify terraform

* remove redundant line

* fix

* Add bicep to bootstrap script

* docs refactor and simplification
</commit_message>
<xml_diff>
--- a/docs/static/examples/tf/accelerator/config/checklist.xlsx
+++ b/docs/static/examples/tf/accelerator/config/checklist.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29530"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jaredholgate\Code\azure-landing-zones\docs\static\examples\tf\accelerator\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45CFA1FB-225C-46AB-9470-C6E08B523B56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{485682DB-19D0-41B6-A7CF-DFC0C69DD288}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" tabRatio="415" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Accelerator - Bootstrap" sheetId="13" r:id="rId1"/>
     <sheet name="Accelerator - Bicep" sheetId="5" r:id="rId2"/>
-    <sheet name="Accelerator - Terraform - ALZ" sheetId="14" r:id="rId3"/>
+    <sheet name="Accelerator - Terraform" sheetId="14" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -2457,14 +2457,14 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2839,15 +2839,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="77.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="38" t="s">
         <v>630</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
-      <c r="G1" s="37"/>
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
+      <c r="G1" s="38"/>
     </row>
     <row r="3" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="32" t="s">
@@ -7909,15 +7909,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="77.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="39" t="s">
         <v>631</v>
       </c>
-      <c r="B1" s="38"/>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="38"/>
-      <c r="G1" s="38"/>
+      <c r="B1" s="39"/>
+      <c r="C1" s="39"/>
+      <c r="D1" s="39"/>
+      <c r="E1" s="39"/>
+      <c r="F1" s="39"/>
+      <c r="G1" s="39"/>
     </row>
     <row r="3" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="29" t="s">
@@ -8353,7 +8353,7 @@
       <c r="E29" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F29" s="39"/>
+      <c r="F29" s="37"/>
       <c r="G29" s="22"/>
     </row>
     <row r="30" spans="1:7" ht="29" x14ac:dyDescent="0.35">
@@ -8370,7 +8370,7 @@
       <c r="E30" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F30" s="39"/>
+      <c r="F30" s="37"/>
       <c r="G30" s="22"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.35">
@@ -8391,36 +8391,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="cea7764e-6bf9-427d-be15-e74097e0a61c">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <SharedWithUsers xmlns="fb9ea31f-0ab8-44ff-80d1-5777f6d9d945">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-    <MediaLengthInSeconds xmlns="cea7764e-6bf9-427d-be15-e74097e0a61c" xsi:nil="true"/>
-    <Sign_x002d_off_x0020_status xmlns="cea7764e-6bf9-427d-be15-e74097e0a61c" xsi:nil="true"/>
-    <Title_x0020_URL xmlns="cea7764e-6bf9-427d-be15-e74097e0a61c">
-      <Url xsi:nil="true"/>
-      <Description xsi:nil="true"/>
-    </Title_x0020_URL>
-    <Mail_x0020_Sent xmlns="cea7764e-6bf9-427d-be15-e74097e0a61c">false</Mail_x0020_Sent>
-    <_Flow_SignoffStatus xmlns="cea7764e-6bf9-427d-be15-e74097e0a61c" xsi:nil="true"/>
-    <State xmlns="cea7764e-6bf9-427d-be15-e74097e0a61c">Open</State>
-    <Comments xmlns="cea7764e-6bf9-427d-be15-e74097e0a61c" xsi:nil="true"/>
-    <Lead_x0020_Signoff xmlns="cea7764e-6bf9-427d-be15-e74097e0a61c">false</Lead_x0020_Signoff>
-    <Title_x0020_ID xmlns="cea7764e-6bf9-427d-be15-e74097e0a61c" xsi:nil="true"/>
-    <TranslatedLang xmlns="cea7764e-6bf9-427d-be15-e74097e0a61c" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -8766,29 +8742,42 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="cea7764e-6bf9-427d-be15-e74097e0a61c">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <SharedWithUsers xmlns="fb9ea31f-0ab8-44ff-80d1-5777f6d9d945">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+    <MediaLengthInSeconds xmlns="cea7764e-6bf9-427d-be15-e74097e0a61c" xsi:nil="true"/>
+    <Sign_x002d_off_x0020_status xmlns="cea7764e-6bf9-427d-be15-e74097e0a61c" xsi:nil="true"/>
+    <Title_x0020_URL xmlns="cea7764e-6bf9-427d-be15-e74097e0a61c">
+      <Url xsi:nil="true"/>
+      <Description xsi:nil="true"/>
+    </Title_x0020_URL>
+    <Mail_x0020_Sent xmlns="cea7764e-6bf9-427d-be15-e74097e0a61c">false</Mail_x0020_Sent>
+    <_Flow_SignoffStatus xmlns="cea7764e-6bf9-427d-be15-e74097e0a61c" xsi:nil="true"/>
+    <State xmlns="cea7764e-6bf9-427d-be15-e74097e0a61c">Open</State>
+    <Comments xmlns="cea7764e-6bf9-427d-be15-e74097e0a61c" xsi:nil="true"/>
+    <Lead_x0020_Signoff xmlns="cea7764e-6bf9-427d-be15-e74097e0a61c">false</Lead_x0020_Signoff>
+    <Title_x0020_ID xmlns="cea7764e-6bf9-427d-be15-e74097e0a61c" xsi:nil="true"/>
+    <TranslatedLang xmlns="cea7764e-6bf9-427d-be15-e74097e0a61c" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E53D8182-34C2-4EE5-8FD0-D750C3EB0900}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3F377113-5718-41B1-A1CE-B96F830D3573}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="fb9ea31f-0ab8-44ff-80d1-5777f6d9d945"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
-    <ds:schemaRef ds:uri="cea7764e-6bf9-427d-be15-e74097e0a61c"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -8815,9 +8804,20 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3F377113-5718-41B1-A1CE-B96F830D3573}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E53D8182-34C2-4EE5-8FD0-D750C3EB0900}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="fb9ea31f-0ab8-44ff-80d1-5777f6d9d945"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
+    <ds:schemaRef ds:uri="cea7764e-6bf9-427d-be15-e74097e0a61c"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Add missing checklist items
</commit_message>
<xml_diff>
--- a/docs/static/examples/tf/accelerator/config/checklist.xlsx
+++ b/docs/static/examples/tf/accelerator/config/checklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jaredholgate\Code\azure-landing-zones\docs\static\examples\tf\accelerator\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{485682DB-19D0-41B6-A7CF-DFC0C69DD288}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DC3DDED-CB9B-4E69-996C-B09E5C83B9FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" tabRatio="415" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1177" uniqueCount="654">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1183" uniqueCount="656">
   <si>
     <t>Description</t>
   </si>
@@ -2135,6 +2135,12 @@
   </si>
   <si>
     <t>Do you want to configure Sovereign Landing Zone controls?</t>
+  </si>
+  <si>
+    <t>Single-Region Hub and Spoke Virtual Network with Network Virtual Appliance (NVA)</t>
+  </si>
+  <si>
+    <t>Single-Region Virtual WAN with Network Virtual Appliance (NVA)</t>
   </si>
 </sst>
 </file>
@@ -7891,7 +7897,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE440EAA-007A-486E-B4E3-7FE7599AA545}">
-  <dimension ref="A1:G31"/>
+  <dimension ref="A1:G33"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
@@ -7966,7 +7972,7 @@
       <c r="A6" s="31">
         <v>1</v>
       </c>
-      <c r="B6" s="22" t="s">
+      <c r="B6" s="1" t="s">
         <v>596</v>
       </c>
       <c r="C6" s="1" t="s">
@@ -7983,7 +7989,7 @@
       <c r="A7" s="31">
         <v>2</v>
       </c>
-      <c r="B7" s="22" t="s">
+      <c r="B7" s="1" t="s">
         <v>597</v>
       </c>
       <c r="C7" s="1" t="s">
@@ -8000,7 +8006,7 @@
       <c r="A8" s="31">
         <v>3</v>
       </c>
-      <c r="B8" s="22" t="s">
+      <c r="B8" s="1" t="s">
         <v>600</v>
       </c>
       <c r="C8" s="1" t="s">
@@ -8017,7 +8023,7 @@
       <c r="A9" s="31">
         <v>4</v>
       </c>
-      <c r="B9" s="22" t="s">
+      <c r="B9" s="1" t="s">
         <v>602</v>
       </c>
       <c r="C9" s="1" t="s">
@@ -8034,7 +8040,7 @@
       <c r="A10" s="31">
         <v>5</v>
       </c>
-      <c r="B10" s="22" t="s">
+      <c r="B10" s="1" t="s">
         <v>608</v>
       </c>
       <c r="C10" s="1" t="s">
@@ -8051,7 +8057,7 @@
       <c r="A11" s="31">
         <v>6</v>
       </c>
-      <c r="B11" s="22" t="s">
+      <c r="B11" s="1" t="s">
         <v>604</v>
       </c>
       <c r="C11" s="1" t="s">
@@ -8068,7 +8074,7 @@
       <c r="A12" s="31">
         <v>7</v>
       </c>
-      <c r="B12" s="22" t="s">
+      <c r="B12" s="1" t="s">
         <v>606</v>
       </c>
       <c r="C12" s="1" t="s">
@@ -8081,86 +8087,86 @@
       <c r="F12" s="23"/>
       <c r="G12" s="22"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A13" s="33"/>
-      <c r="B13" s="24"/>
-      <c r="C13" s="25"/>
-      <c r="D13" s="24"/>
-      <c r="E13" s="25"/>
-      <c r="F13" s="24"/>
-      <c r="G13" s="24"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A14" s="35" t="s">
+    <row r="13" spans="1:7" ht="58" x14ac:dyDescent="0.35">
+      <c r="A13" s="31">
+        <v>8</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>654</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="D13" s="22"/>
+      <c r="E13" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F13" s="23"/>
+      <c r="G13" s="22"/>
+    </row>
+    <row r="14" spans="1:7" ht="58" x14ac:dyDescent="0.35">
+      <c r="A14" s="31">
+        <v>9</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>655</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>603</v>
+      </c>
+      <c r="D14" s="22"/>
+      <c r="E14" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F14" s="23"/>
+      <c r="G14" s="22"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A15" s="33"/>
+      <c r="B15" s="24"/>
+      <c r="C15" s="25"/>
+      <c r="D15" s="24"/>
+      <c r="E15" s="25"/>
+      <c r="F15" s="24"/>
+      <c r="G15" s="24"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A16" s="35" t="s">
         <v>624</v>
       </c>
-      <c r="B14" s="27"/>
-      <c r="C14" s="25"/>
-      <c r="D14" s="24"/>
-      <c r="E14" s="25"/>
-      <c r="F14" s="24"/>
-      <c r="G14" s="24"/>
-    </row>
-    <row r="15" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A15" s="31">
-        <v>1</v>
-      </c>
-      <c r="B15" s="22" t="s">
-        <v>615</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>610</v>
-      </c>
-      <c r="D15" s="22"/>
-      <c r="E15" s="1" t="s">
-        <v>622</v>
-      </c>
-      <c r="F15" s="23"/>
-      <c r="G15" s="22"/>
-    </row>
-    <row r="16" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A16" s="31">
-        <v>2</v>
-      </c>
-      <c r="B16" s="22" t="s">
-        <v>614</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>621</v>
-      </c>
-      <c r="D16" s="22"/>
-      <c r="E16" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F16" s="23"/>
-      <c r="G16" s="22"/>
+      <c r="B16" s="27"/>
+      <c r="C16" s="25"/>
+      <c r="D16" s="24"/>
+      <c r="E16" s="25"/>
+      <c r="F16" s="24"/>
+      <c r="G16" s="24"/>
     </row>
     <row r="17" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A17" s="31">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B17" s="22" t="s">
-        <v>611</v>
+        <v>615</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>617</v>
+        <v>610</v>
       </c>
       <c r="D17" s="22"/>
       <c r="E17" s="1" t="s">
-        <v>5</v>
+        <v>622</v>
       </c>
       <c r="F17" s="23"/>
       <c r="G17" s="22"/>
     </row>
     <row r="18" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A18" s="31">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B18" s="22" t="s">
-        <v>613</v>
+        <v>614</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>620</v>
+        <v>621</v>
       </c>
       <c r="D18" s="22"/>
       <c r="E18" s="1" t="s">
@@ -8171,30 +8177,30 @@
     </row>
     <row r="19" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A19" s="31">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B19" s="22" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>616</v>
+        <v>617</v>
       </c>
       <c r="D19" s="22"/>
       <c r="E19" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F19" s="28"/>
+      <c r="F19" s="23"/>
       <c r="G19" s="22"/>
     </row>
     <row r="20" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A20" s="31">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B20" s="22" t="s">
-        <v>3</v>
+        <v>613</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>618</v>
+        <v>620</v>
       </c>
       <c r="D20" s="22"/>
       <c r="E20" s="1" t="s">
@@ -8205,132 +8211,132 @@
     </row>
     <row r="21" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A21" s="31">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B21" s="22" t="s">
-        <v>4</v>
+        <v>612</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>619</v>
+        <v>616</v>
       </c>
       <c r="D21" s="22"/>
       <c r="E21" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F21" s="23"/>
+      <c r="F21" s="28"/>
       <c r="G21" s="22"/>
     </row>
     <row r="22" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A22" s="31">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B22" s="22" t="s">
-        <v>625</v>
+        <v>3</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>626</v>
+        <v>618</v>
       </c>
       <c r="D22" s="22"/>
       <c r="E22" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F22" s="28"/>
+      <c r="F22" s="23"/>
       <c r="G22" s="22"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A23" s="31">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B23" s="22" t="s">
-        <v>627</v>
+        <v>4</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>628</v>
+        <v>619</v>
       </c>
       <c r="D23" s="22"/>
       <c r="E23" s="1" t="s">
-        <v>629</v>
-      </c>
-      <c r="F23" s="28"/>
+        <v>5</v>
+      </c>
+      <c r="F23" s="23"/>
       <c r="G23" s="22"/>
     </row>
     <row r="24" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A24" s="31">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B24" s="22" t="s">
-        <v>640</v>
+        <v>625</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>639</v>
+        <v>626</v>
       </c>
       <c r="D24" s="22"/>
       <c r="E24" s="1" t="s">
-        <v>638</v>
-      </c>
-      <c r="F24" s="23"/>
+        <v>5</v>
+      </c>
+      <c r="F24" s="28"/>
       <c r="G24" s="22"/>
     </row>
-    <row r="25" spans="1:7" ht="58" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A25" s="31">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B25" s="22" t="s">
-        <v>634</v>
+        <v>627</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>637</v>
+        <v>628</v>
       </c>
       <c r="D25" s="22"/>
       <c r="E25" s="1" t="s">
-        <v>638</v>
+        <v>629</v>
       </c>
       <c r="F25" s="28"/>
       <c r="G25" s="22"/>
     </row>
     <row r="26" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A26" s="31">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B26" s="22" t="s">
-        <v>635</v>
+        <v>640</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>636</v>
+        <v>639</v>
       </c>
       <c r="D26" s="22"/>
       <c r="E26" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F26" s="28"/>
+        <v>638</v>
+      </c>
+      <c r="F26" s="23"/>
       <c r="G26" s="22"/>
     </row>
-    <row r="27" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:7" ht="58" x14ac:dyDescent="0.35">
       <c r="A27" s="31">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B27" s="22" t="s">
-        <v>642</v>
+        <v>634</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>643</v>
+        <v>637</v>
       </c>
       <c r="D27" s="22"/>
       <c r="E27" s="1" t="s">
-        <v>5</v>
+        <v>638</v>
       </c>
       <c r="F27" s="28"/>
       <c r="G27" s="22"/>
     </row>
     <row r="28" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A28" s="31">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B28" s="22" t="s">
-        <v>644</v>
+        <v>635</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>645</v>
+        <v>636</v>
       </c>
       <c r="D28" s="22"/>
       <c r="E28" s="1" t="s">
@@ -8341,45 +8347,79 @@
     </row>
     <row r="29" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A29" s="31">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B29" s="22" t="s">
-        <v>650</v>
+        <v>642</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>651</v>
+        <v>643</v>
       </c>
       <c r="D29" s="22"/>
       <c r="E29" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F29" s="37"/>
+      <c r="F29" s="28"/>
       <c r="G29" s="22"/>
     </row>
     <row r="30" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A30" s="31">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B30" s="22" t="s">
-        <v>652</v>
+        <v>644</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>653</v>
+        <v>645</v>
       </c>
       <c r="D30" s="22"/>
       <c r="E30" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F30" s="37"/>
+      <c r="F30" s="28"/>
       <c r="G30" s="22"/>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="B31" s="24"/>
-      <c r="C31" s="25"/>
-      <c r="D31" s="24"/>
-      <c r="E31" s="25"/>
-      <c r="F31" s="24"/>
-      <c r="G31" s="24"/>
+    <row r="31" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A31" s="31">
+        <v>14</v>
+      </c>
+      <c r="B31" s="22" t="s">
+        <v>650</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>651</v>
+      </c>
+      <c r="D31" s="22"/>
+      <c r="E31" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F31" s="37"/>
+      <c r="G31" s="22"/>
+    </row>
+    <row r="32" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A32" s="31">
+        <v>15</v>
+      </c>
+      <c r="B32" s="22" t="s">
+        <v>652</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>653</v>
+      </c>
+      <c r="D32" s="22"/>
+      <c r="E32" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F32" s="37"/>
+      <c r="G32" s="22"/>
+    </row>
+    <row r="33" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B33" s="24"/>
+      <c r="C33" s="25"/>
+      <c r="D33" s="24"/>
+      <c r="E33" s="25"/>
+      <c r="F33" s="24"/>
+      <c r="G33" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -8400,6 +8440,39 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="cea7764e-6bf9-427d-be15-e74097e0a61c">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <SharedWithUsers xmlns="fb9ea31f-0ab8-44ff-80d1-5777f6d9d945">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+    <MediaLengthInSeconds xmlns="cea7764e-6bf9-427d-be15-e74097e0a61c" xsi:nil="true"/>
+    <Sign_x002d_off_x0020_status xmlns="cea7764e-6bf9-427d-be15-e74097e0a61c" xsi:nil="true"/>
+    <Title_x0020_URL xmlns="cea7764e-6bf9-427d-be15-e74097e0a61c">
+      <Url xsi:nil="true"/>
+      <Description xsi:nil="true"/>
+    </Title_x0020_URL>
+    <Mail_x0020_Sent xmlns="cea7764e-6bf9-427d-be15-e74097e0a61c">false</Mail_x0020_Sent>
+    <_Flow_SignoffStatus xmlns="cea7764e-6bf9-427d-be15-e74097e0a61c" xsi:nil="true"/>
+    <State xmlns="cea7764e-6bf9-427d-be15-e74097e0a61c">Open</State>
+    <Comments xmlns="cea7764e-6bf9-427d-be15-e74097e0a61c" xsi:nil="true"/>
+    <Lead_x0020_Signoff xmlns="cea7764e-6bf9-427d-be15-e74097e0a61c">false</Lead_x0020_Signoff>
+    <Title_x0020_ID xmlns="cea7764e-6bf9-427d-be15-e74097e0a61c" xsi:nil="true"/>
+    <TranslatedLang xmlns="cea7764e-6bf9-427d-be15-e74097e0a61c" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010039A62E282DDA434E979CD3E03185182E" ma:contentTypeVersion="33" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="a6c69cf93bfe1fca5d0e373365e7fdfc">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="cea7764e-6bf9-427d-be15-e74097e0a61c" xmlns:ns3="fb9ea31f-0ab8-44ff-80d1-5777f6d9d945" xmlns:ns4="230e9df3-be65-4c73-a93b-d1236ebd677e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="62cb4c6faf5eab163d0c8ea23c8ff408" ns1:_="" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -8741,39 +8814,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="cea7764e-6bf9-427d-be15-e74097e0a61c">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <SharedWithUsers xmlns="fb9ea31f-0ab8-44ff-80d1-5777f6d9d945">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-    <MediaLengthInSeconds xmlns="cea7764e-6bf9-427d-be15-e74097e0a61c" xsi:nil="true"/>
-    <Sign_x002d_off_x0020_status xmlns="cea7764e-6bf9-427d-be15-e74097e0a61c" xsi:nil="true"/>
-    <Title_x0020_URL xmlns="cea7764e-6bf9-427d-be15-e74097e0a61c">
-      <Url xsi:nil="true"/>
-      <Description xsi:nil="true"/>
-    </Title_x0020_URL>
-    <Mail_x0020_Sent xmlns="cea7764e-6bf9-427d-be15-e74097e0a61c">false</Mail_x0020_Sent>
-    <_Flow_SignoffStatus xmlns="cea7764e-6bf9-427d-be15-e74097e0a61c" xsi:nil="true"/>
-    <State xmlns="cea7764e-6bf9-427d-be15-e74097e0a61c">Open</State>
-    <Comments xmlns="cea7764e-6bf9-427d-be15-e74097e0a61c" xsi:nil="true"/>
-    <Lead_x0020_Signoff xmlns="cea7764e-6bf9-427d-be15-e74097e0a61c">false</Lead_x0020_Signoff>
-    <Title_x0020_ID xmlns="cea7764e-6bf9-427d-be15-e74097e0a61c" xsi:nil="true"/>
-    <TranslatedLang xmlns="cea7764e-6bf9-427d-be15-e74097e0a61c" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3F377113-5718-41B1-A1CE-B96F830D3573}">
   <ds:schemaRefs>
@@ -8783,6 +8823,25 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E53D8182-34C2-4EE5-8FD0-D750C3EB0900}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="fb9ea31f-0ab8-44ff-80d1-5777f6d9d945"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
+    <ds:schemaRef ds:uri="cea7764e-6bf9-427d-be15-e74097e0a61c"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{23B9621B-458A-4676-8042-F53348150B3A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -8803,25 +8862,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E53D8182-34C2-4EE5-8FD0-D750C3EB0900}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="fb9ea31f-0ab8-44ff-80d1-5777f6d9d945"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
-    <ds:schemaRef ds:uri="cea7764e-6bf9-427d-be15-e74097e0a61c"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{87867195-f2b8-4ac2-b0b6-6bb73cb33afc}" enabled="1" method="Privileged" siteId="{72f988bf-86f1-41af-91ab-2d7cd011db47}" contentBits="0" removed="0"/>

</xml_diff>